<commit_message>
Excel Data sheets update
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8BEDEB-E34B-4DC0-8623-BA1C9D52BFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE646F72-32E1-424F-AEAF-AFC835BF7023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="482">
   <si>
     <t>Topic</t>
   </si>
@@ -6152,7 +6152,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6512,7 +6512,7 @@
         <v>8</v>
       </c>
       <c r="E18" s="27">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F18" s="94">
         <v>45670</v>
@@ -6534,13 +6534,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="27">
-        <v>0.75</v>
+        <v>2.5</v>
       </c>
       <c r="F19" s="94">
-        <v>45670</v>
+        <v>45672</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>473</v>
+        <v>433</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -6555,9 +6555,15 @@
       <c r="D20" s="27">
         <v>1.5</v>
       </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
+      <c r="E20" s="27">
+        <v>2</v>
+      </c>
+      <c r="F20" s="94">
+        <v>45672</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>433</v>
+      </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
@@ -6571,9 +6577,15 @@
       <c r="D21" s="27">
         <v>6</v>
       </c>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
+      <c r="E21" s="27">
+        <v>1</v>
+      </c>
+      <c r="F21" s="94">
+        <v>45672</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>473</v>
+      </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>

</xml_diff>

<commit_message>
Modifications into DBFinal Demo and Database with C# basic parts complete
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764E72F1-C47B-44D1-A013-E5574FAC2970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F6B4ED-6CA1-43CB-80B4-D7B6BD204053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
@@ -6151,8 +6151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51642604-D68B-4E5E-9160-A3EE5943E7C7}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6578,10 +6578,10 @@
         <v>6</v>
       </c>
       <c r="E21" s="27">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F21" s="94">
-        <v>45672</v>
+        <v>45673</v>
       </c>
       <c r="G21" s="27" t="s">
         <v>473</v>

</xml_diff>

<commit_message>
Basic API final demo
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CB5158-C804-4558-A257-FA7C8EA77293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F373D1C3-F77D-479D-B900-5DDEF3F62DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
+    <workbookView xWindow="1620" yWindow="1470" windowWidth="21600" windowHeight="14130" activeTab="2" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
   <sheets>
     <sheet name=" Basic GUI" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="481">
   <si>
     <t>Topic</t>
   </si>
@@ -1457,9 +1457,6 @@
   </si>
   <si>
     <t xml:space="preserve">Add DataTable &amp; DateTime </t>
-  </si>
-  <si>
-    <t>Ongoing</t>
   </si>
   <si>
     <t>Update view table name, Add full query which covers all DBMS topics, Default value flags</t>
@@ -5647,7 +5644,7 @@
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -5691,7 +5688,7 @@
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -5721,7 +5718,7 @@
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="J48" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -5765,7 +5762,7 @@
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
       <c r="J51" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -5795,7 +5792,7 @@
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -5809,7 +5806,7 @@
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -5823,7 +5820,7 @@
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -5851,7 +5848,7 @@
       </c>
       <c r="I56" s="56"/>
       <c r="J56" s="56" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -6152,7 +6149,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6626,13 +6623,13 @@
         <v>12</v>
       </c>
       <c r="E24" s="57">
-        <v>4.5</v>
+        <v>12</v>
       </c>
       <c r="F24" s="96">
         <v>45674</v>
       </c>
       <c r="G24" s="57" t="s">
-        <v>473</v>
+        <v>433</v>
       </c>
       <c r="H24" s="56"/>
       <c r="I24" s="56"/>

</xml_diff>

<commit_message>
basic api final demo with versioning and caching
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F373D1C3-F77D-479D-B900-5DDEF3F62DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C762A18F-41DC-4662-9E5D-ADE3E7B814AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="1470" windowWidth="21600" windowHeight="14130" activeTab="2" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
   <sheets>
     <sheet name=" Basic GUI" sheetId="1" r:id="rId1"/>
@@ -4701,8 +4701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55139DF5-AA94-4588-B3E8-F184A6C42757}">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView topLeftCell="C43" zoomScale="105" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView tabSelected="1" topLeftCell="C43" zoomScale="105" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6148,7 +6148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51642604-D68B-4E5E-9160-A3EE5943E7C7}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Basic api web development demo
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C762A18F-41DC-4662-9E5D-ADE3E7B814AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EB2101-527D-416E-B08B-E83B1A613D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
@@ -4701,8 +4701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55139DF5-AA94-4588-B3E8-F184A6C42757}">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C43" zoomScale="105" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="B43" zoomScale="105" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70:C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Versioning and Basic web development final demo modifications
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEB84BC-1DF5-43FB-B5D3-C1109160488A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6A9D14-E094-4BDA-B6B2-DF9A36DFB3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="482">
   <si>
     <t>Topic</t>
   </si>
@@ -1481,6 +1481,9 @@
   </si>
   <si>
     <t>How to replace OFFSET</t>
+  </si>
+  <si>
+    <t>Ongoing</t>
   </si>
 </sst>
 </file>
@@ -1804,7 +1807,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2105,6 +2108,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4702,7 +4706,7 @@
   <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView topLeftCell="B43" zoomScale="105" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6712,7 +6716,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6782,12 +6786,14 @@
         <v>8</v>
       </c>
       <c r="F2" s="27">
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="G2" s="94">
         <v>45679</v>
       </c>
-      <c r="H2" s="27"/>
+      <c r="H2" s="27" t="s">
+        <v>433</v>
+      </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -6934,15 +6940,21 @@
       <c r="C11" s="27">
         <v>1</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="110" t="s">
         <v>259</v>
       </c>
       <c r="E11" s="27">
         <v>5</v>
       </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
+      <c r="F11" s="27">
+        <v>2.5</v>
+      </c>
+      <c r="G11" s="94">
+        <v>45680</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>481</v>
+      </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>

</xml_diff>

<commit_message>
Debugging in visual studio
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6A9D14-E094-4BDA-B6B2-DF9A36DFB3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C23884-052C-4B95-8C5B-167D5EEB0CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
   <sheets>
     <sheet name=" Basic GUI" sheetId="1" r:id="rId1"/>
@@ -1807,7 +1807,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2108,7 +2108,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6156,8 +6155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51642604-D68B-4E5E-9160-A3EE5943E7C7}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6715,8 +6714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE125957-E0FE-4793-875C-A900941606E5}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6940,7 +6939,7 @@
       <c r="C11" s="27">
         <v>1</v>
       </c>
-      <c r="D11" s="110" t="s">
+      <c r="D11" s="3" t="s">
         <v>259</v>
       </c>
       <c r="E11" s="27">

</xml_diff>

<commit_message>
filter and action method demo
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F28809-CE6B-44AE-A287-17E402CEFD71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D106088-1380-44CD-BC02-C290F0971FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
@@ -1807,7 +1807,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2108,6 +2108,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6715,7 +6716,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7014,14 +7015,14 @@
       <c r="C14" s="27">
         <v>4</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="110" t="s">
         <v>262</v>
       </c>
       <c r="E14" s="27">
         <v>1.5</v>
       </c>
       <c r="F14" s="27">
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="G14" s="94">
         <v>45684</v>
@@ -7088,10 +7089,10 @@
         <v>10</v>
       </c>
       <c r="F17" s="27">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G17" s="94">
-        <v>45684</v>
+        <v>45686</v>
       </c>
       <c r="H17" s="27" t="s">
         <v>481</v>

</xml_diff>

<commit_message>
Advance API final demo complete
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RKIT\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D106088-1380-44CD-BC02-C290F0971FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2DBBA5-9CED-4EAA-8070-9A1F2CAE67CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
   <sheets>
     <sheet name=" Basic GUI" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1807,7 +1816,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2108,7 +2117,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2452,20 +2460,20 @@
       <selection activeCell="J95" sqref="J95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="72" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="72" customWidth="1"/>
     <col min="2" max="2" width="6" style="29" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" customWidth="1"/>
     <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="5" width="53.42578125" customWidth="1"/>
-    <col min="6" max="9" width="9.28515625" style="29" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="51.42578125" customWidth="1"/>
+    <col min="5" max="5" width="53.44140625" customWidth="1"/>
+    <col min="6" max="9" width="9.33203125" style="29" customWidth="1"/>
+    <col min="10" max="10" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="51.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="40" customFormat="1" ht="18.75">
+    <row r="1" spans="1:12" s="40" customFormat="1" ht="18">
       <c r="A1" s="101" t="s">
         <v>0</v>
       </c>
@@ -2491,7 +2499,7 @@
       <c r="K1" s="41"/>
       <c r="L1" s="41"/>
     </row>
-    <row r="2" spans="1:12" s="29" customFormat="1" ht="18.75">
+    <row r="2" spans="1:12" s="29" customFormat="1" ht="18">
       <c r="A2" s="66">
         <v>1</v>
       </c>
@@ -2515,7 +2523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75">
+    <row r="3" spans="1:12" ht="15.6">
       <c r="A3" s="47"/>
       <c r="B3" s="46">
         <v>1.1000000000000001</v>
@@ -2543,7 +2551,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="31.5">
+    <row r="4" spans="1:12" ht="31.2">
       <c r="A4" s="67"/>
       <c r="B4" s="24"/>
       <c r="C4" s="31" t="s">
@@ -2563,7 +2571,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75">
+    <row r="5" spans="1:12" ht="15.6">
       <c r="A5" s="67"/>
       <c r="B5" s="24"/>
       <c r="C5" s="31" t="s">
@@ -2581,7 +2589,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75">
+    <row r="6" spans="1:12" ht="15.6">
       <c r="A6" s="67"/>
       <c r="B6" s="24"/>
       <c r="C6" s="31" t="s">
@@ -2599,7 +2607,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75">
+    <row r="7" spans="1:12" ht="15.6">
       <c r="A7" s="47"/>
       <c r="B7" s="49">
         <v>1.2</v>
@@ -2627,7 +2635,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75">
+    <row r="8" spans="1:12" ht="15.6">
       <c r="A8" s="67"/>
       <c r="B8" s="24"/>
       <c r="C8" s="31" t="s">
@@ -2645,7 +2653,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75">
+    <row r="9" spans="1:12" ht="15.6">
       <c r="A9" s="67"/>
       <c r="B9" s="24"/>
       <c r="C9" s="31" t="s">
@@ -2663,7 +2671,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75">
+    <row r="10" spans="1:12" ht="15.6">
       <c r="A10" s="67"/>
       <c r="B10" s="24"/>
       <c r="C10" s="31" t="s">
@@ -2681,7 +2689,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75">
+    <row r="11" spans="1:12" ht="15.6">
       <c r="A11" s="67"/>
       <c r="B11" s="24"/>
       <c r="C11" s="31" t="s">
@@ -2699,7 +2707,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75">
+    <row r="12" spans="1:12" ht="15.6">
       <c r="A12" s="67"/>
       <c r="B12" s="24"/>
       <c r="C12" s="31" t="s">
@@ -2717,7 +2725,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75">
+    <row r="13" spans="1:12" ht="15.6">
       <c r="A13" s="67"/>
       <c r="B13" s="24"/>
       <c r="C13" s="31" t="s">
@@ -2735,7 +2743,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75">
+    <row r="14" spans="1:12" ht="15.6">
       <c r="A14" s="67"/>
       <c r="B14" s="24"/>
       <c r="C14" s="31" t="s">
@@ -2753,7 +2761,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75">
+    <row r="15" spans="1:12" ht="15.6">
       <c r="A15" s="67"/>
       <c r="B15" s="24"/>
       <c r="C15" s="31" t="s">
@@ -2771,7 +2779,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75">
+    <row r="16" spans="1:12" ht="15.6">
       <c r="A16" s="67"/>
       <c r="B16" s="24"/>
       <c r="C16" s="31" t="s">
@@ -2789,7 +2797,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75">
+    <row r="17" spans="1:12" ht="15.6">
       <c r="A17" s="47"/>
       <c r="B17" s="49">
         <v>1.3</v>
@@ -2817,7 +2825,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75">
+    <row r="18" spans="1:12" ht="15.6">
       <c r="A18" s="67"/>
       <c r="B18" s="24"/>
       <c r="C18" s="31" t="s">
@@ -2835,7 +2843,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75">
+    <row r="19" spans="1:12" ht="15.6">
       <c r="A19" s="67"/>
       <c r="B19" s="24"/>
       <c r="C19" s="31" t="s">
@@ -2853,7 +2861,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" ht="15.75">
+    <row r="20" spans="1:12" ht="15.6">
       <c r="A20" s="67"/>
       <c r="B20" s="24"/>
       <c r="C20" s="31" t="s">
@@ -2871,7 +2879,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75">
+    <row r="21" spans="1:12" ht="15.6">
       <c r="A21" s="67"/>
       <c r="B21" s="24"/>
       <c r="C21" s="31" t="s">
@@ -2889,7 +2897,7 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75">
+    <row r="22" spans="1:12" ht="15.6">
       <c r="A22" s="47"/>
       <c r="B22" s="49">
         <v>1.4</v>
@@ -2919,7 +2927,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75">
+    <row r="23" spans="1:12" ht="15.6">
       <c r="A23" s="67"/>
       <c r="B23" s="24"/>
       <c r="C23" s="31" t="s">
@@ -2937,7 +2945,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75">
+    <row r="24" spans="1:12" ht="15.6">
       <c r="A24" s="67"/>
       <c r="B24" s="24"/>
       <c r="C24" s="31" t="s">
@@ -2955,7 +2963,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" ht="31.5">
+    <row r="25" spans="1:12" ht="31.2">
       <c r="A25" s="67"/>
       <c r="B25" s="24"/>
       <c r="C25" s="31" t="s">
@@ -2973,7 +2981,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:12" ht="15.75">
+    <row r="26" spans="1:12" ht="15.6">
       <c r="A26" s="67"/>
       <c r="B26" s="24"/>
       <c r="C26" s="31"/>
@@ -2987,7 +2995,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:12" ht="15.75">
+    <row r="27" spans="1:12" ht="15.6">
       <c r="A27" s="85"/>
       <c r="B27" s="86">
         <v>1.5</v>
@@ -3017,7 +3025,7 @@
       <c r="K27" s="56"/>
       <c r="L27" s="56"/>
     </row>
-    <row r="28" spans="1:12" ht="15.75">
+    <row r="28" spans="1:12" ht="15.6">
       <c r="A28" s="67"/>
       <c r="B28" s="24"/>
       <c r="C28" s="31"/>
@@ -3031,7 +3039,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" ht="18.75">
+    <row r="29" spans="1:12" ht="18">
       <c r="A29" s="66">
         <v>2</v>
       </c>
@@ -3049,7 +3057,7 @@
       <c r="K29" s="44"/>
       <c r="L29" s="44"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75">
+    <row r="30" spans="1:12" ht="15.6">
       <c r="A30" s="47"/>
       <c r="B30" s="50">
         <v>2.1</v>
@@ -3077,7 +3085,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12" ht="15.75">
+    <row r="31" spans="1:12" ht="15.6">
       <c r="A31" s="67"/>
       <c r="B31" s="24"/>
       <c r="C31" s="11" t="s">
@@ -3097,7 +3105,7 @@
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
     </row>
-    <row r="32" spans="1:12" ht="47.25">
+    <row r="32" spans="1:12" ht="46.8">
       <c r="A32" s="67"/>
       <c r="B32" s="24"/>
       <c r="C32" s="11" t="s">
@@ -3117,7 +3125,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="1:12" ht="15.75">
+    <row r="33" spans="1:12" ht="15.6">
       <c r="A33" s="67"/>
       <c r="B33" s="24"/>
       <c r="C33" s="11" t="s">
@@ -3137,7 +3145,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="1:12" ht="15.75">
+    <row r="34" spans="1:12" ht="15.6">
       <c r="A34" s="67"/>
       <c r="B34" s="24"/>
       <c r="C34" s="11" t="s">
@@ -3157,7 +3165,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="1:12" ht="15.75">
+    <row r="35" spans="1:12" ht="15.6">
       <c r="A35" s="67"/>
       <c r="B35" s="24"/>
       <c r="C35" s="11" t="s">
@@ -3175,7 +3183,7 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="1:12" ht="15.75">
+    <row r="36" spans="1:12" ht="15.6">
       <c r="A36" s="67"/>
       <c r="B36" s="24"/>
       <c r="C36" s="11" t="s">
@@ -3195,7 +3203,7 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="1:12" ht="15.75">
+    <row r="37" spans="1:12" ht="15.6">
       <c r="A37" s="67"/>
       <c r="B37" s="24"/>
       <c r="C37" s="11"/>
@@ -3209,7 +3217,7 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="1:12" ht="15.75">
+    <row r="38" spans="1:12" ht="15.6">
       <c r="A38" s="85"/>
       <c r="B38" s="89" t="s">
         <v>70</v>
@@ -3239,7 +3247,7 @@
       <c r="K38" s="56"/>
       <c r="L38" s="56"/>
     </row>
-    <row r="39" spans="1:12" ht="15.75">
+    <row r="39" spans="1:12" ht="15.6">
       <c r="A39" s="67"/>
       <c r="B39" s="24"/>
       <c r="C39" s="31"/>
@@ -3253,7 +3261,7 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="1:12" ht="18.75">
+    <row r="40" spans="1:12" ht="18">
       <c r="A40" s="66">
         <v>3</v>
       </c>
@@ -3271,7 +3279,7 @@
       <c r="K40" s="44"/>
       <c r="L40" s="44"/>
     </row>
-    <row r="41" spans="1:12" ht="15.75">
+    <row r="41" spans="1:12" ht="15.6">
       <c r="A41" s="6"/>
       <c r="B41" s="49">
         <v>3.1</v>
@@ -3299,7 +3307,7 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="1:12" ht="15.75">
+    <row r="42" spans="1:12" ht="15.6">
       <c r="A42" s="67"/>
       <c r="B42" s="51"/>
       <c r="C42" s="11" t="s">
@@ -3317,7 +3325,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="1:12" ht="15.75">
+    <row r="43" spans="1:12" ht="15.6">
       <c r="A43" s="67"/>
       <c r="B43" s="24"/>
       <c r="C43" s="11" t="s">
@@ -3335,7 +3343,7 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="1:12" ht="15.75">
+    <row r="44" spans="1:12" ht="15.6">
       <c r="A44" s="67"/>
       <c r="B44" s="24"/>
       <c r="C44" s="11" t="s">
@@ -3353,7 +3361,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="1:12" ht="15.75">
+    <row r="45" spans="1:12" ht="15.6">
       <c r="A45" s="67"/>
       <c r="B45" s="24"/>
       <c r="C45" s="11"/>
@@ -3367,7 +3375,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="1:12" ht="15.75">
+    <row r="46" spans="1:12" ht="15.6">
       <c r="A46" s="67"/>
       <c r="B46" s="24"/>
       <c r="C46" s="100"/>
@@ -3381,7 +3389,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="1:12" ht="18.75">
+    <row r="47" spans="1:12" ht="18">
       <c r="A47" s="66">
         <v>4</v>
       </c>
@@ -3399,7 +3407,7 @@
       <c r="K47" s="44"/>
       <c r="L47" s="44"/>
     </row>
-    <row r="48" spans="1:12" ht="15.75">
+    <row r="48" spans="1:12" ht="15.6">
       <c r="A48" s="6"/>
       <c r="B48" s="49">
         <v>4.0999999999999996</v>
@@ -3429,7 +3437,7 @@
       </c>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:12" ht="15.75">
+    <row r="49" spans="1:12" ht="15.6">
       <c r="A49" s="67"/>
       <c r="B49" s="51"/>
       <c r="C49" s="11" t="s">
@@ -3447,7 +3455,7 @@
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:12" ht="15.75">
+    <row r="50" spans="1:12" ht="15.6">
       <c r="A50" s="67"/>
       <c r="B50" s="24"/>
       <c r="C50" s="11" t="s">
@@ -3465,7 +3473,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="1:12" ht="15.75">
+    <row r="51" spans="1:12" ht="15.6">
       <c r="A51" s="67"/>
       <c r="B51" s="24"/>
       <c r="C51" s="11" t="s">
@@ -3483,7 +3491,7 @@
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="1:12" ht="15.75">
+    <row r="52" spans="1:12" ht="15.6">
       <c r="A52" s="67"/>
       <c r="B52" s="24"/>
       <c r="C52" s="11" t="s">
@@ -3501,7 +3509,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="1:12" ht="15.75">
+    <row r="53" spans="1:12" ht="15.6">
       <c r="A53" s="67"/>
       <c r="B53" s="24"/>
       <c r="C53" s="11" t="s">
@@ -3519,7 +3527,7 @@
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="1:12" ht="15.75">
+    <row r="54" spans="1:12" ht="15.6">
       <c r="A54" s="67"/>
       <c r="B54" s="24"/>
       <c r="C54" s="11" t="s">
@@ -3537,7 +3545,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="1:12" ht="15.75">
+    <row r="55" spans="1:12" ht="15.6">
       <c r="A55" s="67"/>
       <c r="B55" s="24"/>
       <c r="C55" s="11"/>
@@ -3551,7 +3559,7 @@
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="1:12" ht="15.75">
+    <row r="56" spans="1:12" ht="15.6">
       <c r="A56" s="85"/>
       <c r="B56" s="89" t="s">
         <v>93</v>
@@ -3595,7 +3603,7 @@
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="1:12" ht="18.75">
+    <row r="58" spans="1:12" ht="18">
       <c r="A58" s="66">
         <v>5</v>
       </c>
@@ -3627,7 +3635,7 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="1:12" ht="15.75">
+    <row r="60" spans="1:12" ht="15.6">
       <c r="A60" s="69">
         <v>1</v>
       </c>
@@ -3657,7 +3665,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="15.75">
+    <row r="61" spans="1:12" ht="15.6">
       <c r="A61" s="67"/>
       <c r="B61" s="52">
         <v>1.1000000000000001</v>
@@ -3675,7 +3683,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="1:12" ht="15.75">
+    <row r="62" spans="1:12" ht="15.6">
       <c r="A62" s="67"/>
       <c r="B62" s="52">
         <v>1.2</v>
@@ -3693,7 +3701,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="1:12" ht="15.75">
+    <row r="63" spans="1:12" ht="15.6">
       <c r="A63" s="67"/>
       <c r="B63" s="52">
         <v>1.3</v>
@@ -3723,7 +3731,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="15.75">
+    <row r="64" spans="1:12" ht="15.6">
       <c r="A64" s="67"/>
       <c r="B64" s="52"/>
       <c r="C64" s="8" t="s">
@@ -3743,7 +3751,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="31.5">
+    <row r="65" spans="1:12" ht="31.2">
       <c r="A65" s="47"/>
       <c r="B65" s="52"/>
       <c r="C65" s="8" t="s">
@@ -3761,7 +3769,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75">
+    <row r="66" spans="1:12" ht="15.6">
       <c r="A66" s="67"/>
       <c r="B66" s="52"/>
       <c r="C66" s="8" t="s">
@@ -3779,7 +3787,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75">
+    <row r="67" spans="1:12" ht="15.6">
       <c r="A67" s="69">
         <v>2</v>
       </c>
@@ -3807,7 +3815,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75">
+    <row r="68" spans="1:12" ht="15.6">
       <c r="A68" s="70"/>
       <c r="B68" s="52">
         <v>2.1</v>
@@ -3825,7 +3833,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75">
+    <row r="69" spans="1:12" ht="15.6">
       <c r="A69" s="70"/>
       <c r="B69" s="52">
         <v>2.2000000000000002</v>
@@ -3843,7 +3851,7 @@
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75">
+    <row r="70" spans="1:12" ht="15.6">
       <c r="A70" s="70"/>
       <c r="B70" s="52">
         <v>2.2999999999999998</v>
@@ -3861,7 +3869,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75">
+    <row r="71" spans="1:12" ht="15.6">
       <c r="A71" s="70"/>
       <c r="B71" s="52"/>
       <c r="C71" s="8"/>
@@ -3875,7 +3883,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75">
+    <row r="72" spans="1:12" ht="15.6">
       <c r="A72" s="69">
         <v>3</v>
       </c>
@@ -3905,7 +3913,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75">
+    <row r="73" spans="1:12" ht="15.6">
       <c r="A73" s="70"/>
       <c r="B73" s="52">
         <v>3.1</v>
@@ -3923,7 +3931,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75">
+    <row r="74" spans="1:12" ht="15.6">
       <c r="A74" s="70"/>
       <c r="B74" s="52">
         <v>3.2</v>
@@ -3941,7 +3949,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75">
+    <row r="75" spans="1:12" ht="15.6">
       <c r="A75" s="70"/>
       <c r="B75" s="52">
         <v>3.3</v>
@@ -3959,7 +3967,7 @@
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75">
+    <row r="76" spans="1:12" ht="15.6">
       <c r="A76" s="70"/>
       <c r="B76" s="52">
         <v>3.4</v>
@@ -3977,7 +3985,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75">
+    <row r="77" spans="1:12" ht="15.6">
       <c r="A77" s="69">
         <v>4</v>
       </c>
@@ -4005,7 +4013,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75">
+    <row r="78" spans="1:12" ht="15.6">
       <c r="A78" s="70"/>
       <c r="B78" s="52">
         <v>4.0999999999999996</v>
@@ -4037,7 +4045,7 @@
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="1:12" ht="18.75">
+    <row r="80" spans="1:12" ht="18">
       <c r="A80" s="66">
         <v>5</v>
       </c>
@@ -4055,7 +4063,7 @@
       <c r="K80" s="44"/>
       <c r="L80" s="44"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75">
+    <row r="81" spans="1:12" ht="15.6">
       <c r="A81" s="6"/>
       <c r="B81" s="49">
         <v>5.0999999999999996</v>
@@ -4083,7 +4091,7 @@
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75">
+    <row r="82" spans="1:12" ht="15.6">
       <c r="A82" s="67"/>
       <c r="B82" s="24"/>
       <c r="C82" s="11" t="s">
@@ -4101,7 +4109,7 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" ht="31.5">
+    <row r="83" spans="1:12" ht="31.2">
       <c r="A83" s="67"/>
       <c r="B83" s="24"/>
       <c r="C83" s="11" t="s">
@@ -4119,7 +4127,7 @@
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" ht="31.5">
+    <row r="84" spans="1:12" ht="31.2">
       <c r="A84" s="67"/>
       <c r="B84" s="24"/>
       <c r="C84" s="11" t="s">
@@ -4139,7 +4147,7 @@
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" ht="31.5">
+    <row r="85" spans="1:12" ht="31.2">
       <c r="A85" s="67"/>
       <c r="B85" s="24"/>
       <c r="C85" s="11" t="s">
@@ -4159,7 +4167,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" ht="31.5">
+    <row r="86" spans="1:12" ht="31.2">
       <c r="A86" s="47"/>
       <c r="B86" s="49">
         <v>5.2</v>
@@ -4189,7 +4197,7 @@
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75">
+    <row r="87" spans="1:12" ht="15.6">
       <c r="A87" s="67"/>
       <c r="B87" s="24"/>
       <c r="C87" s="11" t="s">
@@ -4207,7 +4215,7 @@
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75">
+    <row r="88" spans="1:12" ht="15.6">
       <c r="A88" s="67"/>
       <c r="B88" s="24"/>
       <c r="C88" s="11" t="s">
@@ -4225,7 +4233,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75">
+    <row r="89" spans="1:12" ht="15.6">
       <c r="A89" s="67"/>
       <c r="B89" s="24"/>
       <c r="C89" s="11" t="s">
@@ -4243,7 +4251,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75">
+    <row r="90" spans="1:12" ht="15.6">
       <c r="A90" s="67"/>
       <c r="B90" s="24"/>
       <c r="C90" s="11"/>
@@ -4257,7 +4265,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75">
+    <row r="91" spans="1:12" ht="15.6">
       <c r="A91" s="47"/>
       <c r="B91" s="49">
         <v>5.3</v>
@@ -4285,7 +4293,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75">
+    <row r="92" spans="1:12" ht="15.6">
       <c r="A92" s="67"/>
       <c r="B92" s="24"/>
       <c r="C92" s="11" t="s">
@@ -4303,7 +4311,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75">
+    <row r="93" spans="1:12" ht="15.6">
       <c r="A93" s="67"/>
       <c r="B93" s="24"/>
       <c r="C93" s="11" t="s">
@@ -4321,7 +4329,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75">
+    <row r="94" spans="1:12" ht="15.6">
       <c r="A94" s="67"/>
       <c r="B94" s="24"/>
       <c r="C94" s="11"/>
@@ -4335,7 +4343,7 @@
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
     </row>
-    <row r="95" spans="1:12" ht="47.25">
+    <row r="95" spans="1:12" ht="31.2">
       <c r="A95" s="67"/>
       <c r="B95" s="49">
         <v>5.4</v>
@@ -4365,7 +4373,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="30">
+    <row r="96" spans="1:12" ht="28.8">
       <c r="A96" s="47"/>
       <c r="B96" s="49">
         <v>5.5</v>
@@ -4385,7 +4393,7 @@
       <c r="K96" s="3"/>
       <c r="L96" s="3"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75">
+    <row r="97" spans="1:12" ht="15.6">
       <c r="A97" s="47"/>
       <c r="B97" s="49">
         <v>5.6</v>
@@ -4403,7 +4411,7 @@
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75">
+    <row r="98" spans="1:12" ht="15.6">
       <c r="A98" s="47"/>
       <c r="B98" s="49">
         <v>5.7</v>
@@ -4437,7 +4445,7 @@
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75">
+    <row r="100" spans="1:12" ht="15.6">
       <c r="A100" s="6"/>
       <c r="B100" s="1">
         <v>5.8</v>
@@ -4469,7 +4477,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="15.75">
+    <row r="101" spans="1:12" ht="15.6">
       <c r="A101" s="67"/>
       <c r="B101" s="24"/>
       <c r="C101" s="11" t="s">
@@ -4489,7 +4497,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="15.75">
+    <row r="102" spans="1:12" ht="15.6">
       <c r="A102" s="67"/>
       <c r="B102" s="24"/>
       <c r="C102" s="11" t="s">
@@ -4507,7 +4515,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75">
+    <row r="103" spans="1:12" ht="15.6">
       <c r="A103" s="67"/>
       <c r="B103" s="24"/>
       <c r="C103" s="11" t="s">
@@ -4525,7 +4533,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
     </row>
-    <row r="104" spans="1:12" ht="31.5">
+    <row r="104" spans="1:12" ht="31.2">
       <c r="A104" s="67"/>
       <c r="B104" s="24"/>
       <c r="C104" s="11" t="s">
@@ -4543,7 +4551,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75">
+    <row r="105" spans="1:12" ht="15.6">
       <c r="A105" s="67"/>
       <c r="B105" s="24"/>
       <c r="C105" s="11" t="s">
@@ -4563,7 +4571,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75">
+    <row r="106" spans="1:12" ht="15.6">
       <c r="A106" s="67"/>
       <c r="B106" s="24"/>
       <c r="C106" s="11" t="s">
@@ -4581,7 +4589,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75">
+    <row r="107" spans="1:12" ht="15.6">
       <c r="A107" s="67"/>
       <c r="B107" s="24"/>
       <c r="C107" s="11"/>
@@ -4595,7 +4603,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="1:12" s="20" customFormat="1" ht="37.5">
+    <row r="108" spans="1:12" s="20" customFormat="1" ht="36">
       <c r="A108" s="71">
         <v>6</v>
       </c>
@@ -4709,18 +4717,18 @@
       <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9" style="29" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" style="29" customWidth="1"/>
-    <col min="3" max="3" width="65.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" style="29" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="29" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="89.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" style="29" customWidth="1"/>
+    <col min="3" max="3" width="65.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" style="29" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="29" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="89.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="29" customFormat="1">
@@ -4755,7 +4763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="45">
+    <row r="2" spans="1:10" ht="43.2">
       <c r="A2" s="28" t="s">
         <v>160</v>
       </c>
@@ -6156,21 +6164,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51642604-D68B-4E5E-9160-A3EE5943E7C7}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="29"/>
-    <col min="2" max="2" width="25.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="29"/>
+    <col min="2" max="2" width="25.33203125" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="29"/>
-    <col min="5" max="5" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="29" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="29"/>
+    <col min="5" max="5" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" style="29" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="29" customFormat="1">
@@ -6715,23 +6723,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE125957-E0FE-4793-875C-A900941606E5}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="29"/>
-    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="29"/>
+    <col min="2" max="2" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" style="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="29" customFormat="1">
@@ -7015,7 +7023,7 @@
       <c r="C14" s="27">
         <v>4</v>
       </c>
-      <c r="D14" s="110" t="s">
+      <c r="D14" s="3" t="s">
         <v>262</v>
       </c>
       <c r="E14" s="27">
@@ -7332,17 +7340,17 @@
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="29"/>
-    <col min="4" max="4" width="66.85546875" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="29"/>
+    <col min="4" max="4" width="66.88671875" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" customHeight="1">
@@ -7361,7 +7369,7 @@
       <c r="K1" s="106"/>
       <c r="L1" s="106"/>
     </row>
-    <row r="2" spans="1:12" ht="18.75">
+    <row r="2" spans="1:12" ht="18">
       <c r="A2" s="107" t="s">
         <v>422</v>
       </c>
@@ -7391,7 +7399,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75">
+    <row r="3" spans="1:12" ht="15.6">
       <c r="A3" s="23"/>
       <c r="B3" s="16"/>
       <c r="C3" s="15"/>
@@ -7407,7 +7415,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75">
+    <row r="4" spans="1:12" ht="15.6">
       <c r="A4" s="76">
         <v>1</v>
       </c>
@@ -7427,7 +7435,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75">
+    <row r="5" spans="1:12" ht="15.6">
       <c r="A5" s="78"/>
       <c r="B5" s="18">
         <v>1.1000000000000001</v>
@@ -7447,7 +7455,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75">
+    <row r="6" spans="1:12" ht="15.6">
       <c r="A6" s="78"/>
       <c r="B6" s="18">
         <v>1.2</v>
@@ -7467,7 +7475,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75">
+    <row r="7" spans="1:12" ht="15.6">
       <c r="A7" s="78"/>
       <c r="B7" s="18">
         <v>1.3</v>
@@ -7487,7 +7495,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75">
+    <row r="8" spans="1:12" ht="15.6">
       <c r="A8" s="78"/>
       <c r="B8" s="18"/>
       <c r="C8" s="19" t="s">
@@ -7505,7 +7513,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75">
+    <row r="9" spans="1:12" ht="15.6">
       <c r="A9" s="78"/>
       <c r="B9" s="18"/>
       <c r="C9" s="19" t="s">
@@ -7523,7 +7531,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75">
+    <row r="10" spans="1:12" ht="15.6">
       <c r="A10" s="78"/>
       <c r="B10" s="18"/>
       <c r="C10" s="19" t="s">
@@ -7541,7 +7549,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75">
+    <row r="11" spans="1:12" ht="15.6">
       <c r="A11" s="78"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19" t="s">
@@ -7559,7 +7567,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75">
+    <row r="12" spans="1:12" ht="15.6">
       <c r="A12" s="78"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19" t="s">
@@ -7577,7 +7585,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75">
+    <row r="13" spans="1:12" ht="15.6">
       <c r="A13" s="78"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19" t="s">
@@ -7595,7 +7603,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75">
+    <row r="14" spans="1:12" ht="15.6">
       <c r="A14" s="78"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
@@ -7609,7 +7617,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75">
+    <row r="15" spans="1:12" ht="15.6">
       <c r="A15" s="76">
         <v>2</v>
       </c>
@@ -7631,7 +7639,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75">
+    <row r="16" spans="1:12" ht="15.6">
       <c r="A16" s="78"/>
       <c r="B16" s="18">
         <v>2.1</v>
@@ -7651,7 +7659,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75">
+    <row r="17" spans="1:12" ht="15.6">
       <c r="A17" s="78"/>
       <c r="B17" s="18">
         <v>2.2000000000000002</v>
@@ -7671,7 +7679,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75">
+    <row r="18" spans="1:12" ht="15.6">
       <c r="A18" s="78"/>
       <c r="B18" s="18">
         <v>2.2999999999999998</v>
@@ -7691,7 +7699,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75">
+    <row r="19" spans="1:12" ht="15.6">
       <c r="A19" s="78"/>
       <c r="B19" s="18">
         <v>2.4</v>
@@ -7711,7 +7719,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" ht="15.75">
+    <row r="20" spans="1:12" ht="15.6">
       <c r="A20" s="78"/>
       <c r="B20" s="18">
         <v>2.5</v>
@@ -7731,7 +7739,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75">
+    <row r="21" spans="1:12" ht="15.6">
       <c r="A21" s="78"/>
       <c r="B21" s="18"/>
       <c r="C21" s="19" t="s">
@@ -7749,7 +7757,7 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75">
+    <row r="22" spans="1:12" ht="15.6">
       <c r="A22" s="78"/>
       <c r="B22" s="18"/>
       <c r="C22" s="19" t="s">
@@ -7767,7 +7775,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75">
+    <row r="23" spans="1:12" ht="15.6">
       <c r="A23" s="78"/>
       <c r="B23" s="18"/>
       <c r="C23" s="19" t="s">
@@ -7785,7 +7793,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75">
+    <row r="24" spans="1:12" ht="15.6">
       <c r="A24" s="78"/>
       <c r="B24" s="18">
         <v>2.6</v>
@@ -7805,7 +7813,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" ht="15.75">
+    <row r="25" spans="1:12" ht="15.6">
       <c r="A25" s="78"/>
       <c r="B25" s="18">
         <v>2.7</v>
@@ -7825,7 +7833,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:12" ht="15.75">
+    <row r="26" spans="1:12" ht="15.6">
       <c r="A26" s="78"/>
       <c r="B26" s="18">
         <v>2.8</v>
@@ -7843,7 +7851,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:12" ht="15.75">
+    <row r="27" spans="1:12" ht="15.6">
       <c r="A27" s="78"/>
       <c r="B27" s="18">
         <v>2.9</v>
@@ -7861,7 +7869,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="1:12" ht="15.75">
+    <row r="28" spans="1:12" ht="15.6">
       <c r="A28" s="78"/>
       <c r="B28" s="18">
         <v>2.1</v>
@@ -7881,7 +7889,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" ht="15.75">
+    <row r="29" spans="1:12" ht="15.6">
       <c r="A29" s="78"/>
       <c r="B29" s="18"/>
       <c r="C29" s="19"/>
@@ -7897,7 +7905,7 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75">
+    <row r="30" spans="1:12" ht="15.6">
       <c r="A30" s="78"/>
       <c r="B30" s="18"/>
       <c r="C30" s="17"/>
@@ -7911,7 +7919,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12" ht="31.5">
+    <row r="31" spans="1:12" ht="31.2">
       <c r="A31" s="82"/>
       <c r="B31" s="79"/>
       <c r="C31" s="84" t="s">
@@ -7931,7 +7939,7 @@
       <c r="K31" s="56"/>
       <c r="L31" s="56"/>
     </row>
-    <row r="32" spans="1:12" ht="15.75">
+    <row r="32" spans="1:12" ht="15.6">
       <c r="A32" s="76"/>
       <c r="B32" s="16"/>
       <c r="C32" s="15"/>
@@ -7947,7 +7955,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="1:12" ht="15.75">
+    <row r="33" spans="1:12" ht="15.6">
       <c r="A33" s="78"/>
       <c r="B33" s="18"/>
       <c r="C33" s="19"/>
@@ -7961,7 +7969,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="1:12" ht="15.75">
+    <row r="34" spans="1:12" ht="15.6">
       <c r="A34" s="78"/>
       <c r="B34" s="18"/>
       <c r="C34" s="19"/>
@@ -7977,7 +7985,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="1:12" ht="15.75">
+    <row r="35" spans="1:12" ht="15.6">
       <c r="A35" s="76">
         <v>3</v>
       </c>
@@ -7997,7 +8005,7 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="1:12" ht="15.75">
+    <row r="36" spans="1:12" ht="15.6">
       <c r="A36" s="78"/>
       <c r="B36" s="18">
         <v>3.1</v>
@@ -8017,7 +8025,7 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="1:12" ht="15.75">
+    <row r="37" spans="1:12" ht="15.6">
       <c r="A37" s="78"/>
       <c r="B37" s="18">
         <v>3.2</v>
@@ -8037,7 +8045,7 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="1:12" ht="15.75">
+    <row r="38" spans="1:12" ht="15.6">
       <c r="A38" s="78"/>
       <c r="B38" s="18">
         <v>3.3</v>
@@ -8057,7 +8065,7 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="1:12" ht="15.75">
+    <row r="39" spans="1:12" ht="15.6">
       <c r="A39" s="78"/>
       <c r="B39" s="18">
         <v>3.4</v>
@@ -8077,7 +8085,7 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="1:12" ht="15.75">
+    <row r="40" spans="1:12" ht="15.6">
       <c r="A40" s="78"/>
       <c r="B40" s="18">
         <v>3.5</v>
@@ -8097,7 +8105,7 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="1:12" ht="15.75">
+    <row r="41" spans="1:12" ht="15.6">
       <c r="A41" s="78"/>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
@@ -8111,7 +8119,7 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="1:12" ht="15.75">
+    <row r="42" spans="1:12" ht="15.6">
       <c r="A42" s="78"/>
       <c r="B42" s="18"/>
       <c r="C42" s="19"/>
@@ -8125,7 +8133,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="1:12" ht="15.75">
+    <row r="43" spans="1:12" ht="15.6">
       <c r="A43" s="76">
         <v>4</v>
       </c>
@@ -8145,7 +8153,7 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="1:12" ht="15.75">
+    <row r="44" spans="1:12" ht="15.6">
       <c r="A44" s="78"/>
       <c r="B44" s="18">
         <v>4.0999999999999996</v>
@@ -8165,7 +8173,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="1:12" ht="15.75">
+    <row r="45" spans="1:12" ht="15.6">
       <c r="A45" s="78"/>
       <c r="B45" s="18"/>
       <c r="C45" s="19" t="s">
@@ -8183,7 +8191,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="1:12" ht="15.75">
+    <row r="46" spans="1:12" ht="15.6">
       <c r="A46" s="78"/>
       <c r="B46" s="18"/>
       <c r="C46" s="19" t="s">
@@ -8201,7 +8209,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="1:12" ht="15.75">
+    <row r="47" spans="1:12" ht="15.6">
       <c r="A47" s="78"/>
       <c r="B47" s="18">
         <v>4.2</v>
@@ -8221,7 +8229,7 @@
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="1:12" ht="15.75">
+    <row r="48" spans="1:12" ht="15.6">
       <c r="A48" s="78"/>
       <c r="B48" s="18"/>
       <c r="C48" s="19" t="s">
@@ -8239,7 +8247,7 @@
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:12" ht="15.75">
+    <row r="49" spans="1:12" ht="15.6">
       <c r="A49" s="78"/>
       <c r="B49" s="18"/>
       <c r="C49" s="19" t="s">
@@ -8257,7 +8265,7 @@
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:12" ht="15.75">
+    <row r="50" spans="1:12" ht="15.6">
       <c r="A50" s="78"/>
       <c r="B50" s="18"/>
       <c r="C50" s="19" t="s">
@@ -8275,7 +8283,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="1:12" ht="15.75">
+    <row r="51" spans="1:12" ht="15.6">
       <c r="A51" s="78"/>
       <c r="B51" s="18">
         <v>4.3</v>
@@ -8295,7 +8303,7 @@
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="1:12" ht="15.75">
+    <row r="52" spans="1:12" ht="15.6">
       <c r="A52" s="78"/>
       <c r="B52" s="18"/>
       <c r="C52" s="19" t="s">
@@ -8313,7 +8321,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="1:12" ht="15.75">
+    <row r="53" spans="1:12" ht="15.6">
       <c r="A53" s="78"/>
       <c r="B53" s="18"/>
       <c r="C53" s="19" t="s">
@@ -8331,7 +8339,7 @@
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="1:12" ht="15.75">
+    <row r="54" spans="1:12" ht="15.6">
       <c r="A54" s="78"/>
       <c r="B54" s="18"/>
       <c r="C54" s="19" t="s">
@@ -8349,7 +8357,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="1:12" ht="15.75">
+    <row r="55" spans="1:12" ht="15.6">
       <c r="A55" s="78"/>
       <c r="B55" s="18"/>
       <c r="C55" s="19" t="s">
@@ -8367,7 +8375,7 @@
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="1:12" ht="15.75">
+    <row r="56" spans="1:12" ht="15.6">
       <c r="A56" s="78"/>
       <c r="B56" s="18"/>
       <c r="C56" s="19" t="s">
@@ -8385,7 +8393,7 @@
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
     </row>
-    <row r="57" spans="1:12" ht="15.75">
+    <row r="57" spans="1:12" ht="15.6">
       <c r="A57" s="78"/>
       <c r="B57" s="18"/>
       <c r="C57" s="19" t="s">
@@ -8403,7 +8411,7 @@
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="1:12" ht="15.75">
+    <row r="58" spans="1:12" ht="15.6">
       <c r="A58" s="78"/>
       <c r="B58" s="18"/>
       <c r="C58" s="19" t="s">
@@ -8421,7 +8429,7 @@
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="1:12" ht="15.75">
+    <row r="59" spans="1:12" ht="15.6">
       <c r="A59" s="78"/>
       <c r="B59" s="18">
         <v>4.4000000000000004</v>
@@ -8441,7 +8449,7 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="1:12" ht="15.75">
+    <row r="60" spans="1:12" ht="15.6">
       <c r="A60" s="78"/>
       <c r="B60" s="18"/>
       <c r="C60" s="19" t="s">
@@ -8459,7 +8467,7 @@
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="1:12" ht="15.75">
+    <row r="61" spans="1:12" ht="15.6">
       <c r="A61" s="78"/>
       <c r="B61" s="18">
         <v>4.5</v>
@@ -8479,7 +8487,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="1:12" ht="15.75">
+    <row r="62" spans="1:12" ht="15.6">
       <c r="A62" s="78"/>
       <c r="B62" s="18"/>
       <c r="C62" s="19" t="s">
@@ -8497,7 +8505,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="1:12" ht="15.75">
+    <row r="63" spans="1:12" ht="15.6">
       <c r="A63" s="78"/>
       <c r="B63" s="18"/>
       <c r="C63" s="19" t="s">
@@ -8515,7 +8523,7 @@
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="1:12" ht="15.75">
+    <row r="64" spans="1:12" ht="15.6">
       <c r="A64" s="78"/>
       <c r="B64" s="18">
         <v>4.5999999999999996</v>
@@ -8535,7 +8543,7 @@
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75">
+    <row r="65" spans="1:12" ht="15.6">
       <c r="A65" s="78"/>
       <c r="B65" s="18"/>
       <c r="C65" s="19" t="s">
@@ -8553,7 +8561,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75">
+    <row r="66" spans="1:12" ht="15.6">
       <c r="A66" s="78"/>
       <c r="B66" s="18">
         <v>4.7</v>
@@ -8573,7 +8581,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75">
+    <row r="67" spans="1:12" ht="15.6">
       <c r="A67" s="78"/>
       <c r="B67" s="18"/>
       <c r="C67" s="19" t="s">
@@ -8591,7 +8599,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75">
+    <row r="68" spans="1:12" ht="15.6">
       <c r="A68" s="78"/>
       <c r="B68" s="18"/>
       <c r="C68" s="19" t="s">
@@ -8609,7 +8617,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75">
+    <row r="69" spans="1:12" ht="15.6">
       <c r="A69" s="78"/>
       <c r="B69" s="18">
         <v>4.8</v>
@@ -8629,7 +8637,7 @@
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75">
+    <row r="70" spans="1:12" ht="15.6">
       <c r="A70" s="78"/>
       <c r="B70" s="18"/>
       <c r="C70" s="19" t="s">
@@ -8647,7 +8655,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75">
+    <row r="71" spans="1:12" ht="15.6">
       <c r="A71" s="78"/>
       <c r="B71" s="18"/>
       <c r="C71" s="19" t="s">
@@ -8665,7 +8673,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75">
+    <row r="72" spans="1:12" ht="15.6">
       <c r="A72" s="78"/>
       <c r="B72" s="18"/>
       <c r="C72" s="19" t="s">
@@ -8683,7 +8691,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75">
+    <row r="73" spans="1:12" ht="15.6">
       <c r="A73" s="78"/>
       <c r="B73" s="18"/>
       <c r="C73" s="19" t="s">
@@ -8701,7 +8709,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75">
+    <row r="74" spans="1:12" ht="15.6">
       <c r="A74" s="78"/>
       <c r="B74" s="18"/>
       <c r="C74" s="19" t="s">
@@ -8719,7 +8727,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75">
+    <row r="75" spans="1:12" ht="15.6">
       <c r="A75" s="78"/>
       <c r="B75" s="18">
         <v>4.9000000000000004</v>
@@ -8739,7 +8747,7 @@
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75">
+    <row r="76" spans="1:12" ht="15.6">
       <c r="A76" s="78"/>
       <c r="B76" s="18">
         <v>4.0999999999999996</v>
@@ -8759,7 +8767,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75">
+    <row r="77" spans="1:12" ht="15.6">
       <c r="A77" s="78"/>
       <c r="B77" s="18"/>
       <c r="C77" s="19" t="s">
@@ -8777,7 +8785,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75">
+    <row r="78" spans="1:12" ht="15.6">
       <c r="A78" s="78"/>
       <c r="B78" s="18">
         <v>4.1100000000000003</v>
@@ -8797,7 +8805,7 @@
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75">
+    <row r="79" spans="1:12" ht="15.6">
       <c r="A79" s="78"/>
       <c r="B79" s="18"/>
       <c r="C79" s="19" t="s">
@@ -8815,7 +8823,7 @@
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="1:12" ht="15.75">
+    <row r="80" spans="1:12" ht="15.6">
       <c r="A80" s="78"/>
       <c r="B80" s="18"/>
       <c r="C80" s="19" t="s">
@@ -8833,7 +8841,7 @@
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75">
+    <row r="81" spans="1:12" ht="15.6">
       <c r="A81" s="78"/>
       <c r="B81" s="18"/>
       <c r="C81" s="19" t="s">
@@ -8851,7 +8859,7 @@
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75">
+    <row r="82" spans="1:12" ht="15.6">
       <c r="A82" s="78"/>
       <c r="B82" s="18"/>
       <c r="C82" s="19" t="s">
@@ -8869,7 +8877,7 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" ht="15.75">
+    <row r="83" spans="1:12" ht="15.6">
       <c r="A83" s="78"/>
       <c r="B83" s="18">
         <v>4.12</v>
@@ -8889,7 +8897,7 @@
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" ht="15.75">
+    <row r="84" spans="1:12" ht="15.6">
       <c r="A84" s="78"/>
       <c r="B84" s="18"/>
       <c r="C84" s="19" t="s">
@@ -8907,7 +8915,7 @@
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" ht="15.75">
+    <row r="85" spans="1:12" ht="15.6">
       <c r="A85" s="78"/>
       <c r="B85" s="18"/>
       <c r="C85" s="19" t="s">
@@ -8925,7 +8933,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" ht="15.75">
+    <row r="86" spans="1:12" ht="15.6">
       <c r="A86" s="78"/>
       <c r="B86" s="18"/>
       <c r="C86" s="19" t="s">
@@ -8943,7 +8951,7 @@
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75">
+    <row r="87" spans="1:12" ht="15.6">
       <c r="A87" s="78"/>
       <c r="B87" s="18">
         <v>4.13</v>
@@ -8963,7 +8971,7 @@
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75">
+    <row r="88" spans="1:12" ht="15.6">
       <c r="A88" s="78"/>
       <c r="B88" s="18"/>
       <c r="C88" s="19" t="s">
@@ -8981,7 +8989,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75">
+    <row r="89" spans="1:12" ht="15.6">
       <c r="A89" s="78"/>
       <c r="B89" s="18">
         <v>4.1399999999999997</v>
@@ -9001,7 +9009,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75">
+    <row r="90" spans="1:12" ht="15.6">
       <c r="A90" s="78"/>
       <c r="B90" s="18">
         <v>4.1500000000000004</v>
@@ -9021,7 +9029,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75">
+    <row r="91" spans="1:12" ht="15.6">
       <c r="A91" s="78"/>
       <c r="B91" s="18"/>
       <c r="C91" s="19" t="s">
@@ -9039,7 +9047,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75">
+    <row r="92" spans="1:12" ht="15.6">
       <c r="A92" s="78"/>
       <c r="B92" s="18"/>
       <c r="C92" s="19" t="s">
@@ -9057,7 +9065,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75">
+    <row r="93" spans="1:12" ht="15.6">
       <c r="A93" s="78"/>
       <c r="B93" s="18"/>
       <c r="C93" s="19"/>
@@ -9075,7 +9083,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75">
+    <row r="94" spans="1:12" ht="15.6">
       <c r="A94" s="78"/>
       <c r="B94" s="17"/>
       <c r="C94" s="17"/>
@@ -9089,7 +9097,7 @@
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75">
+    <row r="95" spans="1:12" ht="15.6">
       <c r="A95" s="82"/>
       <c r="B95" s="79"/>
       <c r="C95" s="81" t="s">
@@ -9109,7 +9117,7 @@
       <c r="K95" s="56"/>
       <c r="L95" s="56"/>
     </row>
-    <row r="96" spans="1:12" ht="15.75">
+    <row r="96" spans="1:12" ht="15.6">
       <c r="A96" s="82"/>
       <c r="B96" s="79"/>
       <c r="C96" s="81"/>
@@ -9137,7 +9145,7 @@
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75">
+    <row r="98" spans="1:12" ht="15.6">
       <c r="A98" s="76">
         <v>5</v>
       </c>
@@ -9157,7 +9165,7 @@
       <c r="K98" s="3"/>
       <c r="L98" s="3"/>
     </row>
-    <row r="99" spans="1:12" ht="15.75">
+    <row r="99" spans="1:12" ht="15.6">
       <c r="A99" s="78"/>
       <c r="B99" s="18">
         <v>5.0999999999999996</v>
@@ -9177,7 +9185,7 @@
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75">
+    <row r="100" spans="1:12" ht="15.6">
       <c r="A100" s="78"/>
       <c r="B100" s="18">
         <v>5.2</v>
@@ -9197,7 +9205,7 @@
       <c r="K100" s="3"/>
       <c r="L100" s="3"/>
     </row>
-    <row r="101" spans="1:12" ht="15.75">
+    <row r="101" spans="1:12" ht="15.6">
       <c r="A101" s="78"/>
       <c r="B101" s="18">
         <v>5.3</v>
@@ -9217,7 +9225,7 @@
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
     </row>
-    <row r="102" spans="1:12" ht="15.75">
+    <row r="102" spans="1:12" ht="15.6">
       <c r="A102" s="78"/>
       <c r="B102" s="18"/>
       <c r="C102" s="19"/>
@@ -9231,7 +9239,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75">
+    <row r="103" spans="1:12" ht="15.6">
       <c r="A103" s="76">
         <v>6</v>
       </c>
@@ -9253,7 +9261,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
     </row>
-    <row r="104" spans="1:12" ht="15.75">
+    <row r="104" spans="1:12" ht="15.6">
       <c r="A104" s="78"/>
       <c r="B104" s="18">
         <v>6.1</v>
@@ -9271,7 +9279,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75">
+    <row r="105" spans="1:12" ht="15.6">
       <c r="A105" s="78"/>
       <c r="B105" s="18">
         <v>6.2</v>
@@ -9289,7 +9297,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75">
+    <row r="106" spans="1:12" ht="15.6">
       <c r="A106" s="78"/>
       <c r="B106" s="18">
         <v>6.3</v>
@@ -9307,7 +9315,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75">
+    <row r="107" spans="1:12" ht="15.6">
       <c r="A107" s="78"/>
       <c r="B107" s="18">
         <v>6.4</v>
@@ -9325,7 +9333,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="1:12" ht="15.75">
+    <row r="108" spans="1:12" ht="15.6">
       <c r="A108" s="78"/>
       <c r="B108" s="18">
         <v>6.5</v>
@@ -9343,7 +9351,7 @@
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
     </row>
-    <row r="109" spans="1:12" ht="15.75">
+    <row r="109" spans="1:12" ht="15.6">
       <c r="A109" s="78"/>
       <c r="B109" s="18">
         <v>6.6</v>
@@ -9361,7 +9369,7 @@
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
     </row>
-    <row r="110" spans="1:12" ht="15.75">
+    <row r="110" spans="1:12" ht="15.6">
       <c r="A110" s="78"/>
       <c r="B110" s="18"/>
       <c r="C110" s="19"/>
@@ -9375,7 +9383,7 @@
       <c r="K110" s="3"/>
       <c r="L110" s="3"/>
     </row>
-    <row r="111" spans="1:12" ht="94.5">
+    <row r="111" spans="1:12" ht="93.6">
       <c r="A111" s="82"/>
       <c r="B111" s="79"/>
       <c r="C111" s="81" t="s">
@@ -9432,7 +9440,7 @@
       <c r="K113" s="32"/>
       <c r="L113" s="32"/>
     </row>
-    <row r="114" spans="1:12" ht="15.75">
+    <row r="114" spans="1:12" ht="15.6">
       <c r="D114" s="22" t="s">
         <v>378</v>
       </c>

</xml_diff>

<commit_message>
Exception Handling Demo start
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RKIT\RKIT_Internship_work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2DBBA5-9CED-4EAA-8070-9A1F2CAE67CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BE280E-6A63-44AE-B021-8CA5E143DCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="21600" windowHeight="14130" activeTab="3" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
   <sheets>
     <sheet name=" Basic GUI" sheetId="1" r:id="rId1"/>
@@ -24,21 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="483">
   <si>
     <t>Topic</t>
   </si>
@@ -1493,6 +1484,9 @@
   </si>
   <si>
     <t>Ongoing</t>
+  </si>
+  <si>
+    <t>Final Demo</t>
   </si>
 </sst>
 </file>
@@ -1816,7 +1810,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2076,6 +2070,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2460,27 +2457,27 @@
       <selection activeCell="J95" sqref="J95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="72" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="72" customWidth="1"/>
     <col min="2" max="2" width="6" style="29" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
     <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="5" width="53.44140625" customWidth="1"/>
-    <col min="6" max="9" width="9.33203125" style="29" customWidth="1"/>
-    <col min="10" max="10" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="51.44140625" customWidth="1"/>
+    <col min="5" max="5" width="53.42578125" customWidth="1"/>
+    <col min="6" max="9" width="9.28515625" style="29" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="51.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="40" customFormat="1" ht="18">
-      <c r="A1" s="101" t="s">
+    <row r="1" spans="1:12" s="40" customFormat="1" ht="18.75">
+      <c r="A1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="103"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="104"/>
       <c r="F1" s="39" t="s">
         <v>425</v>
       </c>
@@ -2499,7 +2496,7 @@
       <c r="K1" s="41"/>
       <c r="L1" s="41"/>
     </row>
-    <row r="2" spans="1:12" s="29" customFormat="1" ht="18">
+    <row r="2" spans="1:12" s="29" customFormat="1" ht="18.75">
       <c r="A2" s="66">
         <v>1</v>
       </c>
@@ -2523,7 +2520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6">
+    <row r="3" spans="1:12" ht="15.75">
       <c r="A3" s="47"/>
       <c r="B3" s="46">
         <v>1.1000000000000001</v>
@@ -2551,7 +2548,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="31.2">
+    <row r="4" spans="1:12" ht="31.5">
       <c r="A4" s="67"/>
       <c r="B4" s="24"/>
       <c r="C4" s="31" t="s">
@@ -2571,7 +2568,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="15.6">
+    <row r="5" spans="1:12" ht="15.75">
       <c r="A5" s="67"/>
       <c r="B5" s="24"/>
       <c r="C5" s="31" t="s">
@@ -2589,7 +2586,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="15.6">
+    <row r="6" spans="1:12" ht="15.75">
       <c r="A6" s="67"/>
       <c r="B6" s="24"/>
       <c r="C6" s="31" t="s">
@@ -2607,7 +2604,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="15.6">
+    <row r="7" spans="1:12" ht="15.75">
       <c r="A7" s="47"/>
       <c r="B7" s="49">
         <v>1.2</v>
@@ -2635,7 +2632,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15.6">
+    <row r="8" spans="1:12" ht="15.75">
       <c r="A8" s="67"/>
       <c r="B8" s="24"/>
       <c r="C8" s="31" t="s">
@@ -2653,7 +2650,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="15.6">
+    <row r="9" spans="1:12" ht="15.75">
       <c r="A9" s="67"/>
       <c r="B9" s="24"/>
       <c r="C9" s="31" t="s">
@@ -2671,7 +2668,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15.6">
+    <row r="10" spans="1:12" ht="15.75">
       <c r="A10" s="67"/>
       <c r="B10" s="24"/>
       <c r="C10" s="31" t="s">
@@ -2689,7 +2686,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15.6">
+    <row r="11" spans="1:12" ht="15.75">
       <c r="A11" s="67"/>
       <c r="B11" s="24"/>
       <c r="C11" s="31" t="s">
@@ -2707,7 +2704,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15.6">
+    <row r="12" spans="1:12" ht="15.75">
       <c r="A12" s="67"/>
       <c r="B12" s="24"/>
       <c r="C12" s="31" t="s">
@@ -2725,7 +2722,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15.6">
+    <row r="13" spans="1:12" ht="15.75">
       <c r="A13" s="67"/>
       <c r="B13" s="24"/>
       <c r="C13" s="31" t="s">
@@ -2743,7 +2740,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15.6">
+    <row r="14" spans="1:12" ht="15.75">
       <c r="A14" s="67"/>
       <c r="B14" s="24"/>
       <c r="C14" s="31" t="s">
@@ -2761,7 +2758,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="15.6">
+    <row r="15" spans="1:12" ht="15.75">
       <c r="A15" s="67"/>
       <c r="B15" s="24"/>
       <c r="C15" s="31" t="s">
@@ -2779,7 +2776,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15.6">
+    <row r="16" spans="1:12" ht="15.75">
       <c r="A16" s="67"/>
       <c r="B16" s="24"/>
       <c r="C16" s="31" t="s">
@@ -2797,7 +2794,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" ht="15.6">
+    <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="47"/>
       <c r="B17" s="49">
         <v>1.3</v>
@@ -2825,7 +2822,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" ht="15.6">
+    <row r="18" spans="1:12" ht="15.75">
       <c r="A18" s="67"/>
       <c r="B18" s="24"/>
       <c r="C18" s="31" t="s">
@@ -2843,7 +2840,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" ht="15.6">
+    <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="67"/>
       <c r="B19" s="24"/>
       <c r="C19" s="31" t="s">
@@ -2861,7 +2858,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" ht="15.6">
+    <row r="20" spans="1:12" ht="15.75">
       <c r="A20" s="67"/>
       <c r="B20" s="24"/>
       <c r="C20" s="31" t="s">
@@ -2879,7 +2876,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" ht="15.6">
+    <row r="21" spans="1:12" ht="15.75">
       <c r="A21" s="67"/>
       <c r="B21" s="24"/>
       <c r="C21" s="31" t="s">
@@ -2897,7 +2894,7 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:12" ht="15.6">
+    <row r="22" spans="1:12" ht="15.75">
       <c r="A22" s="47"/>
       <c r="B22" s="49">
         <v>1.4</v>
@@ -2927,7 +2924,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12" ht="15.6">
+    <row r="23" spans="1:12" ht="15.75">
       <c r="A23" s="67"/>
       <c r="B23" s="24"/>
       <c r="C23" s="31" t="s">
@@ -2945,7 +2942,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" ht="15.6">
+    <row r="24" spans="1:12" ht="15.75">
       <c r="A24" s="67"/>
       <c r="B24" s="24"/>
       <c r="C24" s="31" t="s">
@@ -2963,7 +2960,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" ht="31.2">
+    <row r="25" spans="1:12" ht="31.5">
       <c r="A25" s="67"/>
       <c r="B25" s="24"/>
       <c r="C25" s="31" t="s">
@@ -2981,7 +2978,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:12" ht="15.6">
+    <row r="26" spans="1:12" ht="15.75">
       <c r="A26" s="67"/>
       <c r="B26" s="24"/>
       <c r="C26" s="31"/>
@@ -2995,7 +2992,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:12" ht="15.6">
+    <row r="27" spans="1:12" ht="15.75">
       <c r="A27" s="85"/>
       <c r="B27" s="86">
         <v>1.5</v>
@@ -3025,7 +3022,7 @@
       <c r="K27" s="56"/>
       <c r="L27" s="56"/>
     </row>
-    <row r="28" spans="1:12" ht="15.6">
+    <row r="28" spans="1:12" ht="15.75">
       <c r="A28" s="67"/>
       <c r="B28" s="24"/>
       <c r="C28" s="31"/>
@@ -3039,7 +3036,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" ht="18">
+    <row r="29" spans="1:12" ht="18.75">
       <c r="A29" s="66">
         <v>2</v>
       </c>
@@ -3057,7 +3054,7 @@
       <c r="K29" s="44"/>
       <c r="L29" s="44"/>
     </row>
-    <row r="30" spans="1:12" ht="15.6">
+    <row r="30" spans="1:12" ht="15.75">
       <c r="A30" s="47"/>
       <c r="B30" s="50">
         <v>2.1</v>
@@ -3085,7 +3082,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12" ht="15.6">
+    <row r="31" spans="1:12" ht="15.75">
       <c r="A31" s="67"/>
       <c r="B31" s="24"/>
       <c r="C31" s="11" t="s">
@@ -3105,7 +3102,7 @@
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
     </row>
-    <row r="32" spans="1:12" ht="46.8">
+    <row r="32" spans="1:12" ht="47.25">
       <c r="A32" s="67"/>
       <c r="B32" s="24"/>
       <c r="C32" s="11" t="s">
@@ -3125,7 +3122,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="1:12" ht="15.6">
+    <row r="33" spans="1:12" ht="15.75">
       <c r="A33" s="67"/>
       <c r="B33" s="24"/>
       <c r="C33" s="11" t="s">
@@ -3145,7 +3142,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="1:12" ht="15.6">
+    <row r="34" spans="1:12" ht="15.75">
       <c r="A34" s="67"/>
       <c r="B34" s="24"/>
       <c r="C34" s="11" t="s">
@@ -3165,7 +3162,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="1:12" ht="15.6">
+    <row r="35" spans="1:12" ht="15.75">
       <c r="A35" s="67"/>
       <c r="B35" s="24"/>
       <c r="C35" s="11" t="s">
@@ -3183,7 +3180,7 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="1:12" ht="15.6">
+    <row r="36" spans="1:12" ht="15.75">
       <c r="A36" s="67"/>
       <c r="B36" s="24"/>
       <c r="C36" s="11" t="s">
@@ -3203,7 +3200,7 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="1:12" ht="15.6">
+    <row r="37" spans="1:12" ht="15.75">
       <c r="A37" s="67"/>
       <c r="B37" s="24"/>
       <c r="C37" s="11"/>
@@ -3217,7 +3214,7 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="1:12" ht="15.6">
+    <row r="38" spans="1:12" ht="15.75">
       <c r="A38" s="85"/>
       <c r="B38" s="89" t="s">
         <v>70</v>
@@ -3247,7 +3244,7 @@
       <c r="K38" s="56"/>
       <c r="L38" s="56"/>
     </row>
-    <row r="39" spans="1:12" ht="15.6">
+    <row r="39" spans="1:12" ht="15.75">
       <c r="A39" s="67"/>
       <c r="B39" s="24"/>
       <c r="C39" s="31"/>
@@ -3261,7 +3258,7 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="1:12" ht="18">
+    <row r="40" spans="1:12" ht="18.75">
       <c r="A40" s="66">
         <v>3</v>
       </c>
@@ -3279,7 +3276,7 @@
       <c r="K40" s="44"/>
       <c r="L40" s="44"/>
     </row>
-    <row r="41" spans="1:12" ht="15.6">
+    <row r="41" spans="1:12" ht="15.75">
       <c r="A41" s="6"/>
       <c r="B41" s="49">
         <v>3.1</v>
@@ -3307,7 +3304,7 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="1:12" ht="15.6">
+    <row r="42" spans="1:12" ht="15.75">
       <c r="A42" s="67"/>
       <c r="B42" s="51"/>
       <c r="C42" s="11" t="s">
@@ -3325,7 +3322,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="1:12" ht="15.6">
+    <row r="43" spans="1:12" ht="15.75">
       <c r="A43" s="67"/>
       <c r="B43" s="24"/>
       <c r="C43" s="11" t="s">
@@ -3343,7 +3340,7 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="1:12" ht="15.6">
+    <row r="44" spans="1:12" ht="15.75">
       <c r="A44" s="67"/>
       <c r="B44" s="24"/>
       <c r="C44" s="11" t="s">
@@ -3361,7 +3358,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="1:12" ht="15.6">
+    <row r="45" spans="1:12" ht="15.75">
       <c r="A45" s="67"/>
       <c r="B45" s="24"/>
       <c r="C45" s="11"/>
@@ -3375,11 +3372,11 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="1:12" ht="15.6">
+    <row r="46" spans="1:12" ht="15.75">
       <c r="A46" s="67"/>
       <c r="B46" s="24"/>
-      <c r="C46" s="100"/>
-      <c r="D46" s="100"/>
+      <c r="C46" s="101"/>
+      <c r="D46" s="101"/>
       <c r="E46" s="8"/>
       <c r="F46" s="27"/>
       <c r="G46" s="27"/>
@@ -3389,7 +3386,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="1:12" ht="18">
+    <row r="47" spans="1:12" ht="18.75">
       <c r="A47" s="66">
         <v>4</v>
       </c>
@@ -3407,7 +3404,7 @@
       <c r="K47" s="44"/>
       <c r="L47" s="44"/>
     </row>
-    <row r="48" spans="1:12" ht="15.6">
+    <row r="48" spans="1:12" ht="15.75">
       <c r="A48" s="6"/>
       <c r="B48" s="49">
         <v>4.0999999999999996</v>
@@ -3437,7 +3434,7 @@
       </c>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:12" ht="15.6">
+    <row r="49" spans="1:12" ht="15.75">
       <c r="A49" s="67"/>
       <c r="B49" s="51"/>
       <c r="C49" s="11" t="s">
@@ -3455,7 +3452,7 @@
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:12" ht="15.6">
+    <row r="50" spans="1:12" ht="15.75">
       <c r="A50" s="67"/>
       <c r="B50" s="24"/>
       <c r="C50" s="11" t="s">
@@ -3473,7 +3470,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="1:12" ht="15.6">
+    <row r="51" spans="1:12" ht="15.75">
       <c r="A51" s="67"/>
       <c r="B51" s="24"/>
       <c r="C51" s="11" t="s">
@@ -3491,7 +3488,7 @@
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="1:12" ht="15.6">
+    <row r="52" spans="1:12" ht="15.75">
       <c r="A52" s="67"/>
       <c r="B52" s="24"/>
       <c r="C52" s="11" t="s">
@@ -3509,7 +3506,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="1:12" ht="15.6">
+    <row r="53" spans="1:12" ht="15.75">
       <c r="A53" s="67"/>
       <c r="B53" s="24"/>
       <c r="C53" s="11" t="s">
@@ -3527,7 +3524,7 @@
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="1:12" ht="15.6">
+    <row r="54" spans="1:12" ht="15.75">
       <c r="A54" s="67"/>
       <c r="B54" s="24"/>
       <c r="C54" s="11" t="s">
@@ -3545,7 +3542,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="1:12" ht="15.6">
+    <row r="55" spans="1:12" ht="15.75">
       <c r="A55" s="67"/>
       <c r="B55" s="24"/>
       <c r="C55" s="11"/>
@@ -3559,7 +3556,7 @@
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="1:12" ht="15.6">
+    <row r="56" spans="1:12" ht="15.75">
       <c r="A56" s="85"/>
       <c r="B56" s="89" t="s">
         <v>93</v>
@@ -3603,7 +3600,7 @@
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="1:12" ht="18">
+    <row r="58" spans="1:12" ht="18.75">
       <c r="A58" s="66">
         <v>5</v>
       </c>
@@ -3635,7 +3632,7 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="1:12" ht="15.6">
+    <row r="60" spans="1:12" ht="15.75">
       <c r="A60" s="69">
         <v>1</v>
       </c>
@@ -3665,7 +3662,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="15.6">
+    <row r="61" spans="1:12" ht="15.75">
       <c r="A61" s="67"/>
       <c r="B61" s="52">
         <v>1.1000000000000001</v>
@@ -3683,7 +3680,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="1:12" ht="15.6">
+    <row r="62" spans="1:12" ht="15.75">
       <c r="A62" s="67"/>
       <c r="B62" s="52">
         <v>1.2</v>
@@ -3701,7 +3698,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="1:12" ht="15.6">
+    <row r="63" spans="1:12" ht="15.75">
       <c r="A63" s="67"/>
       <c r="B63" s="52">
         <v>1.3</v>
@@ -3731,7 +3728,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="15.6">
+    <row r="64" spans="1:12" ht="15.75">
       <c r="A64" s="67"/>
       <c r="B64" s="52"/>
       <c r="C64" s="8" t="s">
@@ -3751,7 +3748,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="31.2">
+    <row r="65" spans="1:12" ht="31.5">
       <c r="A65" s="47"/>
       <c r="B65" s="52"/>
       <c r="C65" s="8" t="s">
@@ -3769,7 +3766,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" ht="15.6">
+    <row r="66" spans="1:12" ht="15.75">
       <c r="A66" s="67"/>
       <c r="B66" s="52"/>
       <c r="C66" s="8" t="s">
@@ -3787,7 +3784,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:12" ht="15.6">
+    <row r="67" spans="1:12" ht="15.75">
       <c r="A67" s="69">
         <v>2</v>
       </c>
@@ -3815,7 +3812,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" ht="15.6">
+    <row r="68" spans="1:12" ht="15.75">
       <c r="A68" s="70"/>
       <c r="B68" s="52">
         <v>2.1</v>
@@ -3833,7 +3830,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" ht="15.6">
+    <row r="69" spans="1:12" ht="15.75">
       <c r="A69" s="70"/>
       <c r="B69" s="52">
         <v>2.2000000000000002</v>
@@ -3851,7 +3848,7 @@
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:12" ht="15.6">
+    <row r="70" spans="1:12" ht="15.75">
       <c r="A70" s="70"/>
       <c r="B70" s="52">
         <v>2.2999999999999998</v>
@@ -3869,7 +3866,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" ht="15.6">
+    <row r="71" spans="1:12" ht="15.75">
       <c r="A71" s="70"/>
       <c r="B71" s="52"/>
       <c r="C71" s="8"/>
@@ -3883,7 +3880,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" ht="15.6">
+    <row r="72" spans="1:12" ht="15.75">
       <c r="A72" s="69">
         <v>3</v>
       </c>
@@ -3913,7 +3910,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" ht="15.6">
+    <row r="73" spans="1:12" ht="15.75">
       <c r="A73" s="70"/>
       <c r="B73" s="52">
         <v>3.1</v>
@@ -3931,7 +3928,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" ht="15.6">
+    <row r="74" spans="1:12" ht="15.75">
       <c r="A74" s="70"/>
       <c r="B74" s="52">
         <v>3.2</v>
@@ -3949,7 +3946,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" ht="15.6">
+    <row r="75" spans="1:12" ht="15.75">
       <c r="A75" s="70"/>
       <c r="B75" s="52">
         <v>3.3</v>
@@ -3967,7 +3964,7 @@
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" ht="15.6">
+    <row r="76" spans="1:12" ht="15.75">
       <c r="A76" s="70"/>
       <c r="B76" s="52">
         <v>3.4</v>
@@ -3985,7 +3982,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" ht="15.6">
+    <row r="77" spans="1:12" ht="15.75">
       <c r="A77" s="69">
         <v>4</v>
       </c>
@@ -4013,7 +4010,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" ht="15.6">
+    <row r="78" spans="1:12" ht="15.75">
       <c r="A78" s="70"/>
       <c r="B78" s="52">
         <v>4.0999999999999996</v>
@@ -4045,7 +4042,7 @@
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="1:12" ht="18">
+    <row r="80" spans="1:12" ht="18.75">
       <c r="A80" s="66">
         <v>5</v>
       </c>
@@ -4063,7 +4060,7 @@
       <c r="K80" s="44"/>
       <c r="L80" s="44"/>
     </row>
-    <row r="81" spans="1:12" ht="15.6">
+    <row r="81" spans="1:12" ht="15.75">
       <c r="A81" s="6"/>
       <c r="B81" s="49">
         <v>5.0999999999999996</v>
@@ -4091,7 +4088,7 @@
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" ht="15.6">
+    <row r="82" spans="1:12" ht="15.75">
       <c r="A82" s="67"/>
       <c r="B82" s="24"/>
       <c r="C82" s="11" t="s">
@@ -4109,7 +4106,7 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" ht="31.2">
+    <row r="83" spans="1:12" ht="31.5">
       <c r="A83" s="67"/>
       <c r="B83" s="24"/>
       <c r="C83" s="11" t="s">
@@ -4127,7 +4124,7 @@
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" ht="31.2">
+    <row r="84" spans="1:12" ht="31.5">
       <c r="A84" s="67"/>
       <c r="B84" s="24"/>
       <c r="C84" s="11" t="s">
@@ -4147,7 +4144,7 @@
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" ht="31.2">
+    <row r="85" spans="1:12" ht="31.5">
       <c r="A85" s="67"/>
       <c r="B85" s="24"/>
       <c r="C85" s="11" t="s">
@@ -4167,7 +4164,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" ht="31.2">
+    <row r="86" spans="1:12" ht="31.5">
       <c r="A86" s="47"/>
       <c r="B86" s="49">
         <v>5.2</v>
@@ -4197,7 +4194,7 @@
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="1:12" ht="15.6">
+    <row r="87" spans="1:12" ht="15.75">
       <c r="A87" s="67"/>
       <c r="B87" s="24"/>
       <c r="C87" s="11" t="s">
@@ -4215,7 +4212,7 @@
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="1:12" ht="15.6">
+    <row r="88" spans="1:12" ht="15.75">
       <c r="A88" s="67"/>
       <c r="B88" s="24"/>
       <c r="C88" s="11" t="s">
@@ -4233,7 +4230,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="1:12" ht="15.6">
+    <row r="89" spans="1:12" ht="15.75">
       <c r="A89" s="67"/>
       <c r="B89" s="24"/>
       <c r="C89" s="11" t="s">
@@ -4251,7 +4248,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="1:12" ht="15.6">
+    <row r="90" spans="1:12" ht="15.75">
       <c r="A90" s="67"/>
       <c r="B90" s="24"/>
       <c r="C90" s="11"/>
@@ -4265,7 +4262,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="1:12" ht="15.6">
+    <row r="91" spans="1:12" ht="15.75">
       <c r="A91" s="47"/>
       <c r="B91" s="49">
         <v>5.3</v>
@@ -4293,7 +4290,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:12" ht="15.6">
+    <row r="92" spans="1:12" ht="15.75">
       <c r="A92" s="67"/>
       <c r="B92" s="24"/>
       <c r="C92" s="11" t="s">
@@ -4311,7 +4308,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="1:12" ht="15.6">
+    <row r="93" spans="1:12" ht="15.75">
       <c r="A93" s="67"/>
       <c r="B93" s="24"/>
       <c r="C93" s="11" t="s">
@@ -4329,7 +4326,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
     </row>
-    <row r="94" spans="1:12" ht="15.6">
+    <row r="94" spans="1:12" ht="15.75">
       <c r="A94" s="67"/>
       <c r="B94" s="24"/>
       <c r="C94" s="11"/>
@@ -4343,7 +4340,7 @@
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
     </row>
-    <row r="95" spans="1:12" ht="31.2">
+    <row r="95" spans="1:12" ht="47.25">
       <c r="A95" s="67"/>
       <c r="B95" s="49">
         <v>5.4</v>
@@ -4373,7 +4370,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="28.8">
+    <row r="96" spans="1:12" ht="30">
       <c r="A96" s="47"/>
       <c r="B96" s="49">
         <v>5.5</v>
@@ -4393,7 +4390,7 @@
       <c r="K96" s="3"/>
       <c r="L96" s="3"/>
     </row>
-    <row r="97" spans="1:12" ht="15.6">
+    <row r="97" spans="1:12" ht="15.75">
       <c r="A97" s="47"/>
       <c r="B97" s="49">
         <v>5.6</v>
@@ -4411,7 +4408,7 @@
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
     </row>
-    <row r="98" spans="1:12" ht="15.6">
+    <row r="98" spans="1:12" ht="15.75">
       <c r="A98" s="47"/>
       <c r="B98" s="49">
         <v>5.7</v>
@@ -4445,7 +4442,7 @@
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
     </row>
-    <row r="100" spans="1:12" ht="15.6">
+    <row r="100" spans="1:12" ht="15.75">
       <c r="A100" s="6"/>
       <c r="B100" s="1">
         <v>5.8</v>
@@ -4477,7 +4474,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="15.6">
+    <row r="101" spans="1:12" ht="15.75">
       <c r="A101" s="67"/>
       <c r="B101" s="24"/>
       <c r="C101" s="11" t="s">
@@ -4497,7 +4494,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="15.6">
+    <row r="102" spans="1:12" ht="15.75">
       <c r="A102" s="67"/>
       <c r="B102" s="24"/>
       <c r="C102" s="11" t="s">
@@ -4515,7 +4512,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
     </row>
-    <row r="103" spans="1:12" ht="15.6">
+    <row r="103" spans="1:12" ht="15.75">
       <c r="A103" s="67"/>
       <c r="B103" s="24"/>
       <c r="C103" s="11" t="s">
@@ -4533,7 +4530,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
     </row>
-    <row r="104" spans="1:12" ht="31.2">
+    <row r="104" spans="1:12" ht="31.5">
       <c r="A104" s="67"/>
       <c r="B104" s="24"/>
       <c r="C104" s="11" t="s">
@@ -4551,7 +4548,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
     </row>
-    <row r="105" spans="1:12" ht="15.6">
+    <row r="105" spans="1:12" ht="15.75">
       <c r="A105" s="67"/>
       <c r="B105" s="24"/>
       <c r="C105" s="11" t="s">
@@ -4571,7 +4568,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
     </row>
-    <row r="106" spans="1:12" ht="15.6">
+    <row r="106" spans="1:12" ht="15.75">
       <c r="A106" s="67"/>
       <c r="B106" s="24"/>
       <c r="C106" s="11" t="s">
@@ -4589,7 +4586,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
     </row>
-    <row r="107" spans="1:12" ht="15.6">
+    <row r="107" spans="1:12" ht="15.75">
       <c r="A107" s="67"/>
       <c r="B107" s="24"/>
       <c r="C107" s="11"/>
@@ -4603,7 +4600,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="1:12" s="20" customFormat="1" ht="36">
+    <row r="108" spans="1:12" s="20" customFormat="1" ht="37.5">
       <c r="A108" s="71">
         <v>6</v>
       </c>
@@ -4634,13 +4631,13 @@
       </c>
     </row>
     <row r="109" spans="1:12">
-      <c r="A109" s="97" t="s">
+      <c r="A109" s="98" t="s">
         <v>155</v>
       </c>
-      <c r="B109" s="98"/>
-      <c r="C109" s="98"/>
-      <c r="D109" s="98"/>
-      <c r="E109" s="99"/>
+      <c r="B109" s="99"/>
+      <c r="C109" s="99"/>
+      <c r="D109" s="99"/>
+      <c r="E109" s="100"/>
       <c r="F109" s="33">
         <f>SUM(F3:F108)</f>
         <v>95</v>
@@ -4655,13 +4652,13 @@
       <c r="L109" s="32"/>
     </row>
     <row r="110" spans="1:12">
-      <c r="A110" s="97" t="s">
+      <c r="A110" s="98" t="s">
         <v>156</v>
       </c>
-      <c r="B110" s="98"/>
-      <c r="C110" s="98"/>
-      <c r="D110" s="98"/>
-      <c r="E110" s="99"/>
+      <c r="B110" s="99"/>
+      <c r="C110" s="99"/>
+      <c r="D110" s="99"/>
+      <c r="E110" s="100"/>
       <c r="F110" s="33">
         <v>100</v>
       </c>
@@ -4717,18 +4714,18 @@
       <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" style="29" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" style="29" customWidth="1"/>
-    <col min="3" max="3" width="65.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" style="29" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="29" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="89.109375" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" style="29" customWidth="1"/>
+    <col min="3" max="3" width="65.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" style="29" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="29" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="89.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="29" customFormat="1">
@@ -4763,7 +4760,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="43.2">
+    <row r="2" spans="1:10" ht="45">
       <c r="A2" s="28" t="s">
         <v>160</v>
       </c>
@@ -5395,7 +5392,7 @@
       <c r="C28" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="D28" s="104">
+      <c r="D28" s="105">
         <v>8</v>
       </c>
       <c r="E28" s="27"/>
@@ -5417,7 +5414,7 @@
       <c r="C29" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D29" s="104"/>
+      <c r="D29" s="105"/>
       <c r="E29" s="27"/>
       <c r="F29" s="94">
         <v>45640</v>
@@ -5437,7 +5434,7 @@
       <c r="C30" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D30" s="104"/>
+      <c r="D30" s="105"/>
       <c r="E30" s="27">
         <v>7</v>
       </c>
@@ -5481,10 +5478,10 @@
       <c r="A33" s="55" t="s">
         <v>194</v>
       </c>
-      <c r="B33" s="105" t="s">
+      <c r="B33" s="106" t="s">
         <v>379</v>
       </c>
-      <c r="C33" s="105"/>
+      <c r="C33" s="106"/>
       <c r="D33" s="57">
         <v>8</v>
       </c>
@@ -5839,10 +5836,10 @@
       <c r="A56" s="55" t="s">
         <v>216</v>
       </c>
-      <c r="B56" s="105" t="s">
+      <c r="B56" s="106" t="s">
         <v>380</v>
       </c>
-      <c r="C56" s="105"/>
+      <c r="C56" s="106"/>
       <c r="D56" s="57">
         <v>14</v>
       </c>
@@ -6091,10 +6088,10 @@
       <c r="A70" s="55" t="s">
         <v>226</v>
       </c>
-      <c r="B70" s="105" t="s">
+      <c r="B70" s="106" t="s">
         <v>381</v>
       </c>
-      <c r="C70" s="105"/>
+      <c r="C70" s="106"/>
       <c r="D70" s="57">
         <v>8</v>
       </c>
@@ -6110,11 +6107,11 @@
       <c r="J70" s="56"/>
     </row>
     <row r="71" spans="1:10">
-      <c r="A71" s="97" t="s">
+      <c r="A71" s="98" t="s">
         <v>155</v>
       </c>
-      <c r="B71" s="98"/>
-      <c r="C71" s="99"/>
+      <c r="B71" s="99"/>
+      <c r="C71" s="100"/>
       <c r="D71" s="33">
         <f>SUM(D2:D70)</f>
         <v>110.5</v>
@@ -6127,11 +6124,11 @@
       <c r="J71" s="32"/>
     </row>
     <row r="72" spans="1:10">
-      <c r="A72" s="97" t="s">
+      <c r="A72" s="98" t="s">
         <v>156</v>
       </c>
-      <c r="B72" s="98"/>
-      <c r="C72" s="99"/>
+      <c r="B72" s="99"/>
+      <c r="C72" s="100"/>
       <c r="D72" s="33">
         <v>120.5</v>
       </c>
@@ -6164,21 +6161,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51642604-D68B-4E5E-9160-A3EE5943E7C7}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E2:E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="29"/>
-    <col min="2" max="2" width="25.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="29"/>
+    <col min="2" max="2" width="25.28515625" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="29"/>
-    <col min="5" max="5" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" style="29" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="29"/>
+    <col min="5" max="5" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="29" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="29" customFormat="1">
@@ -6631,10 +6628,10 @@
       <c r="A24" s="55" t="s">
         <v>226</v>
       </c>
-      <c r="B24" s="105" t="s">
+      <c r="B24" s="106" t="s">
         <v>382</v>
       </c>
-      <c r="C24" s="105"/>
+      <c r="C24" s="106"/>
       <c r="D24" s="57">
         <v>12</v>
       </c>
@@ -6670,11 +6667,11 @@
       <c r="J25" s="3"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="97" t="s">
+      <c r="A26" s="98" t="s">
         <v>155</v>
       </c>
-      <c r="B26" s="98"/>
-      <c r="C26" s="99"/>
+      <c r="B26" s="99"/>
+      <c r="C26" s="100"/>
       <c r="D26" s="33">
         <f>SUM(D2:D25)</f>
         <v>54</v>
@@ -6695,7 +6692,10 @@
       <c r="D27" s="33">
         <v>64</v>
       </c>
-      <c r="E27" s="33"/>
+      <c r="E27" s="33">
+        <f>SUM(E2:E26)</f>
+        <v>62.5</v>
+      </c>
       <c r="F27" s="33"/>
       <c r="G27" s="33"/>
       <c r="H27" s="32"/>
@@ -6721,25 +6721,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE125957-E0FE-4793-875C-A900941606E5}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="29"/>
-    <col min="2" max="2" width="40.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="29"/>
+    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="29" customFormat="1">
@@ -7097,13 +7097,13 @@
         <v>10</v>
       </c>
       <c r="F17" s="27">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G17" s="94">
-        <v>45686</v>
+        <v>45691</v>
       </c>
       <c r="H17" s="27" t="s">
-        <v>481</v>
+        <v>433</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -7206,9 +7206,15 @@
       <c r="E23" s="27">
         <v>2</v>
       </c>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
+      <c r="F23" s="27">
+        <v>2</v>
+      </c>
+      <c r="G23" s="94">
+        <v>45691</v>
+      </c>
+      <c r="H23" s="27" t="s">
+        <v>433</v>
+      </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -7259,9 +7265,15 @@
       <c r="E26" s="27">
         <v>2</v>
       </c>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
+      <c r="F26" s="27">
+        <v>2</v>
+      </c>
+      <c r="G26" s="94">
+        <v>45691</v>
+      </c>
+      <c r="H26" s="27" t="s">
+        <v>433</v>
+      </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -7284,44 +7296,73 @@
       <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="97" t="s">
+      <c r="A28" s="98" t="s">
         <v>155</v>
       </c>
-      <c r="B28" s="98"/>
-      <c r="C28" s="98"/>
-      <c r="D28" s="99"/>
+      <c r="B28" s="99"/>
+      <c r="C28" s="99"/>
+      <c r="D28" s="100"/>
       <c r="E28" s="33">
         <f>SUM(E2:E27)</f>
         <v>34.5</v>
       </c>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
+      <c r="F28" s="33">
+        <v>39.5</v>
+      </c>
+      <c r="G28" s="97">
+        <v>45691</v>
+      </c>
+      <c r="H28" s="33" t="s">
+        <v>433</v>
+      </c>
       <c r="I28" s="32"/>
       <c r="J28" s="32"/>
       <c r="K28" s="32"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="97" t="s">
-        <v>156</v>
-      </c>
-      <c r="B29" s="98"/>
-      <c r="C29" s="98"/>
-      <c r="D29" s="99"/>
-      <c r="E29" s="90">
-        <v>44.5</v>
-      </c>
-      <c r="F29" s="90"/>
-      <c r="G29" s="90"/>
-      <c r="H29" s="90"/>
+      <c r="A29" s="91"/>
+      <c r="B29" s="92" t="s">
+        <v>482</v>
+      </c>
+      <c r="C29" s="92"/>
+      <c r="D29" s="93"/>
+      <c r="E29" s="33">
+        <v>10</v>
+      </c>
+      <c r="F29" s="33">
+        <v>7.75</v>
+      </c>
+      <c r="G29" s="97">
+        <v>45692</v>
+      </c>
+      <c r="H29" s="33" t="s">
+        <v>481</v>
+      </c>
       <c r="I29" s="32"/>
       <c r="J29" s="32"/>
       <c r="K29" s="32"/>
     </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="98" t="s">
+        <v>156</v>
+      </c>
+      <c r="B30" s="99"/>
+      <c r="C30" s="99"/>
+      <c r="D30" s="100"/>
+      <c r="E30" s="90">
+        <v>44.5</v>
+      </c>
+      <c r="F30" s="90"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="90"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{B4DD89C1-C2AF-41F5-BD01-A0C9F40FB553}">
@@ -7340,43 +7381,43 @@
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="29"/>
-    <col min="4" max="4" width="66.88671875" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="29"/>
+    <col min="4" max="4" width="66.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="107" t="s">
         <v>275</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="106"/>
-      <c r="L1" s="106"/>
-    </row>
-    <row r="2" spans="1:12" ht="18">
-      <c r="A2" s="107" t="s">
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+    </row>
+    <row r="2" spans="1:12" ht="18.75">
+      <c r="A2" s="108" t="s">
         <v>422</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
       <c r="F2" s="73" t="s">
         <v>1</v>
       </c>
@@ -7399,7 +7440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6">
+    <row r="3" spans="1:12" ht="15.75">
       <c r="A3" s="23"/>
       <c r="B3" s="16"/>
       <c r="C3" s="15"/>
@@ -7415,7 +7456,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="15.6">
+    <row r="4" spans="1:12" ht="15.75">
       <c r="A4" s="76">
         <v>1</v>
       </c>
@@ -7425,7 +7466,7 @@
         <v>276</v>
       </c>
       <c r="E4" s="16"/>
-      <c r="F4" s="108">
+      <c r="F4" s="109">
         <v>4</v>
       </c>
       <c r="G4" s="23"/>
@@ -7435,7 +7476,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="15.6">
+    <row r="5" spans="1:12" ht="15.75">
       <c r="A5" s="78"/>
       <c r="B5" s="18">
         <v>1.1000000000000001</v>
@@ -7447,7 +7488,7 @@
       <c r="E5" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F5" s="108"/>
+      <c r="F5" s="109"/>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
@@ -7455,7 +7496,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="15.6">
+    <row r="6" spans="1:12" ht="15.75">
       <c r="A6" s="78"/>
       <c r="B6" s="18">
         <v>1.2</v>
@@ -7467,7 +7508,7 @@
       <c r="E6" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F6" s="108"/>
+      <c r="F6" s="109"/>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
@@ -7475,7 +7516,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="15.6">
+    <row r="7" spans="1:12" ht="15.75">
       <c r="A7" s="78"/>
       <c r="B7" s="18">
         <v>1.3</v>
@@ -7487,7 +7528,7 @@
       <c r="E7" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F7" s="108"/>
+      <c r="F7" s="109"/>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
@@ -7495,7 +7536,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15.6">
+    <row r="8" spans="1:12" ht="15.75">
       <c r="A8" s="78"/>
       <c r="B8" s="18"/>
       <c r="C8" s="19" t="s">
@@ -7505,7 +7546,7 @@
         <v>280</v>
       </c>
       <c r="E8" s="18"/>
-      <c r="F8" s="108"/>
+      <c r="F8" s="109"/>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
@@ -7513,7 +7554,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="15.6">
+    <row r="9" spans="1:12" ht="15.75">
       <c r="A9" s="78"/>
       <c r="B9" s="18"/>
       <c r="C9" s="19" t="s">
@@ -7523,7 +7564,7 @@
         <v>281</v>
       </c>
       <c r="E9" s="18"/>
-      <c r="F9" s="108"/>
+      <c r="F9" s="109"/>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
       <c r="I9" s="23"/>
@@ -7531,7 +7572,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15.6">
+    <row r="10" spans="1:12" ht="15.75">
       <c r="A10" s="78"/>
       <c r="B10" s="18"/>
       <c r="C10" s="19" t="s">
@@ -7541,7 +7582,7 @@
         <v>282</v>
       </c>
       <c r="E10" s="18"/>
-      <c r="F10" s="108"/>
+      <c r="F10" s="109"/>
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
       <c r="I10" s="23"/>
@@ -7549,7 +7590,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15.6">
+    <row r="11" spans="1:12" ht="15.75">
       <c r="A11" s="78"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19" t="s">
@@ -7559,7 +7600,7 @@
         <v>284</v>
       </c>
       <c r="E11" s="18"/>
-      <c r="F11" s="108"/>
+      <c r="F11" s="109"/>
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
       <c r="I11" s="23"/>
@@ -7567,7 +7608,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15.6">
+    <row r="12" spans="1:12" ht="15.75">
       <c r="A12" s="78"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19" t="s">
@@ -7577,7 +7618,7 @@
         <v>286</v>
       </c>
       <c r="E12" s="18"/>
-      <c r="F12" s="108"/>
+      <c r="F12" s="109"/>
       <c r="G12" s="23"/>
       <c r="H12" s="23"/>
       <c r="I12" s="23"/>
@@ -7585,7 +7626,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15.6">
+    <row r="13" spans="1:12" ht="15.75">
       <c r="A13" s="78"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19" t="s">
@@ -7595,7 +7636,7 @@
         <v>288</v>
       </c>
       <c r="E13" s="18"/>
-      <c r="F13" s="108"/>
+      <c r="F13" s="109"/>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
       <c r="I13" s="23"/>
@@ -7603,7 +7644,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15.6">
+    <row r="14" spans="1:12" ht="15.75">
       <c r="A14" s="78"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
@@ -7617,7 +7658,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="15.6">
+    <row r="15" spans="1:12" ht="15.75">
       <c r="A15" s="76">
         <v>2</v>
       </c>
@@ -7629,7 +7670,7 @@
       <c r="E15" s="74" t="s">
         <v>290</v>
       </c>
-      <c r="F15" s="108">
+      <c r="F15" s="109">
         <v>35</v>
       </c>
       <c r="G15" s="23"/>
@@ -7639,7 +7680,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15.6">
+    <row r="16" spans="1:12" ht="15.75">
       <c r="A16" s="78"/>
       <c r="B16" s="18">
         <v>2.1</v>
@@ -7651,7 +7692,7 @@
       <c r="E16" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F16" s="108"/>
+      <c r="F16" s="109"/>
       <c r="G16" s="23"/>
       <c r="H16" s="23"/>
       <c r="I16" s="23"/>
@@ -7659,7 +7700,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" ht="15.6">
+    <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="78"/>
       <c r="B17" s="18">
         <v>2.2000000000000002</v>
@@ -7671,7 +7712,7 @@
       <c r="E17" s="74" t="s">
         <v>293</v>
       </c>
-      <c r="F17" s="108"/>
+      <c r="F17" s="109"/>
       <c r="G17" s="23"/>
       <c r="H17" s="23"/>
       <c r="I17" s="23"/>
@@ -7679,7 +7720,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" ht="15.6">
+    <row r="18" spans="1:12" ht="15.75">
       <c r="A18" s="78"/>
       <c r="B18" s="18">
         <v>2.2999999999999998</v>
@@ -7691,7 +7732,7 @@
       <c r="E18" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F18" s="108"/>
+      <c r="F18" s="109"/>
       <c r="G18" s="23"/>
       <c r="H18" s="23"/>
       <c r="I18" s="23"/>
@@ -7699,7 +7740,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" ht="15.6">
+    <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="78"/>
       <c r="B19" s="18">
         <v>2.4</v>
@@ -7711,7 +7752,7 @@
       <c r="E19" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F19" s="108"/>
+      <c r="F19" s="109"/>
       <c r="G19" s="23"/>
       <c r="H19" s="23"/>
       <c r="I19" s="23"/>
@@ -7719,7 +7760,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" ht="15.6">
+    <row r="20" spans="1:12" ht="15.75">
       <c r="A20" s="78"/>
       <c r="B20" s="18">
         <v>2.5</v>
@@ -7731,7 +7772,7 @@
       <c r="E20" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F20" s="108"/>
+      <c r="F20" s="109"/>
       <c r="G20" s="23"/>
       <c r="H20" s="23"/>
       <c r="I20" s="23"/>
@@ -7739,7 +7780,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" ht="15.6">
+    <row r="21" spans="1:12" ht="15.75">
       <c r="A21" s="78"/>
       <c r="B21" s="18"/>
       <c r="C21" s="19" t="s">
@@ -7749,7 +7790,7 @@
         <v>298</v>
       </c>
       <c r="E21" s="18"/>
-      <c r="F21" s="108"/>
+      <c r="F21" s="109"/>
       <c r="G21" s="23"/>
       <c r="H21" s="23"/>
       <c r="I21" s="23"/>
@@ -7757,7 +7798,7 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:12" ht="15.6">
+    <row r="22" spans="1:12" ht="15.75">
       <c r="A22" s="78"/>
       <c r="B22" s="18"/>
       <c r="C22" s="19" t="s">
@@ -7767,7 +7808,7 @@
         <v>300</v>
       </c>
       <c r="E22" s="18"/>
-      <c r="F22" s="108"/>
+      <c r="F22" s="109"/>
       <c r="G22" s="23"/>
       <c r="H22" s="23"/>
       <c r="I22" s="23"/>
@@ -7775,7 +7816,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12" ht="15.6">
+    <row r="23" spans="1:12" ht="15.75">
       <c r="A23" s="78"/>
       <c r="B23" s="18"/>
       <c r="C23" s="19" t="s">
@@ -7785,7 +7826,7 @@
         <v>302</v>
       </c>
       <c r="E23" s="18"/>
-      <c r="F23" s="108"/>
+      <c r="F23" s="109"/>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>
       <c r="I23" s="23"/>
@@ -7793,7 +7834,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" ht="15.6">
+    <row r="24" spans="1:12" ht="15.75">
       <c r="A24" s="78"/>
       <c r="B24" s="18">
         <v>2.6</v>
@@ -7805,7 +7846,7 @@
       <c r="E24" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F24" s="108"/>
+      <c r="F24" s="109"/>
       <c r="G24" s="23"/>
       <c r="H24" s="23"/>
       <c r="I24" s="23"/>
@@ -7813,7 +7854,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" ht="15.6">
+    <row r="25" spans="1:12" ht="15.75">
       <c r="A25" s="78"/>
       <c r="B25" s="18">
         <v>2.7</v>
@@ -7825,7 +7866,7 @@
       <c r="E25" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="F25" s="108"/>
+      <c r="F25" s="109"/>
       <c r="G25" s="23"/>
       <c r="H25" s="23"/>
       <c r="I25" s="23"/>
@@ -7833,7 +7874,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:12" ht="15.6">
+    <row r="26" spans="1:12" ht="15.75">
       <c r="A26" s="78"/>
       <c r="B26" s="18">
         <v>2.8</v>
@@ -7843,7 +7884,7 @@
         <v>305</v>
       </c>
       <c r="E26" s="18"/>
-      <c r="F26" s="108"/>
+      <c r="F26" s="109"/>
       <c r="G26" s="23"/>
       <c r="H26" s="23"/>
       <c r="I26" s="23"/>
@@ -7851,7 +7892,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:12" ht="15.6">
+    <row r="27" spans="1:12" ht="15.75">
       <c r="A27" s="78"/>
       <c r="B27" s="18">
         <v>2.9</v>
@@ -7861,7 +7902,7 @@
         <v>306</v>
       </c>
       <c r="E27" s="18"/>
-      <c r="F27" s="108"/>
+      <c r="F27" s="109"/>
       <c r="G27" s="23"/>
       <c r="H27" s="23"/>
       <c r="I27" s="23"/>
@@ -7869,7 +7910,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="1:12" ht="15.6">
+    <row r="28" spans="1:12" ht="15.75">
       <c r="A28" s="78"/>
       <c r="B28" s="18">
         <v>2.1</v>
@@ -7881,7 +7922,7 @@
       <c r="E28" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="F28" s="108"/>
+      <c r="F28" s="109"/>
       <c r="G28" s="23"/>
       <c r="H28" s="23"/>
       <c r="I28" s="23"/>
@@ -7889,7 +7930,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" ht="15.6">
+    <row r="29" spans="1:12" ht="15.75">
       <c r="A29" s="78"/>
       <c r="B29" s="18"/>
       <c r="C29" s="19"/>
@@ -7905,7 +7946,7 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="1:12" ht="15.6">
+    <row r="30" spans="1:12" ht="15.75">
       <c r="A30" s="78"/>
       <c r="B30" s="18"/>
       <c r="C30" s="17"/>
@@ -7919,7 +7960,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12" ht="31.2">
+    <row r="31" spans="1:12" ht="31.5">
       <c r="A31" s="82"/>
       <c r="B31" s="79"/>
       <c r="C31" s="84" t="s">
@@ -7939,7 +7980,7 @@
       <c r="K31" s="56"/>
       <c r="L31" s="56"/>
     </row>
-    <row r="32" spans="1:12" ht="15.6">
+    <row r="32" spans="1:12" ht="15.75">
       <c r="A32" s="76"/>
       <c r="B32" s="16"/>
       <c r="C32" s="15"/>
@@ -7947,7 +7988,7 @@
       <c r="E32" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="F32" s="108"/>
+      <c r="F32" s="109"/>
       <c r="G32" s="23"/>
       <c r="H32" s="23"/>
       <c r="I32" s="23"/>
@@ -7955,13 +7996,13 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="1:12" ht="15.6">
+    <row r="33" spans="1:12" ht="15.75">
       <c r="A33" s="78"/>
       <c r="B33" s="18"/>
       <c r="C33" s="19"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
-      <c r="F33" s="108"/>
+      <c r="F33" s="109"/>
       <c r="G33" s="23"/>
       <c r="H33" s="23"/>
       <c r="I33" s="23"/>
@@ -7969,7 +8010,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="1:12" ht="15.6">
+    <row r="34" spans="1:12" ht="15.75">
       <c r="A34" s="78"/>
       <c r="B34" s="18"/>
       <c r="C34" s="19"/>
@@ -7977,7 +8018,7 @@
         <v>311</v>
       </c>
       <c r="E34" s="18"/>
-      <c r="F34" s="108"/>
+      <c r="F34" s="109"/>
       <c r="G34" s="23"/>
       <c r="H34" s="23"/>
       <c r="I34" s="23"/>
@@ -7985,7 +8026,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="1:12" ht="15.6">
+    <row r="35" spans="1:12" ht="15.75">
       <c r="A35" s="76">
         <v>3</v>
       </c>
@@ -7995,7 +8036,7 @@
         <v>312</v>
       </c>
       <c r="E35" s="16"/>
-      <c r="F35" s="108">
+      <c r="F35" s="109">
         <v>10</v>
       </c>
       <c r="G35" s="23"/>
@@ -8005,7 +8046,7 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="1:12" ht="15.6">
+    <row r="36" spans="1:12" ht="15.75">
       <c r="A36" s="78"/>
       <c r="B36" s="18">
         <v>3.1</v>
@@ -8017,7 +8058,7 @@
       <c r="E36" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F36" s="108"/>
+      <c r="F36" s="109"/>
       <c r="G36" s="23"/>
       <c r="H36" s="23"/>
       <c r="I36" s="23"/>
@@ -8025,7 +8066,7 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="1:12" ht="15.6">
+    <row r="37" spans="1:12" ht="15.75">
       <c r="A37" s="78"/>
       <c r="B37" s="18">
         <v>3.2</v>
@@ -8037,7 +8078,7 @@
       <c r="E37" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F37" s="108"/>
+      <c r="F37" s="109"/>
       <c r="G37" s="23"/>
       <c r="H37" s="23"/>
       <c r="I37" s="23"/>
@@ -8045,7 +8086,7 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="1:12" ht="15.6">
+    <row r="38" spans="1:12" ht="15.75">
       <c r="A38" s="78"/>
       <c r="B38" s="18">
         <v>3.3</v>
@@ -8057,7 +8098,7 @@
       <c r="E38" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F38" s="108"/>
+      <c r="F38" s="109"/>
       <c r="G38" s="23"/>
       <c r="H38" s="23"/>
       <c r="I38" s="23"/>
@@ -8065,7 +8106,7 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="1:12" ht="15.6">
+    <row r="39" spans="1:12" ht="15.75">
       <c r="A39" s="78"/>
       <c r="B39" s="18">
         <v>3.4</v>
@@ -8077,7 +8118,7 @@
       <c r="E39" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F39" s="108"/>
+      <c r="F39" s="109"/>
       <c r="G39" s="23"/>
       <c r="H39" s="23"/>
       <c r="I39" s="23"/>
@@ -8085,7 +8126,7 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="1:12" ht="15.6">
+    <row r="40" spans="1:12" ht="15.75">
       <c r="A40" s="78"/>
       <c r="B40" s="18">
         <v>3.5</v>
@@ -8097,7 +8138,7 @@
       <c r="E40" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="F40" s="108"/>
+      <c r="F40" s="109"/>
       <c r="G40" s="23"/>
       <c r="H40" s="23"/>
       <c r="I40" s="23"/>
@@ -8105,7 +8146,7 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="1:12" ht="15.6">
+    <row r="41" spans="1:12" ht="15.75">
       <c r="A41" s="78"/>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
@@ -8119,7 +8160,7 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="1:12" ht="15.6">
+    <row r="42" spans="1:12" ht="15.75">
       <c r="A42" s="78"/>
       <c r="B42" s="18"/>
       <c r="C42" s="19"/>
@@ -8133,7 +8174,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="1:12" ht="15.6">
+    <row r="43" spans="1:12" ht="15.75">
       <c r="A43" s="76">
         <v>4</v>
       </c>
@@ -8153,7 +8194,7 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="1:12" ht="15.6">
+    <row r="44" spans="1:12" ht="15.75">
       <c r="A44" s="78"/>
       <c r="B44" s="18">
         <v>4.0999999999999996</v>
@@ -8173,7 +8214,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="1:12" ht="15.6">
+    <row r="45" spans="1:12" ht="15.75">
       <c r="A45" s="78"/>
       <c r="B45" s="18"/>
       <c r="C45" s="19" t="s">
@@ -8191,7 +8232,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="1:12" ht="15.6">
+    <row r="46" spans="1:12" ht="15.75">
       <c r="A46" s="78"/>
       <c r="B46" s="18"/>
       <c r="C46" s="19" t="s">
@@ -8209,7 +8250,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="1:12" ht="15.6">
+    <row r="47" spans="1:12" ht="15.75">
       <c r="A47" s="78"/>
       <c r="B47" s="18">
         <v>4.2</v>
@@ -8229,7 +8270,7 @@
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="1:12" ht="15.6">
+    <row r="48" spans="1:12" ht="15.75">
       <c r="A48" s="78"/>
       <c r="B48" s="18"/>
       <c r="C48" s="19" t="s">
@@ -8247,7 +8288,7 @@
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:12" ht="15.6">
+    <row r="49" spans="1:12" ht="15.75">
       <c r="A49" s="78"/>
       <c r="B49" s="18"/>
       <c r="C49" s="19" t="s">
@@ -8265,7 +8306,7 @@
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:12" ht="15.6">
+    <row r="50" spans="1:12" ht="15.75">
       <c r="A50" s="78"/>
       <c r="B50" s="18"/>
       <c r="C50" s="19" t="s">
@@ -8283,7 +8324,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="1:12" ht="15.6">
+    <row r="51" spans="1:12" ht="15.75">
       <c r="A51" s="78"/>
       <c r="B51" s="18">
         <v>4.3</v>
@@ -8303,7 +8344,7 @@
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="1:12" ht="15.6">
+    <row r="52" spans="1:12" ht="15.75">
       <c r="A52" s="78"/>
       <c r="B52" s="18"/>
       <c r="C52" s="19" t="s">
@@ -8321,7 +8362,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="1:12" ht="15.6">
+    <row r="53" spans="1:12" ht="15.75">
       <c r="A53" s="78"/>
       <c r="B53" s="18"/>
       <c r="C53" s="19" t="s">
@@ -8339,7 +8380,7 @@
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="1:12" ht="15.6">
+    <row r="54" spans="1:12" ht="15.75">
       <c r="A54" s="78"/>
       <c r="B54" s="18"/>
       <c r="C54" s="19" t="s">
@@ -8357,7 +8398,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="1:12" ht="15.6">
+    <row r="55" spans="1:12" ht="15.75">
       <c r="A55" s="78"/>
       <c r="B55" s="18"/>
       <c r="C55" s="19" t="s">
@@ -8375,7 +8416,7 @@
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="1:12" ht="15.6">
+    <row r="56" spans="1:12" ht="15.75">
       <c r="A56" s="78"/>
       <c r="B56" s="18"/>
       <c r="C56" s="19" t="s">
@@ -8393,7 +8434,7 @@
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
     </row>
-    <row r="57" spans="1:12" ht="15.6">
+    <row r="57" spans="1:12" ht="15.75">
       <c r="A57" s="78"/>
       <c r="B57" s="18"/>
       <c r="C57" s="19" t="s">
@@ -8411,7 +8452,7 @@
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="1:12" ht="15.6">
+    <row r="58" spans="1:12" ht="15.75">
       <c r="A58" s="78"/>
       <c r="B58" s="18"/>
       <c r="C58" s="19" t="s">
@@ -8429,7 +8470,7 @@
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="1:12" ht="15.6">
+    <row r="59" spans="1:12" ht="15.75">
       <c r="A59" s="78"/>
       <c r="B59" s="18">
         <v>4.4000000000000004</v>
@@ -8449,7 +8490,7 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="1:12" ht="15.6">
+    <row r="60" spans="1:12" ht="15.75">
       <c r="A60" s="78"/>
       <c r="B60" s="18"/>
       <c r="C60" s="19" t="s">
@@ -8467,7 +8508,7 @@
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="1:12" ht="15.6">
+    <row r="61" spans="1:12" ht="15.75">
       <c r="A61" s="78"/>
       <c r="B61" s="18">
         <v>4.5</v>
@@ -8487,7 +8528,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="1:12" ht="15.6">
+    <row r="62" spans="1:12" ht="15.75">
       <c r="A62" s="78"/>
       <c r="B62" s="18"/>
       <c r="C62" s="19" t="s">
@@ -8505,7 +8546,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="1:12" ht="15.6">
+    <row r="63" spans="1:12" ht="15.75">
       <c r="A63" s="78"/>
       <c r="B63" s="18"/>
       <c r="C63" s="19" t="s">
@@ -8523,7 +8564,7 @@
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="1:12" ht="15.6">
+    <row r="64" spans="1:12" ht="15.75">
       <c r="A64" s="78"/>
       <c r="B64" s="18">
         <v>4.5999999999999996</v>
@@ -8543,7 +8584,7 @@
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="1:12" ht="15.6">
+    <row r="65" spans="1:12" ht="15.75">
       <c r="A65" s="78"/>
       <c r="B65" s="18"/>
       <c r="C65" s="19" t="s">
@@ -8561,7 +8602,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" ht="15.6">
+    <row r="66" spans="1:12" ht="15.75">
       <c r="A66" s="78"/>
       <c r="B66" s="18">
         <v>4.7</v>
@@ -8581,7 +8622,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:12" ht="15.6">
+    <row r="67" spans="1:12" ht="15.75">
       <c r="A67" s="78"/>
       <c r="B67" s="18"/>
       <c r="C67" s="19" t="s">
@@ -8599,7 +8640,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" ht="15.6">
+    <row r="68" spans="1:12" ht="15.75">
       <c r="A68" s="78"/>
       <c r="B68" s="18"/>
       <c r="C68" s="19" t="s">
@@ -8617,7 +8658,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" ht="15.6">
+    <row r="69" spans="1:12" ht="15.75">
       <c r="A69" s="78"/>
       <c r="B69" s="18">
         <v>4.8</v>
@@ -8637,7 +8678,7 @@
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:12" ht="15.6">
+    <row r="70" spans="1:12" ht="15.75">
       <c r="A70" s="78"/>
       <c r="B70" s="18"/>
       <c r="C70" s="19" t="s">
@@ -8655,7 +8696,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" ht="15.6">
+    <row r="71" spans="1:12" ht="15.75">
       <c r="A71" s="78"/>
       <c r="B71" s="18"/>
       <c r="C71" s="19" t="s">
@@ -8673,7 +8714,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" ht="15.6">
+    <row r="72" spans="1:12" ht="15.75">
       <c r="A72" s="78"/>
       <c r="B72" s="18"/>
       <c r="C72" s="19" t="s">
@@ -8691,7 +8732,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" ht="15.6">
+    <row r="73" spans="1:12" ht="15.75">
       <c r="A73" s="78"/>
       <c r="B73" s="18"/>
       <c r="C73" s="19" t="s">
@@ -8709,7 +8750,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" ht="15.6">
+    <row r="74" spans="1:12" ht="15.75">
       <c r="A74" s="78"/>
       <c r="B74" s="18"/>
       <c r="C74" s="19" t="s">
@@ -8727,7 +8768,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" ht="15.6">
+    <row r="75" spans="1:12" ht="15.75">
       <c r="A75" s="78"/>
       <c r="B75" s="18">
         <v>4.9000000000000004</v>
@@ -8747,7 +8788,7 @@
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" ht="15.6">
+    <row r="76" spans="1:12" ht="15.75">
       <c r="A76" s="78"/>
       <c r="B76" s="18">
         <v>4.0999999999999996</v>
@@ -8767,7 +8808,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" ht="15.6">
+    <row r="77" spans="1:12" ht="15.75">
       <c r="A77" s="78"/>
       <c r="B77" s="18"/>
       <c r="C77" s="19" t="s">
@@ -8785,7 +8826,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" ht="15.6">
+    <row r="78" spans="1:12" ht="15.75">
       <c r="A78" s="78"/>
       <c r="B78" s="18">
         <v>4.1100000000000003</v>
@@ -8805,7 +8846,7 @@
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
     </row>
-    <row r="79" spans="1:12" ht="15.6">
+    <row r="79" spans="1:12" ht="15.75">
       <c r="A79" s="78"/>
       <c r="B79" s="18"/>
       <c r="C79" s="19" t="s">
@@ -8823,7 +8864,7 @@
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="1:12" ht="15.6">
+    <row r="80" spans="1:12" ht="15.75">
       <c r="A80" s="78"/>
       <c r="B80" s="18"/>
       <c r="C80" s="19" t="s">
@@ -8841,7 +8882,7 @@
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
     </row>
-    <row r="81" spans="1:12" ht="15.6">
+    <row r="81" spans="1:12" ht="15.75">
       <c r="A81" s="78"/>
       <c r="B81" s="18"/>
       <c r="C81" s="19" t="s">
@@ -8859,7 +8900,7 @@
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" ht="15.6">
+    <row r="82" spans="1:12" ht="15.75">
       <c r="A82" s="78"/>
       <c r="B82" s="18"/>
       <c r="C82" s="19" t="s">
@@ -8877,7 +8918,7 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" ht="15.6">
+    <row r="83" spans="1:12" ht="15.75">
       <c r="A83" s="78"/>
       <c r="B83" s="18">
         <v>4.12</v>
@@ -8897,7 +8938,7 @@
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" ht="15.6">
+    <row r="84" spans="1:12" ht="15.75">
       <c r="A84" s="78"/>
       <c r="B84" s="18"/>
       <c r="C84" s="19" t="s">
@@ -8915,7 +8956,7 @@
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" ht="15.6">
+    <row r="85" spans="1:12" ht="15.75">
       <c r="A85" s="78"/>
       <c r="B85" s="18"/>
       <c r="C85" s="19" t="s">
@@ -8933,7 +8974,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" ht="15.6">
+    <row r="86" spans="1:12" ht="15.75">
       <c r="A86" s="78"/>
       <c r="B86" s="18"/>
       <c r="C86" s="19" t="s">
@@ -8951,7 +8992,7 @@
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="1:12" ht="15.6">
+    <row r="87" spans="1:12" ht="15.75">
       <c r="A87" s="78"/>
       <c r="B87" s="18">
         <v>4.13</v>
@@ -8971,7 +9012,7 @@
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="1:12" ht="15.6">
+    <row r="88" spans="1:12" ht="15.75">
       <c r="A88" s="78"/>
       <c r="B88" s="18"/>
       <c r="C88" s="19" t="s">
@@ -8989,7 +9030,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="1:12" ht="15.6">
+    <row r="89" spans="1:12" ht="15.75">
       <c r="A89" s="78"/>
       <c r="B89" s="18">
         <v>4.1399999999999997</v>
@@ -9009,7 +9050,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="1:12" ht="15.6">
+    <row r="90" spans="1:12" ht="15.75">
       <c r="A90" s="78"/>
       <c r="B90" s="18">
         <v>4.1500000000000004</v>
@@ -9029,7 +9070,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="1:12" ht="15.6">
+    <row r="91" spans="1:12" ht="15.75">
       <c r="A91" s="78"/>
       <c r="B91" s="18"/>
       <c r="C91" s="19" t="s">
@@ -9047,7 +9088,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:12" ht="15.6">
+    <row r="92" spans="1:12" ht="15.75">
       <c r="A92" s="78"/>
       <c r="B92" s="18"/>
       <c r="C92" s="19" t="s">
@@ -9065,7 +9106,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="1:12" ht="15.6">
+    <row r="93" spans="1:12" ht="15.75">
       <c r="A93" s="78"/>
       <c r="B93" s="18"/>
       <c r="C93" s="19"/>
@@ -9083,7 +9124,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
     </row>
-    <row r="94" spans="1:12" ht="15.6">
+    <row r="94" spans="1:12" ht="15.75">
       <c r="A94" s="78"/>
       <c r="B94" s="17"/>
       <c r="C94" s="17"/>
@@ -9097,7 +9138,7 @@
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
     </row>
-    <row r="95" spans="1:12" ht="15.6">
+    <row r="95" spans="1:12" ht="15.75">
       <c r="A95" s="82"/>
       <c r="B95" s="79"/>
       <c r="C95" s="81" t="s">
@@ -9117,7 +9158,7 @@
       <c r="K95" s="56"/>
       <c r="L95" s="56"/>
     </row>
-    <row r="96" spans="1:12" ht="15.6">
+    <row r="96" spans="1:12" ht="15.75">
       <c r="A96" s="82"/>
       <c r="B96" s="79"/>
       <c r="C96" s="81"/>
@@ -9145,7 +9186,7 @@
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
     </row>
-    <row r="98" spans="1:12" ht="15.6">
+    <row r="98" spans="1:12" ht="15.75">
       <c r="A98" s="76">
         <v>5</v>
       </c>
@@ -9155,7 +9196,7 @@
         <v>368</v>
       </c>
       <c r="E98" s="16"/>
-      <c r="F98" s="109">
+      <c r="F98" s="110">
         <v>5</v>
       </c>
       <c r="G98" s="83"/>
@@ -9165,7 +9206,7 @@
       <c r="K98" s="3"/>
       <c r="L98" s="3"/>
     </row>
-    <row r="99" spans="1:12" ht="15.6">
+    <row r="99" spans="1:12" ht="15.75">
       <c r="A99" s="78"/>
       <c r="B99" s="18">
         <v>5.0999999999999996</v>
@@ -9177,7 +9218,7 @@
       <c r="E99" s="74" t="s">
         <v>290</v>
       </c>
-      <c r="F99" s="109"/>
+      <c r="F99" s="110"/>
       <c r="G99" s="83"/>
       <c r="H99" s="83"/>
       <c r="I99" s="83"/>
@@ -9185,7 +9226,7 @@
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
     </row>
-    <row r="100" spans="1:12" ht="15.6">
+    <row r="100" spans="1:12" ht="15.75">
       <c r="A100" s="78"/>
       <c r="B100" s="18">
         <v>5.2</v>
@@ -9197,7 +9238,7 @@
       <c r="E100" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F100" s="109"/>
+      <c r="F100" s="110"/>
       <c r="G100" s="83"/>
       <c r="H100" s="83"/>
       <c r="I100" s="83"/>
@@ -9205,7 +9246,7 @@
       <c r="K100" s="3"/>
       <c r="L100" s="3"/>
     </row>
-    <row r="101" spans="1:12" ht="15.6">
+    <row r="101" spans="1:12" ht="15.75">
       <c r="A101" s="78"/>
       <c r="B101" s="18">
         <v>5.3</v>
@@ -9217,7 +9258,7 @@
       <c r="E101" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F101" s="109"/>
+      <c r="F101" s="110"/>
       <c r="G101" s="83"/>
       <c r="H101" s="83"/>
       <c r="I101" s="83"/>
@@ -9225,7 +9266,7 @@
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
     </row>
-    <row r="102" spans="1:12" ht="15.6">
+    <row r="102" spans="1:12" ht="15.75">
       <c r="A102" s="78"/>
       <c r="B102" s="18"/>
       <c r="C102" s="19"/>
@@ -9239,7 +9280,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
     </row>
-    <row r="103" spans="1:12" ht="15.6">
+    <row r="103" spans="1:12" ht="15.75">
       <c r="A103" s="76">
         <v>6</v>
       </c>
@@ -9251,7 +9292,7 @@
       <c r="E103" s="74" t="s">
         <v>290</v>
       </c>
-      <c r="F103" s="109">
+      <c r="F103" s="110">
         <v>6</v>
       </c>
       <c r="G103" s="83"/>
@@ -9261,7 +9302,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
     </row>
-    <row r="104" spans="1:12" ht="15.6">
+    <row r="104" spans="1:12" ht="15.75">
       <c r="A104" s="78"/>
       <c r="B104" s="18">
         <v>6.1</v>
@@ -9271,7 +9312,7 @@
         <v>298</v>
       </c>
       <c r="E104" s="18"/>
-      <c r="F104" s="109"/>
+      <c r="F104" s="110"/>
       <c r="G104" s="83"/>
       <c r="H104" s="83"/>
       <c r="I104" s="83"/>
@@ -9279,7 +9320,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
     </row>
-    <row r="105" spans="1:12" ht="15.6">
+    <row r="105" spans="1:12" ht="15.75">
       <c r="A105" s="78"/>
       <c r="B105" s="18">
         <v>6.2</v>
@@ -9289,7 +9330,7 @@
         <v>372</v>
       </c>
       <c r="E105" s="18"/>
-      <c r="F105" s="109"/>
+      <c r="F105" s="110"/>
       <c r="G105" s="83"/>
       <c r="H105" s="83"/>
       <c r="I105" s="83"/>
@@ -9297,7 +9338,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
     </row>
-    <row r="106" spans="1:12" ht="15.6">
+    <row r="106" spans="1:12" ht="15.75">
       <c r="A106" s="78"/>
       <c r="B106" s="18">
         <v>6.3</v>
@@ -9307,7 +9348,7 @@
         <v>373</v>
       </c>
       <c r="E106" s="18"/>
-      <c r="F106" s="109"/>
+      <c r="F106" s="110"/>
       <c r="G106" s="83"/>
       <c r="H106" s="83"/>
       <c r="I106" s="83"/>
@@ -9315,7 +9356,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
     </row>
-    <row r="107" spans="1:12" ht="15.6">
+    <row r="107" spans="1:12" ht="15.75">
       <c r="A107" s="78"/>
       <c r="B107" s="18">
         <v>6.4</v>
@@ -9325,7 +9366,7 @@
         <v>374</v>
       </c>
       <c r="E107" s="18"/>
-      <c r="F107" s="109"/>
+      <c r="F107" s="110"/>
       <c r="G107" s="83"/>
       <c r="H107" s="83"/>
       <c r="I107" s="83"/>
@@ -9333,7 +9374,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="1:12" ht="15.6">
+    <row r="108" spans="1:12" ht="15.75">
       <c r="A108" s="78"/>
       <c r="B108" s="18">
         <v>6.5</v>
@@ -9343,7 +9384,7 @@
         <v>375</v>
       </c>
       <c r="E108" s="18"/>
-      <c r="F108" s="109"/>
+      <c r="F108" s="110"/>
       <c r="G108" s="83"/>
       <c r="H108" s="83"/>
       <c r="I108" s="83"/>
@@ -9351,7 +9392,7 @@
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
     </row>
-    <row r="109" spans="1:12" ht="15.6">
+    <row r="109" spans="1:12" ht="15.75">
       <c r="A109" s="78"/>
       <c r="B109" s="18">
         <v>6.6</v>
@@ -9361,7 +9402,7 @@
         <v>376</v>
       </c>
       <c r="E109" s="18"/>
-      <c r="F109" s="109"/>
+      <c r="F109" s="110"/>
       <c r="G109" s="83"/>
       <c r="H109" s="83"/>
       <c r="I109" s="83"/>
@@ -9369,7 +9410,7 @@
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
     </row>
-    <row r="110" spans="1:12" ht="15.6">
+    <row r="110" spans="1:12" ht="15.75">
       <c r="A110" s="78"/>
       <c r="B110" s="18"/>
       <c r="C110" s="19"/>
@@ -9383,7 +9424,7 @@
       <c r="K110" s="3"/>
       <c r="L110" s="3"/>
     </row>
-    <row r="111" spans="1:12" ht="93.6">
+    <row r="111" spans="1:12" ht="94.5">
       <c r="A111" s="82"/>
       <c r="B111" s="79"/>
       <c r="C111" s="81" t="s">
@@ -9404,12 +9445,12 @@
       <c r="L111" s="56"/>
     </row>
     <row r="112" spans="1:12">
-      <c r="A112" s="97" t="s">
+      <c r="A112" s="98" t="s">
         <v>155</v>
       </c>
-      <c r="B112" s="98"/>
-      <c r="C112" s="98"/>
-      <c r="D112" s="99"/>
+      <c r="B112" s="99"/>
+      <c r="C112" s="99"/>
+      <c r="D112" s="100"/>
       <c r="E112" s="53"/>
       <c r="F112" s="53">
         <f>SUM(F4:F111)</f>
@@ -9423,12 +9464,12 @@
       <c r="L112" s="32"/>
     </row>
     <row r="113" spans="1:12">
-      <c r="A113" s="97" t="s">
+      <c r="A113" s="98" t="s">
         <v>156</v>
       </c>
-      <c r="B113" s="98"/>
-      <c r="C113" s="98"/>
-      <c r="D113" s="99"/>
+      <c r="B113" s="99"/>
+      <c r="C113" s="99"/>
+      <c r="D113" s="100"/>
       <c r="E113" s="32"/>
       <c r="F113" s="53">
         <v>145</v>
@@ -9440,7 +9481,7 @@
       <c r="K113" s="32"/>
       <c r="L113" s="32"/>
     </row>
-    <row r="114" spans="1:12" ht="15.6">
+    <row r="114" spans="1:12" ht="15.75">
       <c r="D114" s="22" t="s">
         <v>378</v>
       </c>

</xml_diff>

<commit_message>
Exception handling using developer exception page
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RKIT\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2DBBA5-9CED-4EAA-8070-9A1F2CAE67CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C0D50B-3A8E-4CE2-A2C3-B51FF925FF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
   <sheets>
     <sheet name=" Basic GUI" sheetId="1" r:id="rId1"/>
@@ -6164,7 +6164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51642604-D68B-4E5E-9160-A3EE5943E7C7}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -6723,8 +6723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE125957-E0FE-4793-875C-A900941606E5}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
DateBox and AdvAPI final demo modifications
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779695A2-B6B3-497D-B225-ACECE72B0037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A2FDC5-A1D8-4103-860A-7FC427514C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
@@ -7392,7 +7392,7 @@
   <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7678,7 +7678,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="31.5">
+    <row r="15" spans="1:12" ht="15.75">
       <c r="A15" s="76">
         <v>2</v>
       </c>
@@ -7694,10 +7694,10 @@
         <v>35</v>
       </c>
       <c r="G15" s="23">
-        <v>4</v>
+        <v>12.5</v>
       </c>
       <c r="H15" s="98">
-        <v>45695</v>
+        <v>45698</v>
       </c>
       <c r="I15" s="23" t="s">
         <v>483</v>

</xml_diff>

<commit_message>
NumberBox and modifications into core demos
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E406388-FDA5-4647-AB05-2D7504AB5B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6BC202-A020-4046-ADFB-F8E34D34C840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
   <sheets>
     <sheet name=" Basic GUI" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="483">
   <si>
     <t>Topic</t>
   </si>
@@ -6731,7 +6731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE125957-E0FE-4793-875C-A900941606E5}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -7388,8 +7388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3782443B-979F-4126-A9F9-516CD045F0D0}">
   <dimension ref="A1:L114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7809,8 +7809,12 @@
       </c>
       <c r="F20" s="110"/>
       <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
+      <c r="H20" s="98">
+        <v>45700</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>433</v>
+      </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>

</xml_diff>

<commit_message>
Editors - textBox, button
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2705D168-5E08-4FDC-8310-09D16D643CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52238AD6-CA39-43CD-9F9F-4B32CB753246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="14130" firstSheet="1" activeTab="4" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
+    <workbookView xWindow="0" yWindow="1470" windowWidth="21600" windowHeight="14130" firstSheet="1" activeTab="4" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
   <sheets>
     <sheet name=" Basic GUI" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="483">
   <si>
     <t>Topic</t>
   </si>
@@ -1487,9 +1487,6 @@
   </si>
   <si>
     <t>https://docs.servicestack.net/ormlite/apis/select</t>
-  </si>
-  <si>
-    <t>Ongoing</t>
   </si>
 </sst>
 </file>
@@ -7391,8 +7388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3782443B-979F-4126-A9F9-516CD045F0D0}">
   <dimension ref="A1:L114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7923,10 +7920,10 @@
       <c r="F25" s="110"/>
       <c r="G25" s="23"/>
       <c r="H25" s="98">
-        <v>45701</v>
+        <v>45702</v>
       </c>
       <c r="I25" s="23" t="s">
-        <v>483</v>
+        <v>433</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -7944,8 +7941,12 @@
       <c r="E26" s="18"/>
       <c r="F26" s="110"/>
       <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
+      <c r="H26" s="98">
+        <v>45702</v>
+      </c>
+      <c r="I26" s="23" t="s">
+        <v>433</v>
+      </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>

</xml_diff>

<commit_message>
.net core final demo modifications
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B328EED-893D-4D79-866C-5D617FAF9A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546D6800-D41A-495A-BC2C-26F8D4651077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="486">
   <si>
     <t>Topic</t>
   </si>
@@ -1493,6 +1493,9 @@
   </si>
   <si>
     <t>error</t>
+  </si>
+  <si>
+    <t>Ongoing</t>
   </si>
 </sst>
 </file>
@@ -7403,8 +7406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3782443B-979F-4126-A9F9-516CD045F0D0}">
   <dimension ref="A1:L114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8705,9 +8708,15 @@
       <c r="F64" s="78">
         <v>2</v>
       </c>
-      <c r="G64" s="78"/>
-      <c r="H64" s="78"/>
-      <c r="I64" s="78"/>
+      <c r="G64" s="78">
+        <v>1.5</v>
+      </c>
+      <c r="H64" s="101">
+        <v>45714</v>
+      </c>
+      <c r="I64" s="78" t="s">
+        <v>433</v>
+      </c>
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
@@ -8743,9 +8752,15 @@
       <c r="F66" s="78">
         <v>2</v>
       </c>
-      <c r="G66" s="78"/>
-      <c r="H66" s="78"/>
-      <c r="I66" s="78"/>
+      <c r="G66" s="78">
+        <v>1.5</v>
+      </c>
+      <c r="H66" s="101">
+        <v>45714</v>
+      </c>
+      <c r="I66" s="78" t="s">
+        <v>433</v>
+      </c>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
@@ -8799,9 +8814,15 @@
       <c r="F69" s="78">
         <v>10</v>
       </c>
-      <c r="G69" s="78"/>
-      <c r="H69" s="78"/>
-      <c r="I69" s="78"/>
+      <c r="G69" s="78">
+        <v>2</v>
+      </c>
+      <c r="H69" s="101">
+        <v>45714</v>
+      </c>
+      <c r="I69" s="78" t="s">
+        <v>485</v>
+      </c>
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>

</xml_diff>

<commit_message>
Editors final demo modifications
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\officeWork\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B328EED-893D-4D79-866C-5D617FAF9A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EF7CDA-C096-46B5-9EC2-C804375D64A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="4" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
   <sheets>
     <sheet name=" Basic GUI" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2475,20 +2484,20 @@
       <selection activeCell="J95" sqref="J95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="72" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="72" customWidth="1"/>
     <col min="2" max="2" width="6" style="29" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" customWidth="1"/>
     <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="5" width="53.42578125" customWidth="1"/>
-    <col min="6" max="9" width="9.28515625" style="29" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="51.42578125" customWidth="1"/>
+    <col min="5" max="5" width="53.44140625" customWidth="1"/>
+    <col min="6" max="9" width="9.33203125" style="29" customWidth="1"/>
+    <col min="10" max="10" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="51.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="40" customFormat="1" ht="18.75">
+    <row r="1" spans="1:12" s="40" customFormat="1" ht="18">
       <c r="A1" s="106" t="s">
         <v>0</v>
       </c>
@@ -2514,7 +2523,7 @@
       <c r="K1" s="41"/>
       <c r="L1" s="41"/>
     </row>
-    <row r="2" spans="1:12" s="29" customFormat="1" ht="18.75">
+    <row r="2" spans="1:12" s="29" customFormat="1" ht="18">
       <c r="A2" s="66">
         <v>1</v>
       </c>
@@ -2538,7 +2547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75">
+    <row r="3" spans="1:12" ht="15.6">
       <c r="A3" s="47"/>
       <c r="B3" s="46">
         <v>1.1000000000000001</v>
@@ -2566,7 +2575,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="31.5">
+    <row r="4" spans="1:12" ht="31.2">
       <c r="A4" s="67"/>
       <c r="B4" s="24"/>
       <c r="C4" s="31" t="s">
@@ -2586,7 +2595,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75">
+    <row r="5" spans="1:12" ht="15.6">
       <c r="A5" s="67"/>
       <c r="B5" s="24"/>
       <c r="C5" s="31" t="s">
@@ -2604,7 +2613,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75">
+    <row r="6" spans="1:12" ht="15.6">
       <c r="A6" s="67"/>
       <c r="B6" s="24"/>
       <c r="C6" s="31" t="s">
@@ -2622,7 +2631,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75">
+    <row r="7" spans="1:12" ht="15.6">
       <c r="A7" s="47"/>
       <c r="B7" s="49">
         <v>1.2</v>
@@ -2650,7 +2659,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75">
+    <row r="8" spans="1:12" ht="15.6">
       <c r="A8" s="67"/>
       <c r="B8" s="24"/>
       <c r="C8" s="31" t="s">
@@ -2668,7 +2677,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75">
+    <row r="9" spans="1:12" ht="15.6">
       <c r="A9" s="67"/>
       <c r="B9" s="24"/>
       <c r="C9" s="31" t="s">
@@ -2686,7 +2695,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75">
+    <row r="10" spans="1:12" ht="15.6">
       <c r="A10" s="67"/>
       <c r="B10" s="24"/>
       <c r="C10" s="31" t="s">
@@ -2704,7 +2713,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75">
+    <row r="11" spans="1:12" ht="15.6">
       <c r="A11" s="67"/>
       <c r="B11" s="24"/>
       <c r="C11" s="31" t="s">
@@ -2722,7 +2731,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75">
+    <row r="12" spans="1:12" ht="15.6">
       <c r="A12" s="67"/>
       <c r="B12" s="24"/>
       <c r="C12" s="31" t="s">
@@ -2740,7 +2749,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75">
+    <row r="13" spans="1:12" ht="15.6">
       <c r="A13" s="67"/>
       <c r="B13" s="24"/>
       <c r="C13" s="31" t="s">
@@ -2758,7 +2767,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75">
+    <row r="14" spans="1:12" ht="15.6">
       <c r="A14" s="67"/>
       <c r="B14" s="24"/>
       <c r="C14" s="31" t="s">
@@ -2776,7 +2785,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75">
+    <row r="15" spans="1:12" ht="15.6">
       <c r="A15" s="67"/>
       <c r="B15" s="24"/>
       <c r="C15" s="31" t="s">
@@ -2794,7 +2803,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75">
+    <row r="16" spans="1:12" ht="15.6">
       <c r="A16" s="67"/>
       <c r="B16" s="24"/>
       <c r="C16" s="31" t="s">
@@ -2812,7 +2821,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75">
+    <row r="17" spans="1:12" ht="15.6">
       <c r="A17" s="47"/>
       <c r="B17" s="49">
         <v>1.3</v>
@@ -2840,7 +2849,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75">
+    <row r="18" spans="1:12" ht="15.6">
       <c r="A18" s="67"/>
       <c r="B18" s="24"/>
       <c r="C18" s="31" t="s">
@@ -2858,7 +2867,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75">
+    <row r="19" spans="1:12" ht="15.6">
       <c r="A19" s="67"/>
       <c r="B19" s="24"/>
       <c r="C19" s="31" t="s">
@@ -2876,7 +2885,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" ht="15.75">
+    <row r="20" spans="1:12" ht="15.6">
       <c r="A20" s="67"/>
       <c r="B20" s="24"/>
       <c r="C20" s="31" t="s">
@@ -2894,7 +2903,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75">
+    <row r="21" spans="1:12" ht="15.6">
       <c r="A21" s="67"/>
       <c r="B21" s="24"/>
       <c r="C21" s="31" t="s">
@@ -2912,7 +2921,7 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75">
+    <row r="22" spans="1:12" ht="15.6">
       <c r="A22" s="47"/>
       <c r="B22" s="49">
         <v>1.4</v>
@@ -2942,7 +2951,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75">
+    <row r="23" spans="1:12" ht="15.6">
       <c r="A23" s="67"/>
       <c r="B23" s="24"/>
       <c r="C23" s="31" t="s">
@@ -2960,7 +2969,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75">
+    <row r="24" spans="1:12" ht="15.6">
       <c r="A24" s="67"/>
       <c r="B24" s="24"/>
       <c r="C24" s="31" t="s">
@@ -2978,7 +2987,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" ht="31.5">
+    <row r="25" spans="1:12" ht="31.2">
       <c r="A25" s="67"/>
       <c r="B25" s="24"/>
       <c r="C25" s="31" t="s">
@@ -2996,7 +3005,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:12" ht="15.75">
+    <row r="26" spans="1:12" ht="15.6">
       <c r="A26" s="67"/>
       <c r="B26" s="24"/>
       <c r="C26" s="31"/>
@@ -3010,7 +3019,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:12" ht="15.75">
+    <row r="27" spans="1:12" ht="15.6">
       <c r="A27" s="85"/>
       <c r="B27" s="86">
         <v>1.5</v>
@@ -3040,7 +3049,7 @@
       <c r="K27" s="56"/>
       <c r="L27" s="56"/>
     </row>
-    <row r="28" spans="1:12" ht="15.75">
+    <row r="28" spans="1:12" ht="15.6">
       <c r="A28" s="67"/>
       <c r="B28" s="24"/>
       <c r="C28" s="31"/>
@@ -3054,7 +3063,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" ht="18.75">
+    <row r="29" spans="1:12" ht="18">
       <c r="A29" s="66">
         <v>2</v>
       </c>
@@ -3072,7 +3081,7 @@
       <c r="K29" s="44"/>
       <c r="L29" s="44"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75">
+    <row r="30" spans="1:12" ht="15.6">
       <c r="A30" s="47"/>
       <c r="B30" s="50">
         <v>2.1</v>
@@ -3100,7 +3109,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12" ht="15.75">
+    <row r="31" spans="1:12" ht="15.6">
       <c r="A31" s="67"/>
       <c r="B31" s="24"/>
       <c r="C31" s="11" t="s">
@@ -3120,7 +3129,7 @@
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
     </row>
-    <row r="32" spans="1:12" ht="47.25">
+    <row r="32" spans="1:12" ht="46.8">
       <c r="A32" s="67"/>
       <c r="B32" s="24"/>
       <c r="C32" s="11" t="s">
@@ -3140,7 +3149,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="1:12" ht="15.75">
+    <row r="33" spans="1:12" ht="15.6">
       <c r="A33" s="67"/>
       <c r="B33" s="24"/>
       <c r="C33" s="11" t="s">
@@ -3160,7 +3169,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="1:12" ht="15.75">
+    <row r="34" spans="1:12" ht="15.6">
       <c r="A34" s="67"/>
       <c r="B34" s="24"/>
       <c r="C34" s="11" t="s">
@@ -3180,7 +3189,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="1:12" ht="15.75">
+    <row r="35" spans="1:12" ht="15.6">
       <c r="A35" s="67"/>
       <c r="B35" s="24"/>
       <c r="C35" s="11" t="s">
@@ -3198,7 +3207,7 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="1:12" ht="15.75">
+    <row r="36" spans="1:12" ht="15.6">
       <c r="A36" s="67"/>
       <c r="B36" s="24"/>
       <c r="C36" s="11" t="s">
@@ -3218,7 +3227,7 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="1:12" ht="15.75">
+    <row r="37" spans="1:12" ht="15.6">
       <c r="A37" s="67"/>
       <c r="B37" s="24"/>
       <c r="C37" s="11"/>
@@ -3232,7 +3241,7 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="1:12" ht="15.75">
+    <row r="38" spans="1:12" ht="15.6">
       <c r="A38" s="85"/>
       <c r="B38" s="89" t="s">
         <v>70</v>
@@ -3262,7 +3271,7 @@
       <c r="K38" s="56"/>
       <c r="L38" s="56"/>
     </row>
-    <row r="39" spans="1:12" ht="15.75">
+    <row r="39" spans="1:12" ht="15.6">
       <c r="A39" s="67"/>
       <c r="B39" s="24"/>
       <c r="C39" s="31"/>
@@ -3276,7 +3285,7 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="1:12" ht="18.75">
+    <row r="40" spans="1:12" ht="18">
       <c r="A40" s="66">
         <v>3</v>
       </c>
@@ -3294,7 +3303,7 @@
       <c r="K40" s="44"/>
       <c r="L40" s="44"/>
     </row>
-    <row r="41" spans="1:12" ht="15.75">
+    <row r="41" spans="1:12" ht="15.6">
       <c r="A41" s="6"/>
       <c r="B41" s="49">
         <v>3.1</v>
@@ -3322,7 +3331,7 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="1:12" ht="15.75">
+    <row r="42" spans="1:12" ht="15.6">
       <c r="A42" s="67"/>
       <c r="B42" s="51"/>
       <c r="C42" s="11" t="s">
@@ -3340,7 +3349,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="1:12" ht="15.75">
+    <row r="43" spans="1:12" ht="15.6">
       <c r="A43" s="67"/>
       <c r="B43" s="24"/>
       <c r="C43" s="11" t="s">
@@ -3358,7 +3367,7 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="1:12" ht="15.75">
+    <row r="44" spans="1:12" ht="15.6">
       <c r="A44" s="67"/>
       <c r="B44" s="24"/>
       <c r="C44" s="11" t="s">
@@ -3376,7 +3385,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="1:12" ht="15.75">
+    <row r="45" spans="1:12" ht="15.6">
       <c r="A45" s="67"/>
       <c r="B45" s="24"/>
       <c r="C45" s="11"/>
@@ -3390,7 +3399,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="1:12" ht="15.75">
+    <row r="46" spans="1:12" ht="15.6">
       <c r="A46" s="67"/>
       <c r="B46" s="24"/>
       <c r="C46" s="105"/>
@@ -3404,7 +3413,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="1:12" ht="18.75">
+    <row r="47" spans="1:12" ht="18">
       <c r="A47" s="66">
         <v>4</v>
       </c>
@@ -3422,7 +3431,7 @@
       <c r="K47" s="44"/>
       <c r="L47" s="44"/>
     </row>
-    <row r="48" spans="1:12" ht="15.75">
+    <row r="48" spans="1:12" ht="15.6">
       <c r="A48" s="6"/>
       <c r="B48" s="49">
         <v>4.0999999999999996</v>
@@ -3452,7 +3461,7 @@
       </c>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:12" ht="15.75">
+    <row r="49" spans="1:12" ht="15.6">
       <c r="A49" s="67"/>
       <c r="B49" s="51"/>
       <c r="C49" s="11" t="s">
@@ -3470,7 +3479,7 @@
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:12" ht="15.75">
+    <row r="50" spans="1:12" ht="15.6">
       <c r="A50" s="67"/>
       <c r="B50" s="24"/>
       <c r="C50" s="11" t="s">
@@ -3488,7 +3497,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="1:12" ht="15.75">
+    <row r="51" spans="1:12" ht="15.6">
       <c r="A51" s="67"/>
       <c r="B51" s="24"/>
       <c r="C51" s="11" t="s">
@@ -3506,7 +3515,7 @@
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="1:12" ht="15.75">
+    <row r="52" spans="1:12" ht="15.6">
       <c r="A52" s="67"/>
       <c r="B52" s="24"/>
       <c r="C52" s="11" t="s">
@@ -3524,7 +3533,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="1:12" ht="15.75">
+    <row r="53" spans="1:12" ht="15.6">
       <c r="A53" s="67"/>
       <c r="B53" s="24"/>
       <c r="C53" s="11" t="s">
@@ -3542,7 +3551,7 @@
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="1:12" ht="15.75">
+    <row r="54" spans="1:12" ht="15.6">
       <c r="A54" s="67"/>
       <c r="B54" s="24"/>
       <c r="C54" s="11" t="s">
@@ -3560,7 +3569,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="1:12" ht="15.75">
+    <row r="55" spans="1:12" ht="15.6">
       <c r="A55" s="67"/>
       <c r="B55" s="24"/>
       <c r="C55" s="11"/>
@@ -3574,7 +3583,7 @@
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="1:12" ht="15.75">
+    <row r="56" spans="1:12" ht="15.6">
       <c r="A56" s="85"/>
       <c r="B56" s="89" t="s">
         <v>93</v>
@@ -3618,7 +3627,7 @@
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="1:12" ht="18.75">
+    <row r="58" spans="1:12" ht="18">
       <c r="A58" s="66">
         <v>5</v>
       </c>
@@ -3650,7 +3659,7 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="1:12" ht="15.75">
+    <row r="60" spans="1:12" ht="15.6">
       <c r="A60" s="69">
         <v>1</v>
       </c>
@@ -3680,7 +3689,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="15.75">
+    <row r="61" spans="1:12" ht="15.6">
       <c r="A61" s="67"/>
       <c r="B61" s="52">
         <v>1.1000000000000001</v>
@@ -3698,7 +3707,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="1:12" ht="15.75">
+    <row r="62" spans="1:12" ht="15.6">
       <c r="A62" s="67"/>
       <c r="B62" s="52">
         <v>1.2</v>
@@ -3716,7 +3725,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="1:12" ht="15.75">
+    <row r="63" spans="1:12" ht="15.6">
       <c r="A63" s="67"/>
       <c r="B63" s="52">
         <v>1.3</v>
@@ -3746,7 +3755,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="15.75">
+    <row r="64" spans="1:12" ht="15.6">
       <c r="A64" s="67"/>
       <c r="B64" s="52"/>
       <c r="C64" s="8" t="s">
@@ -3766,7 +3775,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="31.5">
+    <row r="65" spans="1:12" ht="31.2">
       <c r="A65" s="47"/>
       <c r="B65" s="52"/>
       <c r="C65" s="8" t="s">
@@ -3784,7 +3793,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75">
+    <row r="66" spans="1:12" ht="15.6">
       <c r="A66" s="67"/>
       <c r="B66" s="52"/>
       <c r="C66" s="8" t="s">
@@ -3802,7 +3811,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75">
+    <row r="67" spans="1:12" ht="15.6">
       <c r="A67" s="69">
         <v>2</v>
       </c>
@@ -3830,7 +3839,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75">
+    <row r="68" spans="1:12" ht="15.6">
       <c r="A68" s="70"/>
       <c r="B68" s="52">
         <v>2.1</v>
@@ -3848,7 +3857,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75">
+    <row r="69" spans="1:12" ht="15.6">
       <c r="A69" s="70"/>
       <c r="B69" s="52">
         <v>2.2000000000000002</v>
@@ -3866,7 +3875,7 @@
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75">
+    <row r="70" spans="1:12" ht="15.6">
       <c r="A70" s="70"/>
       <c r="B70" s="52">
         <v>2.2999999999999998</v>
@@ -3884,7 +3893,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75">
+    <row r="71" spans="1:12" ht="15.6">
       <c r="A71" s="70"/>
       <c r="B71" s="52"/>
       <c r="C71" s="8"/>
@@ -3898,7 +3907,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75">
+    <row r="72" spans="1:12" ht="15.6">
       <c r="A72" s="69">
         <v>3</v>
       </c>
@@ -3928,7 +3937,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75">
+    <row r="73" spans="1:12" ht="15.6">
       <c r="A73" s="70"/>
       <c r="B73" s="52">
         <v>3.1</v>
@@ -3946,7 +3955,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75">
+    <row r="74" spans="1:12" ht="15.6">
       <c r="A74" s="70"/>
       <c r="B74" s="52">
         <v>3.2</v>
@@ -3964,7 +3973,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75">
+    <row r="75" spans="1:12" ht="15.6">
       <c r="A75" s="70"/>
       <c r="B75" s="52">
         <v>3.3</v>
@@ -3982,7 +3991,7 @@
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75">
+    <row r="76" spans="1:12" ht="15.6">
       <c r="A76" s="70"/>
       <c r="B76" s="52">
         <v>3.4</v>
@@ -4000,7 +4009,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75">
+    <row r="77" spans="1:12" ht="15.6">
       <c r="A77" s="69">
         <v>4</v>
       </c>
@@ -4028,7 +4037,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75">
+    <row r="78" spans="1:12" ht="15.6">
       <c r="A78" s="70"/>
       <c r="B78" s="52">
         <v>4.0999999999999996</v>
@@ -4060,7 +4069,7 @@
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="1:12" ht="18.75">
+    <row r="80" spans="1:12" ht="18">
       <c r="A80" s="66">
         <v>5</v>
       </c>
@@ -4078,7 +4087,7 @@
       <c r="K80" s="44"/>
       <c r="L80" s="44"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75">
+    <row r="81" spans="1:12" ht="15.6">
       <c r="A81" s="6"/>
       <c r="B81" s="49">
         <v>5.0999999999999996</v>
@@ -4106,7 +4115,7 @@
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75">
+    <row r="82" spans="1:12" ht="15.6">
       <c r="A82" s="67"/>
       <c r="B82" s="24"/>
       <c r="C82" s="11" t="s">
@@ -4124,7 +4133,7 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" ht="31.5">
+    <row r="83" spans="1:12" ht="31.2">
       <c r="A83" s="67"/>
       <c r="B83" s="24"/>
       <c r="C83" s="11" t="s">
@@ -4142,7 +4151,7 @@
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" ht="31.5">
+    <row r="84" spans="1:12" ht="31.2">
       <c r="A84" s="67"/>
       <c r="B84" s="24"/>
       <c r="C84" s="11" t="s">
@@ -4162,7 +4171,7 @@
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" ht="31.5">
+    <row r="85" spans="1:12" ht="31.2">
       <c r="A85" s="67"/>
       <c r="B85" s="24"/>
       <c r="C85" s="11" t="s">
@@ -4182,7 +4191,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" ht="31.5">
+    <row r="86" spans="1:12" ht="31.2">
       <c r="A86" s="47"/>
       <c r="B86" s="49">
         <v>5.2</v>
@@ -4212,7 +4221,7 @@
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75">
+    <row r="87" spans="1:12" ht="15.6">
       <c r="A87" s="67"/>
       <c r="B87" s="24"/>
       <c r="C87" s="11" t="s">
@@ -4230,7 +4239,7 @@
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75">
+    <row r="88" spans="1:12" ht="15.6">
       <c r="A88" s="67"/>
       <c r="B88" s="24"/>
       <c r="C88" s="11" t="s">
@@ -4248,7 +4257,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75">
+    <row r="89" spans="1:12" ht="15.6">
       <c r="A89" s="67"/>
       <c r="B89" s="24"/>
       <c r="C89" s="11" t="s">
@@ -4266,7 +4275,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75">
+    <row r="90" spans="1:12" ht="15.6">
       <c r="A90" s="67"/>
       <c r="B90" s="24"/>
       <c r="C90" s="11"/>
@@ -4280,7 +4289,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75">
+    <row r="91" spans="1:12" ht="15.6">
       <c r="A91" s="47"/>
       <c r="B91" s="49">
         <v>5.3</v>
@@ -4308,7 +4317,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75">
+    <row r="92" spans="1:12" ht="15.6">
       <c r="A92" s="67"/>
       <c r="B92" s="24"/>
       <c r="C92" s="11" t="s">
@@ -4326,7 +4335,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75">
+    <row r="93" spans="1:12" ht="15.6">
       <c r="A93" s="67"/>
       <c r="B93" s="24"/>
       <c r="C93" s="11" t="s">
@@ -4344,7 +4353,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75">
+    <row r="94" spans="1:12" ht="15.6">
       <c r="A94" s="67"/>
       <c r="B94" s="24"/>
       <c r="C94" s="11"/>
@@ -4358,7 +4367,7 @@
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
     </row>
-    <row r="95" spans="1:12" ht="47.25">
+    <row r="95" spans="1:12" ht="31.2">
       <c r="A95" s="67"/>
       <c r="B95" s="49">
         <v>5.4</v>
@@ -4388,7 +4397,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="30">
+    <row r="96" spans="1:12" ht="28.8">
       <c r="A96" s="47"/>
       <c r="B96" s="49">
         <v>5.5</v>
@@ -4408,7 +4417,7 @@
       <c r="K96" s="3"/>
       <c r="L96" s="3"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75">
+    <row r="97" spans="1:12" ht="15.6">
       <c r="A97" s="47"/>
       <c r="B97" s="49">
         <v>5.6</v>
@@ -4426,7 +4435,7 @@
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75">
+    <row r="98" spans="1:12" ht="15.6">
       <c r="A98" s="47"/>
       <c r="B98" s="49">
         <v>5.7</v>
@@ -4460,7 +4469,7 @@
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75">
+    <row r="100" spans="1:12" ht="15.6">
       <c r="A100" s="6"/>
       <c r="B100" s="1">
         <v>5.8</v>
@@ -4492,7 +4501,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="15.75">
+    <row r="101" spans="1:12" ht="15.6">
       <c r="A101" s="67"/>
       <c r="B101" s="24"/>
       <c r="C101" s="11" t="s">
@@ -4512,7 +4521,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="15.75">
+    <row r="102" spans="1:12" ht="15.6">
       <c r="A102" s="67"/>
       <c r="B102" s="24"/>
       <c r="C102" s="11" t="s">
@@ -4530,7 +4539,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75">
+    <row r="103" spans="1:12" ht="15.6">
       <c r="A103" s="67"/>
       <c r="B103" s="24"/>
       <c r="C103" s="11" t="s">
@@ -4548,7 +4557,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
     </row>
-    <row r="104" spans="1:12" ht="31.5">
+    <row r="104" spans="1:12" ht="31.2">
       <c r="A104" s="67"/>
       <c r="B104" s="24"/>
       <c r="C104" s="11" t="s">
@@ -4566,7 +4575,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75">
+    <row r="105" spans="1:12" ht="15.6">
       <c r="A105" s="67"/>
       <c r="B105" s="24"/>
       <c r="C105" s="11" t="s">
@@ -4586,7 +4595,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75">
+    <row r="106" spans="1:12" ht="15.6">
       <c r="A106" s="67"/>
       <c r="B106" s="24"/>
       <c r="C106" s="11" t="s">
@@ -4604,7 +4613,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75">
+    <row r="107" spans="1:12" ht="15.6">
       <c r="A107" s="67"/>
       <c r="B107" s="24"/>
       <c r="C107" s="11"/>
@@ -4618,7 +4627,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="1:12" s="20" customFormat="1" ht="37.5">
+    <row r="108" spans="1:12" s="20" customFormat="1" ht="36">
       <c r="A108" s="71">
         <v>6</v>
       </c>
@@ -4732,18 +4741,18 @@
       <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9" style="29" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" style="29" customWidth="1"/>
-    <col min="3" max="3" width="65.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" style="29" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="29" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="89.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" style="29" customWidth="1"/>
+    <col min="3" max="3" width="65.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" style="29" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="29" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="89.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="29" customFormat="1">
@@ -4778,7 +4787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="45">
+    <row r="2" spans="1:10" ht="43.2">
       <c r="A2" s="28" t="s">
         <v>160</v>
       </c>
@@ -6183,17 +6192,17 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="29"/>
-    <col min="2" max="2" width="25.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="29"/>
+    <col min="2" max="2" width="25.33203125" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="29"/>
-    <col min="5" max="5" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="29" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="29"/>
+    <col min="5" max="5" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" style="29" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="29" customFormat="1">
@@ -6750,19 +6759,19 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="29"/>
-    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="29"/>
+    <col min="2" max="2" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" style="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="29" customFormat="1">
@@ -7403,21 +7412,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3782443B-979F-4126-A9F9-516CD045F0D0}">
   <dimension ref="A1:L114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="29"/>
-    <col min="4" max="4" width="66.85546875" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" style="29" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" style="29" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="29"/>
+    <col min="4" max="4" width="66.88671875" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" style="29" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" style="29" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" customHeight="1">
@@ -7436,7 +7445,7 @@
       <c r="K1" s="111"/>
       <c r="L1" s="111"/>
     </row>
-    <row r="2" spans="1:12" ht="18.75">
+    <row r="2" spans="1:12" ht="18">
       <c r="A2" s="112" t="s">
         <v>422</v>
       </c>
@@ -7466,7 +7475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75">
+    <row r="3" spans="1:12" ht="15.6">
       <c r="A3" s="23"/>
       <c r="B3" s="16"/>
       <c r="C3" s="15"/>
@@ -7482,7 +7491,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75">
+    <row r="4" spans="1:12" ht="15.6">
       <c r="A4" s="76">
         <v>1</v>
       </c>
@@ -7502,7 +7511,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75">
+    <row r="5" spans="1:12" ht="15.6">
       <c r="A5" s="78"/>
       <c r="B5" s="18">
         <v>1.1000000000000001</v>
@@ -7522,7 +7531,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75">
+    <row r="6" spans="1:12" ht="15.6">
       <c r="A6" s="78"/>
       <c r="B6" s="18">
         <v>1.2</v>
@@ -7542,7 +7551,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75">
+    <row r="7" spans="1:12" ht="15.6">
       <c r="A7" s="78"/>
       <c r="B7" s="18">
         <v>1.3</v>
@@ -7562,7 +7571,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75">
+    <row r="8" spans="1:12" ht="15.6">
       <c r="A8" s="78"/>
       <c r="B8" s="18"/>
       <c r="C8" s="19" t="s">
@@ -7580,7 +7589,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75">
+    <row r="9" spans="1:12" ht="15.6">
       <c r="A9" s="78"/>
       <c r="B9" s="18"/>
       <c r="C9" s="19" t="s">
@@ -7604,7 +7613,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75">
+    <row r="10" spans="1:12" ht="15.6">
       <c r="A10" s="78"/>
       <c r="B10" s="18"/>
       <c r="C10" s="19" t="s">
@@ -7622,7 +7631,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75">
+    <row r="11" spans="1:12" ht="15.6">
       <c r="A11" s="78"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19" t="s">
@@ -7640,7 +7649,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75">
+    <row r="12" spans="1:12" ht="15.6">
       <c r="A12" s="78"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19" t="s">
@@ -7658,7 +7667,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75">
+    <row r="13" spans="1:12" ht="15.6">
       <c r="A13" s="78"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19" t="s">
@@ -7676,7 +7685,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75">
+    <row r="14" spans="1:12" ht="15.6">
       <c r="A14" s="78"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
@@ -7690,7 +7699,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75">
+    <row r="15" spans="1:12" ht="15.6">
       <c r="A15" s="76">
         <v>2</v>
       </c>
@@ -7714,7 +7723,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75">
+    <row r="16" spans="1:12" ht="15.6">
       <c r="A16" s="78"/>
       <c r="B16" s="18">
         <v>2.1</v>
@@ -7738,7 +7747,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75">
+    <row r="17" spans="1:12" ht="15.6">
       <c r="A17" s="78"/>
       <c r="B17" s="18">
         <v>2.2000000000000002</v>
@@ -7762,7 +7771,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75">
+    <row r="18" spans="1:12" ht="15.6">
       <c r="A18" s="78"/>
       <c r="B18" s="18">
         <v>2.2999999999999998</v>
@@ -7788,7 +7797,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75">
+    <row r="19" spans="1:12" ht="15.6">
       <c r="A19" s="78"/>
       <c r="B19" s="18">
         <v>2.4</v>
@@ -7814,7 +7823,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" ht="15.75">
+    <row r="20" spans="1:12" ht="15.6">
       <c r="A20" s="78"/>
       <c r="B20" s="18">
         <v>2.5</v>
@@ -7834,7 +7843,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75">
+    <row r="21" spans="1:12" ht="15.6">
       <c r="A21" s="78"/>
       <c r="B21" s="18"/>
       <c r="C21" s="19" t="s">
@@ -7856,7 +7865,7 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75">
+    <row r="22" spans="1:12" ht="15.6">
       <c r="A22" s="78"/>
       <c r="B22" s="18"/>
       <c r="C22" s="19" t="s">
@@ -7878,7 +7887,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75">
+    <row r="23" spans="1:12" ht="15.6">
       <c r="A23" s="78"/>
       <c r="B23" s="18"/>
       <c r="C23" s="19" t="s">
@@ -7900,7 +7909,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75">
+    <row r="24" spans="1:12" ht="15.6">
       <c r="A24" s="78"/>
       <c r="B24" s="18">
         <v>2.6</v>
@@ -7924,7 +7933,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" ht="15.75">
+    <row r="25" spans="1:12" ht="15.6">
       <c r="A25" s="78"/>
       <c r="B25" s="18">
         <v>2.7</v>
@@ -7948,7 +7957,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:12" ht="15.75">
+    <row r="26" spans="1:12" ht="15.6">
       <c r="A26" s="78"/>
       <c r="B26" s="18">
         <v>2.8</v>
@@ -7972,7 +7981,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:12" ht="15.75">
+    <row r="27" spans="1:12" ht="15.6">
       <c r="A27" s="78"/>
       <c r="B27" s="18">
         <v>2.9</v>
@@ -7994,7 +8003,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="1:12" ht="15.75">
+    <row r="28" spans="1:12" ht="15.6">
       <c r="A28" s="78"/>
       <c r="B28" s="18">
         <v>2.1</v>
@@ -8018,7 +8027,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" ht="15.75">
+    <row r="29" spans="1:12" ht="15.6">
       <c r="A29" s="78"/>
       <c r="B29" s="18"/>
       <c r="C29" s="19"/>
@@ -8038,7 +8047,7 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75">
+    <row r="30" spans="1:12" ht="15.6">
       <c r="A30" s="78"/>
       <c r="B30" s="18"/>
       <c r="C30" s="17"/>
@@ -8052,7 +8061,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12" ht="31.5">
+    <row r="31" spans="1:12" ht="31.2">
       <c r="A31" s="82"/>
       <c r="B31" s="79"/>
       <c r="C31" s="84" t="s">
@@ -8076,7 +8085,7 @@
       <c r="K31" s="56"/>
       <c r="L31" s="56"/>
     </row>
-    <row r="32" spans="1:12" ht="15.75">
+    <row r="32" spans="1:12" ht="15.6">
       <c r="A32" s="76"/>
       <c r="B32" s="16"/>
       <c r="C32" s="15"/>
@@ -8092,7 +8101,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="1:12" ht="15.75">
+    <row r="33" spans="1:12" ht="15.6">
       <c r="A33" s="78"/>
       <c r="B33" s="18"/>
       <c r="C33" s="19"/>
@@ -8106,7 +8115,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="1:12" ht="15.75">
+    <row r="34" spans="1:12" ht="15.6">
       <c r="A34" s="78"/>
       <c r="B34" s="18"/>
       <c r="C34" s="19"/>
@@ -8122,7 +8131,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="1:12" ht="15.75">
+    <row r="35" spans="1:12" ht="15.6">
       <c r="A35" s="76">
         <v>3</v>
       </c>
@@ -8142,7 +8151,7 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="1:12" ht="15.75">
+    <row r="36" spans="1:12" ht="15.6">
       <c r="A36" s="78"/>
       <c r="B36" s="18">
         <v>3.1</v>
@@ -8168,7 +8177,7 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="1:12" ht="15.75">
+    <row r="37" spans="1:12" ht="15.6">
       <c r="A37" s="78"/>
       <c r="B37" s="18">
         <v>3.2</v>
@@ -8188,7 +8197,7 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="1:12" ht="15.75">
+    <row r="38" spans="1:12" ht="15.6">
       <c r="A38" s="78"/>
       <c r="B38" s="18">
         <v>3.3</v>
@@ -8208,7 +8217,7 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="1:12" ht="15.75">
+    <row r="39" spans="1:12" ht="15.6">
       <c r="A39" s="78"/>
       <c r="B39" s="18">
         <v>3.4</v>
@@ -8228,7 +8237,7 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="1:12" ht="15.75">
+    <row r="40" spans="1:12" ht="15.6">
       <c r="A40" s="78"/>
       <c r="B40" s="18">
         <v>3.5</v>
@@ -8248,7 +8257,7 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="1:12" ht="15.75">
+    <row r="41" spans="1:12" ht="15.6">
       <c r="A41" s="78"/>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
@@ -8262,7 +8271,7 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="1:12" ht="15.75">
+    <row r="42" spans="1:12" ht="15.6">
       <c r="A42" s="78"/>
       <c r="B42" s="18"/>
       <c r="C42" s="19"/>
@@ -8276,7 +8285,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="1:12" ht="15.75">
+    <row r="43" spans="1:12" ht="15.6">
       <c r="A43" s="76">
         <v>4</v>
       </c>
@@ -8296,7 +8305,7 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="1:12" ht="15.75">
+    <row r="44" spans="1:12" ht="15.6">
       <c r="A44" s="78"/>
       <c r="B44" s="18">
         <v>4.0999999999999996</v>
@@ -8320,7 +8329,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="1:12" ht="15.75">
+    <row r="45" spans="1:12" ht="15.6">
       <c r="A45" s="78"/>
       <c r="B45" s="18"/>
       <c r="C45" s="19" t="s">
@@ -8338,7 +8347,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="1:12" ht="15.75">
+    <row r="46" spans="1:12" ht="15.6">
       <c r="A46" s="78"/>
       <c r="B46" s="18"/>
       <c r="C46" s="19" t="s">
@@ -8356,7 +8365,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="1:12" ht="15.75">
+    <row r="47" spans="1:12" ht="15.6">
       <c r="A47" s="78"/>
       <c r="B47" s="18">
         <v>4.2</v>
@@ -8380,7 +8389,7 @@
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="1:12" ht="15.75">
+    <row r="48" spans="1:12" ht="15.6">
       <c r="A48" s="78"/>
       <c r="B48" s="18"/>
       <c r="C48" s="19" t="s">
@@ -8398,7 +8407,7 @@
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:12" ht="15.75">
+    <row r="49" spans="1:12" ht="15.6">
       <c r="A49" s="78"/>
       <c r="B49" s="18"/>
       <c r="C49" s="19" t="s">
@@ -8416,7 +8425,7 @@
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:12" ht="15.75">
+    <row r="50" spans="1:12" ht="15.6">
       <c r="A50" s="78"/>
       <c r="B50" s="18"/>
       <c r="C50" s="19" t="s">
@@ -8434,7 +8443,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="1:12" ht="15.75">
+    <row r="51" spans="1:12" ht="15.6">
       <c r="A51" s="78"/>
       <c r="B51" s="18">
         <v>4.3</v>
@@ -8460,7 +8469,7 @@
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="1:12" ht="15.75">
+    <row r="52" spans="1:12" ht="15.6">
       <c r="A52" s="78"/>
       <c r="B52" s="18"/>
       <c r="C52" s="19" t="s">
@@ -8478,7 +8487,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="1:12" ht="15.75">
+    <row r="53" spans="1:12" ht="15.6">
       <c r="A53" s="78"/>
       <c r="B53" s="18"/>
       <c r="C53" s="19" t="s">
@@ -8496,7 +8505,7 @@
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="1:12" ht="15.75">
+    <row r="54" spans="1:12" ht="15.6">
       <c r="A54" s="78"/>
       <c r="B54" s="18"/>
       <c r="C54" s="19" t="s">
@@ -8514,7 +8523,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="1:12" ht="15.75">
+    <row r="55" spans="1:12" ht="15.6">
       <c r="A55" s="78"/>
       <c r="B55" s="18"/>
       <c r="C55" s="19" t="s">
@@ -8532,7 +8541,7 @@
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="1:12" ht="15.75">
+    <row r="56" spans="1:12" ht="15.6">
       <c r="A56" s="78"/>
       <c r="B56" s="18"/>
       <c r="C56" s="19" t="s">
@@ -8550,7 +8559,7 @@
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
     </row>
-    <row r="57" spans="1:12" ht="15.75">
+    <row r="57" spans="1:12" ht="15.6">
       <c r="A57" s="78"/>
       <c r="B57" s="18"/>
       <c r="C57" s="19" t="s">
@@ -8568,7 +8577,7 @@
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="1:12" ht="15.75">
+    <row r="58" spans="1:12" ht="15.6">
       <c r="A58" s="78"/>
       <c r="B58" s="18"/>
       <c r="C58" s="19" t="s">
@@ -8586,7 +8595,7 @@
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="1:12" ht="15.75">
+    <row r="59" spans="1:12" ht="15.6">
       <c r="A59" s="78"/>
       <c r="B59" s="18">
         <v>4.4000000000000004</v>
@@ -8612,7 +8621,7 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="1:12" ht="15.75">
+    <row r="60" spans="1:12" ht="15.6">
       <c r="A60" s="78"/>
       <c r="B60" s="18"/>
       <c r="C60" s="19" t="s">
@@ -8630,7 +8639,7 @@
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="1:12" ht="15.75">
+    <row r="61" spans="1:12" ht="15.6">
       <c r="A61" s="78"/>
       <c r="B61" s="18">
         <v>4.5</v>
@@ -8656,7 +8665,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="1:12" ht="15.75">
+    <row r="62" spans="1:12" ht="15.6">
       <c r="A62" s="78"/>
       <c r="B62" s="18"/>
       <c r="C62" s="19" t="s">
@@ -8674,7 +8683,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="1:12" ht="15.75">
+    <row r="63" spans="1:12" ht="15.6">
       <c r="A63" s="78"/>
       <c r="B63" s="18"/>
       <c r="C63" s="19" t="s">
@@ -8692,7 +8701,7 @@
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="1:12" ht="15.75">
+    <row r="64" spans="1:12" ht="15.6">
       <c r="A64" s="78"/>
       <c r="B64" s="18">
         <v>4.5999999999999996</v>
@@ -8712,7 +8721,7 @@
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75">
+    <row r="65" spans="1:12" ht="15.6">
       <c r="A65" s="78"/>
       <c r="B65" s="18"/>
       <c r="C65" s="19" t="s">
@@ -8730,7 +8739,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75">
+    <row r="66" spans="1:12" ht="15.6">
       <c r="A66" s="78"/>
       <c r="B66" s="18">
         <v>4.7</v>
@@ -8750,7 +8759,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75">
+    <row r="67" spans="1:12" ht="15.6">
       <c r="A67" s="78"/>
       <c r="B67" s="18"/>
       <c r="C67" s="19" t="s">
@@ -8768,7 +8777,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75">
+    <row r="68" spans="1:12" ht="15.6">
       <c r="A68" s="78"/>
       <c r="B68" s="18"/>
       <c r="C68" s="19" t="s">
@@ -8786,7 +8795,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75">
+    <row r="69" spans="1:12" ht="15.6">
       <c r="A69" s="78"/>
       <c r="B69" s="18">
         <v>4.8</v>
@@ -8806,7 +8815,7 @@
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75">
+    <row r="70" spans="1:12" ht="15.6">
       <c r="A70" s="78"/>
       <c r="B70" s="18"/>
       <c r="C70" s="19" t="s">
@@ -8824,7 +8833,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75">
+    <row r="71" spans="1:12" ht="15.6">
       <c r="A71" s="78"/>
       <c r="B71" s="18"/>
       <c r="C71" s="19" t="s">
@@ -8842,7 +8851,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75">
+    <row r="72" spans="1:12" ht="15.6">
       <c r="A72" s="78"/>
       <c r="B72" s="18"/>
       <c r="C72" s="19" t="s">
@@ -8860,7 +8869,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75">
+    <row r="73" spans="1:12" ht="15.6">
       <c r="A73" s="78"/>
       <c r="B73" s="18"/>
       <c r="C73" s="19" t="s">
@@ -8878,7 +8887,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75">
+    <row r="74" spans="1:12" ht="15.6">
       <c r="A74" s="78"/>
       <c r="B74" s="18"/>
       <c r="C74" s="19" t="s">
@@ -8896,7 +8905,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75">
+    <row r="75" spans="1:12" ht="15.6">
       <c r="A75" s="78"/>
       <c r="B75" s="18">
         <v>4.9000000000000004</v>
@@ -8916,7 +8925,7 @@
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75">
+    <row r="76" spans="1:12" ht="15.6">
       <c r="A76" s="78"/>
       <c r="B76" s="18">
         <v>4.0999999999999996</v>
@@ -8936,7 +8945,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75">
+    <row r="77" spans="1:12" ht="15.6">
       <c r="A77" s="78"/>
       <c r="B77" s="18"/>
       <c r="C77" s="19" t="s">
@@ -8954,7 +8963,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75">
+    <row r="78" spans="1:12" ht="15.6">
       <c r="A78" s="78"/>
       <c r="B78" s="18">
         <v>4.1100000000000003</v>
@@ -8974,7 +8983,7 @@
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75">
+    <row r="79" spans="1:12" ht="15.6">
       <c r="A79" s="78"/>
       <c r="B79" s="18"/>
       <c r="C79" s="19" t="s">
@@ -8992,7 +9001,7 @@
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="1:12" ht="15.75">
+    <row r="80" spans="1:12" ht="15.6">
       <c r="A80" s="78"/>
       <c r="B80" s="18"/>
       <c r="C80" s="19" t="s">
@@ -9010,7 +9019,7 @@
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75">
+    <row r="81" spans="1:12" ht="15.6">
       <c r="A81" s="78"/>
       <c r="B81" s="18"/>
       <c r="C81" s="19" t="s">
@@ -9028,7 +9037,7 @@
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75">
+    <row r="82" spans="1:12" ht="15.6">
       <c r="A82" s="78"/>
       <c r="B82" s="18"/>
       <c r="C82" s="19" t="s">
@@ -9046,7 +9055,7 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" ht="15.75">
+    <row r="83" spans="1:12" ht="15.6">
       <c r="A83" s="78"/>
       <c r="B83" s="18">
         <v>4.12</v>
@@ -9066,7 +9075,7 @@
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" ht="15.75">
+    <row r="84" spans="1:12" ht="15.6">
       <c r="A84" s="78"/>
       <c r="B84" s="18"/>
       <c r="C84" s="19" t="s">
@@ -9084,7 +9093,7 @@
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" ht="15.75">
+    <row r="85" spans="1:12" ht="15.6">
       <c r="A85" s="78"/>
       <c r="B85" s="18"/>
       <c r="C85" s="19" t="s">
@@ -9102,7 +9111,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" ht="15.75">
+    <row r="86" spans="1:12" ht="15.6">
       <c r="A86" s="78"/>
       <c r="B86" s="18"/>
       <c r="C86" s="19" t="s">
@@ -9120,7 +9129,7 @@
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75">
+    <row r="87" spans="1:12" ht="15.6">
       <c r="A87" s="78"/>
       <c r="B87" s="18">
         <v>4.13</v>
@@ -9140,7 +9149,7 @@
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75">
+    <row r="88" spans="1:12" ht="15.6">
       <c r="A88" s="78"/>
       <c r="B88" s="18"/>
       <c r="C88" s="19" t="s">
@@ -9158,7 +9167,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75">
+    <row r="89" spans="1:12" ht="15.6">
       <c r="A89" s="78"/>
       <c r="B89" s="18">
         <v>4.1399999999999997</v>
@@ -9178,7 +9187,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75">
+    <row r="90" spans="1:12" ht="15.6">
       <c r="A90" s="78"/>
       <c r="B90" s="18">
         <v>4.1500000000000004</v>
@@ -9198,7 +9207,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75">
+    <row r="91" spans="1:12" ht="15.6">
       <c r="A91" s="78"/>
       <c r="B91" s="18"/>
       <c r="C91" s="19" t="s">
@@ -9216,7 +9225,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75">
+    <row r="92" spans="1:12" ht="15.6">
       <c r="A92" s="78"/>
       <c r="B92" s="18"/>
       <c r="C92" s="19" t="s">
@@ -9234,7 +9243,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75">
+    <row r="93" spans="1:12" ht="15.6">
       <c r="A93" s="78"/>
       <c r="B93" s="18"/>
       <c r="C93" s="19"/>
@@ -9252,7 +9261,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75">
+    <row r="94" spans="1:12" ht="15.6">
       <c r="A94" s="78"/>
       <c r="B94" s="17"/>
       <c r="C94" s="17"/>
@@ -9266,7 +9275,7 @@
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75">
+    <row r="95" spans="1:12" ht="15.6">
       <c r="A95" s="82"/>
       <c r="B95" s="79"/>
       <c r="C95" s="81" t="s">
@@ -9286,7 +9295,7 @@
       <c r="K95" s="56"/>
       <c r="L95" s="56"/>
     </row>
-    <row r="96" spans="1:12" ht="15.75">
+    <row r="96" spans="1:12" ht="15.6">
       <c r="A96" s="82"/>
       <c r="B96" s="79"/>
       <c r="C96" s="81"/>
@@ -9314,7 +9323,7 @@
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75">
+    <row r="98" spans="1:12" ht="15.6">
       <c r="A98" s="76">
         <v>5</v>
       </c>
@@ -9334,7 +9343,7 @@
       <c r="K98" s="3"/>
       <c r="L98" s="3"/>
     </row>
-    <row r="99" spans="1:12" ht="15.75">
+    <row r="99" spans="1:12" ht="15.6">
       <c r="A99" s="78"/>
       <c r="B99" s="18">
         <v>5.0999999999999996</v>
@@ -9354,7 +9363,7 @@
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75">
+    <row r="100" spans="1:12" ht="15.6">
       <c r="A100" s="78"/>
       <c r="B100" s="18">
         <v>5.2</v>
@@ -9374,7 +9383,7 @@
       <c r="K100" s="3"/>
       <c r="L100" s="3"/>
     </row>
-    <row r="101" spans="1:12" ht="15.75">
+    <row r="101" spans="1:12" ht="15.6">
       <c r="A101" s="78"/>
       <c r="B101" s="18">
         <v>5.3</v>
@@ -9394,7 +9403,7 @@
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
     </row>
-    <row r="102" spans="1:12" ht="15.75">
+    <row r="102" spans="1:12" ht="15.6">
       <c r="A102" s="78"/>
       <c r="B102" s="18"/>
       <c r="C102" s="19"/>
@@ -9408,7 +9417,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75">
+    <row r="103" spans="1:12" ht="15.6">
       <c r="A103" s="76">
         <v>6</v>
       </c>
@@ -9430,7 +9439,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
     </row>
-    <row r="104" spans="1:12" ht="15.75">
+    <row r="104" spans="1:12" ht="15.6">
       <c r="A104" s="78"/>
       <c r="B104" s="18">
         <v>6.1</v>
@@ -9448,7 +9457,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75">
+    <row r="105" spans="1:12" ht="15.6">
       <c r="A105" s="78"/>
       <c r="B105" s="18">
         <v>6.2</v>
@@ -9466,7 +9475,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75">
+    <row r="106" spans="1:12" ht="15.6">
       <c r="A106" s="78"/>
       <c r="B106" s="18">
         <v>6.3</v>
@@ -9484,7 +9493,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75">
+    <row r="107" spans="1:12" ht="15.6">
       <c r="A107" s="78"/>
       <c r="B107" s="18">
         <v>6.4</v>
@@ -9502,7 +9511,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="1:12" ht="15.75">
+    <row r="108" spans="1:12" ht="15.6">
       <c r="A108" s="78"/>
       <c r="B108" s="18">
         <v>6.5</v>
@@ -9520,7 +9529,7 @@
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
     </row>
-    <row r="109" spans="1:12" ht="15.75">
+    <row r="109" spans="1:12" ht="15.6">
       <c r="A109" s="78"/>
       <c r="B109" s="18">
         <v>6.6</v>
@@ -9538,7 +9547,7 @@
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
     </row>
-    <row r="110" spans="1:12" ht="15.75">
+    <row r="110" spans="1:12" ht="15.6">
       <c r="A110" s="78"/>
       <c r="B110" s="18"/>
       <c r="C110" s="19"/>
@@ -9552,7 +9561,7 @@
       <c r="K110" s="3"/>
       <c r="L110" s="3"/>
     </row>
-    <row r="111" spans="1:12" ht="94.5">
+    <row r="111" spans="1:12" ht="93.6">
       <c r="A111" s="82"/>
       <c r="B111" s="79"/>
       <c r="C111" s="81" t="s">
@@ -9609,7 +9618,7 @@
       <c r="K113" s="32"/>
       <c r="L113" s="32"/>
     </row>
-    <row r="114" spans="1:12" ht="15.75">
+    <row r="114" spans="1:12" ht="15.6">
       <c r="D114" s="22" t="s">
         <v>378</v>
       </c>

</xml_diff>

<commit_message>
.net core final demo modifications and dexExtreme
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\officeWork\RKIT_Internship_work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EF7CDA-C096-46B5-9EC2-C804375D64A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93473A6E-7BD8-4D31-8AF6-7BC0781F6D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="4" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
   <sheets>
     <sheet name=" Basic GUI" sheetId="1" r:id="rId1"/>
@@ -24,21 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="485">
   <si>
     <t>Topic</t>
   </si>
@@ -2484,20 +2475,20 @@
       <selection activeCell="J95" sqref="J95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="72" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="72" customWidth="1"/>
     <col min="2" max="2" width="6" style="29" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
     <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="5" width="53.44140625" customWidth="1"/>
-    <col min="6" max="9" width="9.33203125" style="29" customWidth="1"/>
-    <col min="10" max="10" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="51.44140625" customWidth="1"/>
+    <col min="5" max="5" width="53.42578125" customWidth="1"/>
+    <col min="6" max="9" width="9.28515625" style="29" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="51.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="40" customFormat="1" ht="18">
+    <row r="1" spans="1:12" s="40" customFormat="1" ht="18.75">
       <c r="A1" s="106" t="s">
         <v>0</v>
       </c>
@@ -2523,7 +2514,7 @@
       <c r="K1" s="41"/>
       <c r="L1" s="41"/>
     </row>
-    <row r="2" spans="1:12" s="29" customFormat="1" ht="18">
+    <row r="2" spans="1:12" s="29" customFormat="1" ht="18.75">
       <c r="A2" s="66">
         <v>1</v>
       </c>
@@ -2547,7 +2538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6">
+    <row r="3" spans="1:12" ht="15.75">
       <c r="A3" s="47"/>
       <c r="B3" s="46">
         <v>1.1000000000000001</v>
@@ -2575,7 +2566,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="31.2">
+    <row r="4" spans="1:12" ht="31.5">
       <c r="A4" s="67"/>
       <c r="B4" s="24"/>
       <c r="C4" s="31" t="s">
@@ -2595,7 +2586,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="15.6">
+    <row r="5" spans="1:12" ht="15.75">
       <c r="A5" s="67"/>
       <c r="B5" s="24"/>
       <c r="C5" s="31" t="s">
@@ -2613,7 +2604,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="15.6">
+    <row r="6" spans="1:12" ht="15.75">
       <c r="A6" s="67"/>
       <c r="B6" s="24"/>
       <c r="C6" s="31" t="s">
@@ -2631,7 +2622,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="15.6">
+    <row r="7" spans="1:12" ht="15.75">
       <c r="A7" s="47"/>
       <c r="B7" s="49">
         <v>1.2</v>
@@ -2659,7 +2650,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15.6">
+    <row r="8" spans="1:12" ht="15.75">
       <c r="A8" s="67"/>
       <c r="B8" s="24"/>
       <c r="C8" s="31" t="s">
@@ -2677,7 +2668,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="15.6">
+    <row r="9" spans="1:12" ht="15.75">
       <c r="A9" s="67"/>
       <c r="B9" s="24"/>
       <c r="C9" s="31" t="s">
@@ -2695,7 +2686,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15.6">
+    <row r="10" spans="1:12" ht="15.75">
       <c r="A10" s="67"/>
       <c r="B10" s="24"/>
       <c r="C10" s="31" t="s">
@@ -2713,7 +2704,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15.6">
+    <row r="11" spans="1:12" ht="15.75">
       <c r="A11" s="67"/>
       <c r="B11" s="24"/>
       <c r="C11" s="31" t="s">
@@ -2731,7 +2722,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15.6">
+    <row r="12" spans="1:12" ht="15.75">
       <c r="A12" s="67"/>
       <c r="B12" s="24"/>
       <c r="C12" s="31" t="s">
@@ -2749,7 +2740,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15.6">
+    <row r="13" spans="1:12" ht="15.75">
       <c r="A13" s="67"/>
       <c r="B13" s="24"/>
       <c r="C13" s="31" t="s">
@@ -2767,7 +2758,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15.6">
+    <row r="14" spans="1:12" ht="15.75">
       <c r="A14" s="67"/>
       <c r="B14" s="24"/>
       <c r="C14" s="31" t="s">
@@ -2785,7 +2776,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="15.6">
+    <row r="15" spans="1:12" ht="15.75">
       <c r="A15" s="67"/>
       <c r="B15" s="24"/>
       <c r="C15" s="31" t="s">
@@ -2803,7 +2794,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15.6">
+    <row r="16" spans="1:12" ht="15.75">
       <c r="A16" s="67"/>
       <c r="B16" s="24"/>
       <c r="C16" s="31" t="s">
@@ -2821,7 +2812,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" ht="15.6">
+    <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="47"/>
       <c r="B17" s="49">
         <v>1.3</v>
@@ -2849,7 +2840,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" ht="15.6">
+    <row r="18" spans="1:12" ht="15.75">
       <c r="A18" s="67"/>
       <c r="B18" s="24"/>
       <c r="C18" s="31" t="s">
@@ -2867,7 +2858,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" ht="15.6">
+    <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="67"/>
       <c r="B19" s="24"/>
       <c r="C19" s="31" t="s">
@@ -2885,7 +2876,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" ht="15.6">
+    <row r="20" spans="1:12" ht="15.75">
       <c r="A20" s="67"/>
       <c r="B20" s="24"/>
       <c r="C20" s="31" t="s">
@@ -2903,7 +2894,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" ht="15.6">
+    <row r="21" spans="1:12" ht="15.75">
       <c r="A21" s="67"/>
       <c r="B21" s="24"/>
       <c r="C21" s="31" t="s">
@@ -2921,7 +2912,7 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:12" ht="15.6">
+    <row r="22" spans="1:12" ht="15.75">
       <c r="A22" s="47"/>
       <c r="B22" s="49">
         <v>1.4</v>
@@ -2951,7 +2942,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12" ht="15.6">
+    <row r="23" spans="1:12" ht="15.75">
       <c r="A23" s="67"/>
       <c r="B23" s="24"/>
       <c r="C23" s="31" t="s">
@@ -2969,7 +2960,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" ht="15.6">
+    <row r="24" spans="1:12" ht="15.75">
       <c r="A24" s="67"/>
       <c r="B24" s="24"/>
       <c r="C24" s="31" t="s">
@@ -2987,7 +2978,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" ht="31.2">
+    <row r="25" spans="1:12" ht="31.5">
       <c r="A25" s="67"/>
       <c r="B25" s="24"/>
       <c r="C25" s="31" t="s">
@@ -3005,7 +2996,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:12" ht="15.6">
+    <row r="26" spans="1:12" ht="15.75">
       <c r="A26" s="67"/>
       <c r="B26" s="24"/>
       <c r="C26" s="31"/>
@@ -3019,7 +3010,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:12" ht="15.6">
+    <row r="27" spans="1:12" ht="15.75">
       <c r="A27" s="85"/>
       <c r="B27" s="86">
         <v>1.5</v>
@@ -3049,7 +3040,7 @@
       <c r="K27" s="56"/>
       <c r="L27" s="56"/>
     </row>
-    <row r="28" spans="1:12" ht="15.6">
+    <row r="28" spans="1:12" ht="15.75">
       <c r="A28" s="67"/>
       <c r="B28" s="24"/>
       <c r="C28" s="31"/>
@@ -3063,7 +3054,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" ht="18">
+    <row r="29" spans="1:12" ht="18.75">
       <c r="A29" s="66">
         <v>2</v>
       </c>
@@ -3081,7 +3072,7 @@
       <c r="K29" s="44"/>
       <c r="L29" s="44"/>
     </row>
-    <row r="30" spans="1:12" ht="15.6">
+    <row r="30" spans="1:12" ht="15.75">
       <c r="A30" s="47"/>
       <c r="B30" s="50">
         <v>2.1</v>
@@ -3109,7 +3100,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12" ht="15.6">
+    <row r="31" spans="1:12" ht="15.75">
       <c r="A31" s="67"/>
       <c r="B31" s="24"/>
       <c r="C31" s="11" t="s">
@@ -3129,7 +3120,7 @@
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
     </row>
-    <row r="32" spans="1:12" ht="46.8">
+    <row r="32" spans="1:12" ht="47.25">
       <c r="A32" s="67"/>
       <c r="B32" s="24"/>
       <c r="C32" s="11" t="s">
@@ -3149,7 +3140,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="1:12" ht="15.6">
+    <row r="33" spans="1:12" ht="15.75">
       <c r="A33" s="67"/>
       <c r="B33" s="24"/>
       <c r="C33" s="11" t="s">
@@ -3169,7 +3160,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="1:12" ht="15.6">
+    <row r="34" spans="1:12" ht="15.75">
       <c r="A34" s="67"/>
       <c r="B34" s="24"/>
       <c r="C34" s="11" t="s">
@@ -3189,7 +3180,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="1:12" ht="15.6">
+    <row r="35" spans="1:12" ht="15.75">
       <c r="A35" s="67"/>
       <c r="B35" s="24"/>
       <c r="C35" s="11" t="s">
@@ -3207,7 +3198,7 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="1:12" ht="15.6">
+    <row r="36" spans="1:12" ht="15.75">
       <c r="A36" s="67"/>
       <c r="B36" s="24"/>
       <c r="C36" s="11" t="s">
@@ -3227,7 +3218,7 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="1:12" ht="15.6">
+    <row r="37" spans="1:12" ht="15.75">
       <c r="A37" s="67"/>
       <c r="B37" s="24"/>
       <c r="C37" s="11"/>
@@ -3241,7 +3232,7 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="1:12" ht="15.6">
+    <row r="38" spans="1:12" ht="15.75">
       <c r="A38" s="85"/>
       <c r="B38" s="89" t="s">
         <v>70</v>
@@ -3271,7 +3262,7 @@
       <c r="K38" s="56"/>
       <c r="L38" s="56"/>
     </row>
-    <row r="39" spans="1:12" ht="15.6">
+    <row r="39" spans="1:12" ht="15.75">
       <c r="A39" s="67"/>
       <c r="B39" s="24"/>
       <c r="C39" s="31"/>
@@ -3285,7 +3276,7 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="1:12" ht="18">
+    <row r="40" spans="1:12" ht="18.75">
       <c r="A40" s="66">
         <v>3</v>
       </c>
@@ -3303,7 +3294,7 @@
       <c r="K40" s="44"/>
       <c r="L40" s="44"/>
     </row>
-    <row r="41" spans="1:12" ht="15.6">
+    <row r="41" spans="1:12" ht="15.75">
       <c r="A41" s="6"/>
       <c r="B41" s="49">
         <v>3.1</v>
@@ -3331,7 +3322,7 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="1:12" ht="15.6">
+    <row r="42" spans="1:12" ht="15.75">
       <c r="A42" s="67"/>
       <c r="B42" s="51"/>
       <c r="C42" s="11" t="s">
@@ -3349,7 +3340,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="1:12" ht="15.6">
+    <row r="43" spans="1:12" ht="15.75">
       <c r="A43" s="67"/>
       <c r="B43" s="24"/>
       <c r="C43" s="11" t="s">
@@ -3367,7 +3358,7 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="1:12" ht="15.6">
+    <row r="44" spans="1:12" ht="15.75">
       <c r="A44" s="67"/>
       <c r="B44" s="24"/>
       <c r="C44" s="11" t="s">
@@ -3385,7 +3376,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="1:12" ht="15.6">
+    <row r="45" spans="1:12" ht="15.75">
       <c r="A45" s="67"/>
       <c r="B45" s="24"/>
       <c r="C45" s="11"/>
@@ -3399,7 +3390,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="1:12" ht="15.6">
+    <row r="46" spans="1:12" ht="15.75">
       <c r="A46" s="67"/>
       <c r="B46" s="24"/>
       <c r="C46" s="105"/>
@@ -3413,7 +3404,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="1:12" ht="18">
+    <row r="47" spans="1:12" ht="18.75">
       <c r="A47" s="66">
         <v>4</v>
       </c>
@@ -3431,7 +3422,7 @@
       <c r="K47" s="44"/>
       <c r="L47" s="44"/>
     </row>
-    <row r="48" spans="1:12" ht="15.6">
+    <row r="48" spans="1:12" ht="15.75">
       <c r="A48" s="6"/>
       <c r="B48" s="49">
         <v>4.0999999999999996</v>
@@ -3461,7 +3452,7 @@
       </c>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:12" ht="15.6">
+    <row r="49" spans="1:12" ht="15.75">
       <c r="A49" s="67"/>
       <c r="B49" s="51"/>
       <c r="C49" s="11" t="s">
@@ -3479,7 +3470,7 @@
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:12" ht="15.6">
+    <row r="50" spans="1:12" ht="15.75">
       <c r="A50" s="67"/>
       <c r="B50" s="24"/>
       <c r="C50" s="11" t="s">
@@ -3497,7 +3488,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="1:12" ht="15.6">
+    <row r="51" spans="1:12" ht="15.75">
       <c r="A51" s="67"/>
       <c r="B51" s="24"/>
       <c r="C51" s="11" t="s">
@@ -3515,7 +3506,7 @@
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="1:12" ht="15.6">
+    <row r="52" spans="1:12" ht="15.75">
       <c r="A52" s="67"/>
       <c r="B52" s="24"/>
       <c r="C52" s="11" t="s">
@@ -3533,7 +3524,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="1:12" ht="15.6">
+    <row r="53" spans="1:12" ht="15.75">
       <c r="A53" s="67"/>
       <c r="B53" s="24"/>
       <c r="C53" s="11" t="s">
@@ -3551,7 +3542,7 @@
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="1:12" ht="15.6">
+    <row r="54" spans="1:12" ht="15.75">
       <c r="A54" s="67"/>
       <c r="B54" s="24"/>
       <c r="C54" s="11" t="s">
@@ -3569,7 +3560,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="1:12" ht="15.6">
+    <row r="55" spans="1:12" ht="15.75">
       <c r="A55" s="67"/>
       <c r="B55" s="24"/>
       <c r="C55" s="11"/>
@@ -3583,7 +3574,7 @@
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="1:12" ht="15.6">
+    <row r="56" spans="1:12" ht="15.75">
       <c r="A56" s="85"/>
       <c r="B56" s="89" t="s">
         <v>93</v>
@@ -3627,7 +3618,7 @@
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="1:12" ht="18">
+    <row r="58" spans="1:12" ht="18.75">
       <c r="A58" s="66">
         <v>5</v>
       </c>
@@ -3659,7 +3650,7 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="1:12" ht="15.6">
+    <row r="60" spans="1:12" ht="15.75">
       <c r="A60" s="69">
         <v>1</v>
       </c>
@@ -3689,7 +3680,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="15.6">
+    <row r="61" spans="1:12" ht="15.75">
       <c r="A61" s="67"/>
       <c r="B61" s="52">
         <v>1.1000000000000001</v>
@@ -3707,7 +3698,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="1:12" ht="15.6">
+    <row r="62" spans="1:12" ht="15.75">
       <c r="A62" s="67"/>
       <c r="B62" s="52">
         <v>1.2</v>
@@ -3725,7 +3716,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="1:12" ht="15.6">
+    <row r="63" spans="1:12" ht="15.75">
       <c r="A63" s="67"/>
       <c r="B63" s="52">
         <v>1.3</v>
@@ -3755,7 +3746,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="15.6">
+    <row r="64" spans="1:12" ht="15.75">
       <c r="A64" s="67"/>
       <c r="B64" s="52"/>
       <c r="C64" s="8" t="s">
@@ -3775,7 +3766,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="31.2">
+    <row r="65" spans="1:12" ht="31.5">
       <c r="A65" s="47"/>
       <c r="B65" s="52"/>
       <c r="C65" s="8" t="s">
@@ -3793,7 +3784,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" ht="15.6">
+    <row r="66" spans="1:12" ht="15.75">
       <c r="A66" s="67"/>
       <c r="B66" s="52"/>
       <c r="C66" s="8" t="s">
@@ -3811,7 +3802,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:12" ht="15.6">
+    <row r="67" spans="1:12" ht="15.75">
       <c r="A67" s="69">
         <v>2</v>
       </c>
@@ -3839,7 +3830,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" ht="15.6">
+    <row r="68" spans="1:12" ht="15.75">
       <c r="A68" s="70"/>
       <c r="B68" s="52">
         <v>2.1</v>
@@ -3857,7 +3848,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" ht="15.6">
+    <row r="69" spans="1:12" ht="15.75">
       <c r="A69" s="70"/>
       <c r="B69" s="52">
         <v>2.2000000000000002</v>
@@ -3875,7 +3866,7 @@
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:12" ht="15.6">
+    <row r="70" spans="1:12" ht="15.75">
       <c r="A70" s="70"/>
       <c r="B70" s="52">
         <v>2.2999999999999998</v>
@@ -3893,7 +3884,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" ht="15.6">
+    <row r="71" spans="1:12" ht="15.75">
       <c r="A71" s="70"/>
       <c r="B71" s="52"/>
       <c r="C71" s="8"/>
@@ -3907,7 +3898,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" ht="15.6">
+    <row r="72" spans="1:12" ht="15.75">
       <c r="A72" s="69">
         <v>3</v>
       </c>
@@ -3937,7 +3928,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" ht="15.6">
+    <row r="73" spans="1:12" ht="15.75">
       <c r="A73" s="70"/>
       <c r="B73" s="52">
         <v>3.1</v>
@@ -3955,7 +3946,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" ht="15.6">
+    <row r="74" spans="1:12" ht="15.75">
       <c r="A74" s="70"/>
       <c r="B74" s="52">
         <v>3.2</v>
@@ -3973,7 +3964,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" ht="15.6">
+    <row r="75" spans="1:12" ht="15.75">
       <c r="A75" s="70"/>
       <c r="B75" s="52">
         <v>3.3</v>
@@ -3991,7 +3982,7 @@
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" ht="15.6">
+    <row r="76" spans="1:12" ht="15.75">
       <c r="A76" s="70"/>
       <c r="B76" s="52">
         <v>3.4</v>
@@ -4009,7 +4000,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" ht="15.6">
+    <row r="77" spans="1:12" ht="15.75">
       <c r="A77" s="69">
         <v>4</v>
       </c>
@@ -4037,7 +4028,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" ht="15.6">
+    <row r="78" spans="1:12" ht="15.75">
       <c r="A78" s="70"/>
       <c r="B78" s="52">
         <v>4.0999999999999996</v>
@@ -4069,7 +4060,7 @@
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="1:12" ht="18">
+    <row r="80" spans="1:12" ht="18.75">
       <c r="A80" s="66">
         <v>5</v>
       </c>
@@ -4087,7 +4078,7 @@
       <c r="K80" s="44"/>
       <c r="L80" s="44"/>
     </row>
-    <row r="81" spans="1:12" ht="15.6">
+    <row r="81" spans="1:12" ht="15.75">
       <c r="A81" s="6"/>
       <c r="B81" s="49">
         <v>5.0999999999999996</v>
@@ -4115,7 +4106,7 @@
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" ht="15.6">
+    <row r="82" spans="1:12" ht="15.75">
       <c r="A82" s="67"/>
       <c r="B82" s="24"/>
       <c r="C82" s="11" t="s">
@@ -4133,7 +4124,7 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" ht="31.2">
+    <row r="83" spans="1:12" ht="31.5">
       <c r="A83" s="67"/>
       <c r="B83" s="24"/>
       <c r="C83" s="11" t="s">
@@ -4151,7 +4142,7 @@
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" ht="31.2">
+    <row r="84" spans="1:12" ht="31.5">
       <c r="A84" s="67"/>
       <c r="B84" s="24"/>
       <c r="C84" s="11" t="s">
@@ -4171,7 +4162,7 @@
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" ht="31.2">
+    <row r="85" spans="1:12" ht="31.5">
       <c r="A85" s="67"/>
       <c r="B85" s="24"/>
       <c r="C85" s="11" t="s">
@@ -4191,7 +4182,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" ht="31.2">
+    <row r="86" spans="1:12" ht="31.5">
       <c r="A86" s="47"/>
       <c r="B86" s="49">
         <v>5.2</v>
@@ -4221,7 +4212,7 @@
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="1:12" ht="15.6">
+    <row r="87" spans="1:12" ht="15.75">
       <c r="A87" s="67"/>
       <c r="B87" s="24"/>
       <c r="C87" s="11" t="s">
@@ -4239,7 +4230,7 @@
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="1:12" ht="15.6">
+    <row r="88" spans="1:12" ht="15.75">
       <c r="A88" s="67"/>
       <c r="B88" s="24"/>
       <c r="C88" s="11" t="s">
@@ -4257,7 +4248,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="1:12" ht="15.6">
+    <row r="89" spans="1:12" ht="15.75">
       <c r="A89" s="67"/>
       <c r="B89" s="24"/>
       <c r="C89" s="11" t="s">
@@ -4275,7 +4266,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="1:12" ht="15.6">
+    <row r="90" spans="1:12" ht="15.75">
       <c r="A90" s="67"/>
       <c r="B90" s="24"/>
       <c r="C90" s="11"/>
@@ -4289,7 +4280,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="1:12" ht="15.6">
+    <row r="91" spans="1:12" ht="15.75">
       <c r="A91" s="47"/>
       <c r="B91" s="49">
         <v>5.3</v>
@@ -4317,7 +4308,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:12" ht="15.6">
+    <row r="92" spans="1:12" ht="15.75">
       <c r="A92" s="67"/>
       <c r="B92" s="24"/>
       <c r="C92" s="11" t="s">
@@ -4335,7 +4326,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="1:12" ht="15.6">
+    <row r="93" spans="1:12" ht="15.75">
       <c r="A93" s="67"/>
       <c r="B93" s="24"/>
       <c r="C93" s="11" t="s">
@@ -4353,7 +4344,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
     </row>
-    <row r="94" spans="1:12" ht="15.6">
+    <row r="94" spans="1:12" ht="15.75">
       <c r="A94" s="67"/>
       <c r="B94" s="24"/>
       <c r="C94" s="11"/>
@@ -4367,7 +4358,7 @@
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
     </row>
-    <row r="95" spans="1:12" ht="31.2">
+    <row r="95" spans="1:12" ht="47.25">
       <c r="A95" s="67"/>
       <c r="B95" s="49">
         <v>5.4</v>
@@ -4397,7 +4388,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="28.8">
+    <row r="96" spans="1:12" ht="30">
       <c r="A96" s="47"/>
       <c r="B96" s="49">
         <v>5.5</v>
@@ -4417,7 +4408,7 @@
       <c r="K96" s="3"/>
       <c r="L96" s="3"/>
     </row>
-    <row r="97" spans="1:12" ht="15.6">
+    <row r="97" spans="1:12" ht="15.75">
       <c r="A97" s="47"/>
       <c r="B97" s="49">
         <v>5.6</v>
@@ -4435,7 +4426,7 @@
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
     </row>
-    <row r="98" spans="1:12" ht="15.6">
+    <row r="98" spans="1:12" ht="15.75">
       <c r="A98" s="47"/>
       <c r="B98" s="49">
         <v>5.7</v>
@@ -4469,7 +4460,7 @@
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
     </row>
-    <row r="100" spans="1:12" ht="15.6">
+    <row r="100" spans="1:12" ht="15.75">
       <c r="A100" s="6"/>
       <c r="B100" s="1">
         <v>5.8</v>
@@ -4501,7 +4492,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="15.6">
+    <row r="101" spans="1:12" ht="15.75">
       <c r="A101" s="67"/>
       <c r="B101" s="24"/>
       <c r="C101" s="11" t="s">
@@ -4521,7 +4512,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="15.6">
+    <row r="102" spans="1:12" ht="15.75">
       <c r="A102" s="67"/>
       <c r="B102" s="24"/>
       <c r="C102" s="11" t="s">
@@ -4539,7 +4530,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
     </row>
-    <row r="103" spans="1:12" ht="15.6">
+    <row r="103" spans="1:12" ht="15.75">
       <c r="A103" s="67"/>
       <c r="B103" s="24"/>
       <c r="C103" s="11" t="s">
@@ -4557,7 +4548,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
     </row>
-    <row r="104" spans="1:12" ht="31.2">
+    <row r="104" spans="1:12" ht="31.5">
       <c r="A104" s="67"/>
       <c r="B104" s="24"/>
       <c r="C104" s="11" t="s">
@@ -4575,7 +4566,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
     </row>
-    <row r="105" spans="1:12" ht="15.6">
+    <row r="105" spans="1:12" ht="15.75">
       <c r="A105" s="67"/>
       <c r="B105" s="24"/>
       <c r="C105" s="11" t="s">
@@ -4595,7 +4586,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
     </row>
-    <row r="106" spans="1:12" ht="15.6">
+    <row r="106" spans="1:12" ht="15.75">
       <c r="A106" s="67"/>
       <c r="B106" s="24"/>
       <c r="C106" s="11" t="s">
@@ -4613,7 +4604,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
     </row>
-    <row r="107" spans="1:12" ht="15.6">
+    <row r="107" spans="1:12" ht="15.75">
       <c r="A107" s="67"/>
       <c r="B107" s="24"/>
       <c r="C107" s="11"/>
@@ -4627,7 +4618,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="1:12" s="20" customFormat="1" ht="36">
+    <row r="108" spans="1:12" s="20" customFormat="1" ht="37.5">
       <c r="A108" s="71">
         <v>6</v>
       </c>
@@ -4741,18 +4732,18 @@
       <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" style="29" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" style="29" customWidth="1"/>
-    <col min="3" max="3" width="65.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" style="29" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="29" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="89.109375" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" style="29" customWidth="1"/>
+    <col min="3" max="3" width="65.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" style="29" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="29" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="89.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="29" customFormat="1">
@@ -4787,7 +4778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="43.2">
+    <row r="2" spans="1:10" ht="45">
       <c r="A2" s="28" t="s">
         <v>160</v>
       </c>
@@ -6192,17 +6183,17 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="29"/>
-    <col min="2" max="2" width="25.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="29"/>
+    <col min="2" max="2" width="25.28515625" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="29"/>
-    <col min="5" max="5" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" style="29" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="29"/>
+    <col min="5" max="5" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="29" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="29" customFormat="1">
@@ -6759,19 +6750,19 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="29"/>
-    <col min="2" max="2" width="40.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="29"/>
+    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="29" customFormat="1">
@@ -7412,21 +7403,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3782443B-979F-4126-A9F9-516CD045F0D0}">
   <dimension ref="A1:L114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="P75" sqref="P75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="29"/>
-    <col min="4" max="4" width="66.88671875" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" style="29" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" style="29" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="29"/>
+    <col min="4" max="4" width="66.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" style="29" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" style="29" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" customHeight="1">
@@ -7445,7 +7436,7 @@
       <c r="K1" s="111"/>
       <c r="L1" s="111"/>
     </row>
-    <row r="2" spans="1:12" ht="18">
+    <row r="2" spans="1:12" ht="18.75">
       <c r="A2" s="112" t="s">
         <v>422</v>
       </c>
@@ -7475,7 +7466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6">
+    <row r="3" spans="1:12" ht="15.75">
       <c r="A3" s="23"/>
       <c r="B3" s="16"/>
       <c r="C3" s="15"/>
@@ -7491,7 +7482,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="15.6">
+    <row r="4" spans="1:12" ht="15.75">
       <c r="A4" s="76">
         <v>1</v>
       </c>
@@ -7511,7 +7502,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="15.6">
+    <row r="5" spans="1:12" ht="15.75">
       <c r="A5" s="78"/>
       <c r="B5" s="18">
         <v>1.1000000000000001</v>
@@ -7531,7 +7522,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="15.6">
+    <row r="6" spans="1:12" ht="15.75">
       <c r="A6" s="78"/>
       <c r="B6" s="18">
         <v>1.2</v>
@@ -7551,7 +7542,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="15.6">
+    <row r="7" spans="1:12" ht="15.75">
       <c r="A7" s="78"/>
       <c r="B7" s="18">
         <v>1.3</v>
@@ -7571,7 +7562,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15.6">
+    <row r="8" spans="1:12" ht="15.75">
       <c r="A8" s="78"/>
       <c r="B8" s="18"/>
       <c r="C8" s="19" t="s">
@@ -7589,7 +7580,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="15.6">
+    <row r="9" spans="1:12" ht="15.75">
       <c r="A9" s="78"/>
       <c r="B9" s="18"/>
       <c r="C9" s="19" t="s">
@@ -7613,7 +7604,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15.6">
+    <row r="10" spans="1:12" ht="15.75">
       <c r="A10" s="78"/>
       <c r="B10" s="18"/>
       <c r="C10" s="19" t="s">
@@ -7631,7 +7622,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15.6">
+    <row r="11" spans="1:12" ht="15.75">
       <c r="A11" s="78"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19" t="s">
@@ -7649,7 +7640,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15.6">
+    <row r="12" spans="1:12" ht="15.75">
       <c r="A12" s="78"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19" t="s">
@@ -7667,7 +7658,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15.6">
+    <row r="13" spans="1:12" ht="15.75">
       <c r="A13" s="78"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19" t="s">
@@ -7685,7 +7676,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15.6">
+    <row r="14" spans="1:12" ht="15.75">
       <c r="A14" s="78"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
@@ -7699,7 +7690,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="15.6">
+    <row r="15" spans="1:12" ht="15.75">
       <c r="A15" s="76">
         <v>2</v>
       </c>
@@ -7723,7 +7714,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15.6">
+    <row r="16" spans="1:12" ht="15.75">
       <c r="A16" s="78"/>
       <c r="B16" s="18">
         <v>2.1</v>
@@ -7747,7 +7738,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" ht="15.6">
+    <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="78"/>
       <c r="B17" s="18">
         <v>2.2000000000000002</v>
@@ -7771,7 +7762,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" ht="15.6">
+    <row r="18" spans="1:12" ht="15.75">
       <c r="A18" s="78"/>
       <c r="B18" s="18">
         <v>2.2999999999999998</v>
@@ -7797,7 +7788,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" ht="15.6">
+    <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="78"/>
       <c r="B19" s="18">
         <v>2.4</v>
@@ -7823,7 +7814,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" ht="15.6">
+    <row r="20" spans="1:12" ht="15.75">
       <c r="A20" s="78"/>
       <c r="B20" s="18">
         <v>2.5</v>
@@ -7843,7 +7834,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" ht="15.6">
+    <row r="21" spans="1:12" ht="15.75">
       <c r="A21" s="78"/>
       <c r="B21" s="18"/>
       <c r="C21" s="19" t="s">
@@ -7865,7 +7856,7 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:12" ht="15.6">
+    <row r="22" spans="1:12" ht="15.75">
       <c r="A22" s="78"/>
       <c r="B22" s="18"/>
       <c r="C22" s="19" t="s">
@@ -7887,7 +7878,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12" ht="15.6">
+    <row r="23" spans="1:12" ht="15.75">
       <c r="A23" s="78"/>
       <c r="B23" s="18"/>
       <c r="C23" s="19" t="s">
@@ -7909,7 +7900,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" ht="15.6">
+    <row r="24" spans="1:12" ht="15.75">
       <c r="A24" s="78"/>
       <c r="B24" s="18">
         <v>2.6</v>
@@ -7933,7 +7924,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" ht="15.6">
+    <row r="25" spans="1:12" ht="15.75">
       <c r="A25" s="78"/>
       <c r="B25" s="18">
         <v>2.7</v>
@@ -7957,7 +7948,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:12" ht="15.6">
+    <row r="26" spans="1:12" ht="15.75">
       <c r="A26" s="78"/>
       <c r="B26" s="18">
         <v>2.8</v>
@@ -7981,7 +7972,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:12" ht="15.6">
+    <row r="27" spans="1:12" ht="15.75">
       <c r="A27" s="78"/>
       <c r="B27" s="18">
         <v>2.9</v>
@@ -8003,7 +7994,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="1:12" ht="15.6">
+    <row r="28" spans="1:12" ht="15.75">
       <c r="A28" s="78"/>
       <c r="B28" s="18">
         <v>2.1</v>
@@ -8027,7 +8018,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" ht="15.6">
+    <row r="29" spans="1:12" ht="15.75">
       <c r="A29" s="78"/>
       <c r="B29" s="18"/>
       <c r="C29" s="19"/>
@@ -8047,7 +8038,7 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="1:12" ht="15.6">
+    <row r="30" spans="1:12" ht="15.75">
       <c r="A30" s="78"/>
       <c r="B30" s="18"/>
       <c r="C30" s="17"/>
@@ -8061,7 +8052,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12" ht="31.2">
+    <row r="31" spans="1:12" ht="31.5">
       <c r="A31" s="82"/>
       <c r="B31" s="79"/>
       <c r="C31" s="84" t="s">
@@ -8085,7 +8076,7 @@
       <c r="K31" s="56"/>
       <c r="L31" s="56"/>
     </row>
-    <row r="32" spans="1:12" ht="15.6">
+    <row r="32" spans="1:12" ht="15.75">
       <c r="A32" s="76"/>
       <c r="B32" s="16"/>
       <c r="C32" s="15"/>
@@ -8101,7 +8092,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="1:12" ht="15.6">
+    <row r="33" spans="1:12" ht="15.75">
       <c r="A33" s="78"/>
       <c r="B33" s="18"/>
       <c r="C33" s="19"/>
@@ -8115,7 +8106,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="1:12" ht="15.6">
+    <row r="34" spans="1:12" ht="15.75">
       <c r="A34" s="78"/>
       <c r="B34" s="18"/>
       <c r="C34" s="19"/>
@@ -8131,7 +8122,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="1:12" ht="15.6">
+    <row r="35" spans="1:12" ht="15.75">
       <c r="A35" s="76">
         <v>3</v>
       </c>
@@ -8151,7 +8142,7 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="1:12" ht="15.6">
+    <row r="36" spans="1:12" ht="15.75">
       <c r="A36" s="78"/>
       <c r="B36" s="18">
         <v>3.1</v>
@@ -8177,7 +8168,7 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="1:12" ht="15.6">
+    <row r="37" spans="1:12" ht="15.75">
       <c r="A37" s="78"/>
       <c r="B37" s="18">
         <v>3.2</v>
@@ -8197,7 +8188,7 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="1:12" ht="15.6">
+    <row r="38" spans="1:12" ht="15.75">
       <c r="A38" s="78"/>
       <c r="B38" s="18">
         <v>3.3</v>
@@ -8217,7 +8208,7 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="1:12" ht="15.6">
+    <row r="39" spans="1:12" ht="15.75">
       <c r="A39" s="78"/>
       <c r="B39" s="18">
         <v>3.4</v>
@@ -8237,7 +8228,7 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="1:12" ht="15.6">
+    <row r="40" spans="1:12" ht="15.75">
       <c r="A40" s="78"/>
       <c r="B40" s="18">
         <v>3.5</v>
@@ -8257,7 +8248,7 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="1:12" ht="15.6">
+    <row r="41" spans="1:12" ht="15.75">
       <c r="A41" s="78"/>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
@@ -8271,7 +8262,7 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="1:12" ht="15.6">
+    <row r="42" spans="1:12" ht="15.75">
       <c r="A42" s="78"/>
       <c r="B42" s="18"/>
       <c r="C42" s="19"/>
@@ -8285,7 +8276,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="1:12" ht="15.6">
+    <row r="43" spans="1:12" ht="15.75">
       <c r="A43" s="76">
         <v>4</v>
       </c>
@@ -8305,7 +8296,7 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="1:12" ht="15.6">
+    <row r="44" spans="1:12" ht="15.75">
       <c r="A44" s="78"/>
       <c r="B44" s="18">
         <v>4.0999999999999996</v>
@@ -8329,7 +8320,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="1:12" ht="15.6">
+    <row r="45" spans="1:12" ht="15.75">
       <c r="A45" s="78"/>
       <c r="B45" s="18"/>
       <c r="C45" s="19" t="s">
@@ -8347,7 +8338,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="1:12" ht="15.6">
+    <row r="46" spans="1:12" ht="15.75">
       <c r="A46" s="78"/>
       <c r="B46" s="18"/>
       <c r="C46" s="19" t="s">
@@ -8365,7 +8356,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="1:12" ht="15.6">
+    <row r="47" spans="1:12" ht="15.75">
       <c r="A47" s="78"/>
       <c r="B47" s="18">
         <v>4.2</v>
@@ -8389,7 +8380,7 @@
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="1:12" ht="15.6">
+    <row r="48" spans="1:12" ht="15.75">
       <c r="A48" s="78"/>
       <c r="B48" s="18"/>
       <c r="C48" s="19" t="s">
@@ -8407,7 +8398,7 @@
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:12" ht="15.6">
+    <row r="49" spans="1:12" ht="15.75">
       <c r="A49" s="78"/>
       <c r="B49" s="18"/>
       <c r="C49" s="19" t="s">
@@ -8425,7 +8416,7 @@
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:12" ht="15.6">
+    <row r="50" spans="1:12" ht="15.75">
       <c r="A50" s="78"/>
       <c r="B50" s="18"/>
       <c r="C50" s="19" t="s">
@@ -8443,7 +8434,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="1:12" ht="15.6">
+    <row r="51" spans="1:12" ht="15.75">
       <c r="A51" s="78"/>
       <c r="B51" s="18">
         <v>4.3</v>
@@ -8469,7 +8460,7 @@
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="1:12" ht="15.6">
+    <row r="52" spans="1:12" ht="15.75">
       <c r="A52" s="78"/>
       <c r="B52" s="18"/>
       <c r="C52" s="19" t="s">
@@ -8487,7 +8478,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="1:12" ht="15.6">
+    <row r="53" spans="1:12" ht="15.75">
       <c r="A53" s="78"/>
       <c r="B53" s="18"/>
       <c r="C53" s="19" t="s">
@@ -8505,7 +8496,7 @@
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="1:12" ht="15.6">
+    <row r="54" spans="1:12" ht="15.75">
       <c r="A54" s="78"/>
       <c r="B54" s="18"/>
       <c r="C54" s="19" t="s">
@@ -8523,7 +8514,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="1:12" ht="15.6">
+    <row r="55" spans="1:12" ht="15.75">
       <c r="A55" s="78"/>
       <c r="B55" s="18"/>
       <c r="C55" s="19" t="s">
@@ -8541,7 +8532,7 @@
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="1:12" ht="15.6">
+    <row r="56" spans="1:12" ht="15.75">
       <c r="A56" s="78"/>
       <c r="B56" s="18"/>
       <c r="C56" s="19" t="s">
@@ -8559,7 +8550,7 @@
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
     </row>
-    <row r="57" spans="1:12" ht="15.6">
+    <row r="57" spans="1:12" ht="15.75">
       <c r="A57" s="78"/>
       <c r="B57" s="18"/>
       <c r="C57" s="19" t="s">
@@ -8577,7 +8568,7 @@
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="1:12" ht="15.6">
+    <row r="58" spans="1:12" ht="15.75">
       <c r="A58" s="78"/>
       <c r="B58" s="18"/>
       <c r="C58" s="19" t="s">
@@ -8595,7 +8586,7 @@
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="1:12" ht="15.6">
+    <row r="59" spans="1:12" ht="15.75">
       <c r="A59" s="78"/>
       <c r="B59" s="18">
         <v>4.4000000000000004</v>
@@ -8621,7 +8612,7 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="1:12" ht="15.6">
+    <row r="60" spans="1:12" ht="15.75">
       <c r="A60" s="78"/>
       <c r="B60" s="18"/>
       <c r="C60" s="19" t="s">
@@ -8639,7 +8630,7 @@
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="1:12" ht="15.6">
+    <row r="61" spans="1:12" ht="15.75">
       <c r="A61" s="78"/>
       <c r="B61" s="18">
         <v>4.5</v>
@@ -8665,7 +8656,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="1:12" ht="15.6">
+    <row r="62" spans="1:12" ht="15.75">
       <c r="A62" s="78"/>
       <c r="B62" s="18"/>
       <c r="C62" s="19" t="s">
@@ -8683,7 +8674,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="1:12" ht="15.6">
+    <row r="63" spans="1:12" ht="15.75">
       <c r="A63" s="78"/>
       <c r="B63" s="18"/>
       <c r="C63" s="19" t="s">
@@ -8701,7 +8692,7 @@
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="1:12" ht="15.6">
+    <row r="64" spans="1:12" ht="15.75">
       <c r="A64" s="78"/>
       <c r="B64" s="18">
         <v>4.5999999999999996</v>
@@ -8714,14 +8705,20 @@
       <c r="F64" s="78">
         <v>2</v>
       </c>
-      <c r="G64" s="78"/>
-      <c r="H64" s="78"/>
-      <c r="I64" s="78"/>
+      <c r="G64" s="78">
+        <v>1.5</v>
+      </c>
+      <c r="H64" s="101">
+        <v>45714</v>
+      </c>
+      <c r="I64" s="78" t="s">
+        <v>433</v>
+      </c>
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="1:12" ht="15.6">
+    <row r="65" spans="1:12" ht="15.75">
       <c r="A65" s="78"/>
       <c r="B65" s="18"/>
       <c r="C65" s="19" t="s">
@@ -8739,7 +8736,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" ht="15.6">
+    <row r="66" spans="1:12" ht="15.75">
       <c r="A66" s="78"/>
       <c r="B66" s="18">
         <v>4.7</v>
@@ -8752,14 +8749,20 @@
       <c r="F66" s="78">
         <v>2</v>
       </c>
-      <c r="G66" s="78"/>
-      <c r="H66" s="78"/>
-      <c r="I66" s="78"/>
+      <c r="G66" s="78">
+        <v>1.5</v>
+      </c>
+      <c r="H66" s="101">
+        <v>45714</v>
+      </c>
+      <c r="I66" s="78" t="s">
+        <v>433</v>
+      </c>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:12" ht="15.6">
+    <row r="67" spans="1:12" ht="15.75">
       <c r="A67" s="78"/>
       <c r="B67" s="18"/>
       <c r="C67" s="19" t="s">
@@ -8777,7 +8780,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" ht="15.6">
+    <row r="68" spans="1:12" ht="15.75">
       <c r="A68" s="78"/>
       <c r="B68" s="18"/>
       <c r="C68" s="19" t="s">
@@ -8795,7 +8798,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" ht="15.6">
+    <row r="69" spans="1:12" ht="15.75">
       <c r="A69" s="78"/>
       <c r="B69" s="18">
         <v>4.8</v>
@@ -8808,14 +8811,20 @@
       <c r="F69" s="78">
         <v>10</v>
       </c>
-      <c r="G69" s="78"/>
-      <c r="H69" s="78"/>
-      <c r="I69" s="78"/>
+      <c r="G69" s="78">
+        <v>6</v>
+      </c>
+      <c r="H69" s="101">
+        <v>45715</v>
+      </c>
+      <c r="I69" s="78" t="s">
+        <v>433</v>
+      </c>
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:12" ht="15.6">
+    <row r="70" spans="1:12" ht="15.75">
       <c r="A70" s="78"/>
       <c r="B70" s="18"/>
       <c r="C70" s="19" t="s">
@@ -8833,7 +8842,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" ht="15.6">
+    <row r="71" spans="1:12" ht="15.75">
       <c r="A71" s="78"/>
       <c r="B71" s="18"/>
       <c r="C71" s="19" t="s">
@@ -8851,7 +8860,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" ht="15.6">
+    <row r="72" spans="1:12" ht="15.75">
       <c r="A72" s="78"/>
       <c r="B72" s="18"/>
       <c r="C72" s="19" t="s">
@@ -8869,7 +8878,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" ht="15.6">
+    <row r="73" spans="1:12" ht="15.75">
       <c r="A73" s="78"/>
       <c r="B73" s="18"/>
       <c r="C73" s="19" t="s">
@@ -8887,7 +8896,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" ht="15.6">
+    <row r="74" spans="1:12" ht="15.75">
       <c r="A74" s="78"/>
       <c r="B74" s="18"/>
       <c r="C74" s="19" t="s">
@@ -8905,7 +8914,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" ht="15.6">
+    <row r="75" spans="1:12" ht="15.75">
       <c r="A75" s="78"/>
       <c r="B75" s="18">
         <v>4.9000000000000004</v>
@@ -8918,14 +8927,20 @@
       <c r="F75" s="78">
         <v>2</v>
       </c>
-      <c r="G75" s="78"/>
-      <c r="H75" s="78"/>
-      <c r="I75" s="78"/>
+      <c r="G75" s="78">
+        <v>2</v>
+      </c>
+      <c r="H75" s="101">
+        <v>45715</v>
+      </c>
+      <c r="I75" s="78" t="s">
+        <v>433</v>
+      </c>
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" ht="15.6">
+    <row r="76" spans="1:12" ht="15.75">
       <c r="A76" s="78"/>
       <c r="B76" s="18">
         <v>4.0999999999999996</v>
@@ -8945,7 +8960,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" ht="15.6">
+    <row r="77" spans="1:12" ht="15.75">
       <c r="A77" s="78"/>
       <c r="B77" s="18"/>
       <c r="C77" s="19" t="s">
@@ -8963,7 +8978,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" ht="15.6">
+    <row r="78" spans="1:12" ht="15.75">
       <c r="A78" s="78"/>
       <c r="B78" s="18">
         <v>4.1100000000000003</v>
@@ -8983,7 +8998,7 @@
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
     </row>
-    <row r="79" spans="1:12" ht="15.6">
+    <row r="79" spans="1:12" ht="15.75">
       <c r="A79" s="78"/>
       <c r="B79" s="18"/>
       <c r="C79" s="19" t="s">
@@ -9001,7 +9016,7 @@
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="1:12" ht="15.6">
+    <row r="80" spans="1:12" ht="15.75">
       <c r="A80" s="78"/>
       <c r="B80" s="18"/>
       <c r="C80" s="19" t="s">
@@ -9019,7 +9034,7 @@
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
     </row>
-    <row r="81" spans="1:12" ht="15.6">
+    <row r="81" spans="1:12" ht="15.75">
       <c r="A81" s="78"/>
       <c r="B81" s="18"/>
       <c r="C81" s="19" t="s">
@@ -9037,7 +9052,7 @@
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" ht="15.6">
+    <row r="82" spans="1:12" ht="15.75">
       <c r="A82" s="78"/>
       <c r="B82" s="18"/>
       <c r="C82" s="19" t="s">
@@ -9055,7 +9070,7 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" ht="15.6">
+    <row r="83" spans="1:12" ht="15.75">
       <c r="A83" s="78"/>
       <c r="B83" s="18">
         <v>4.12</v>
@@ -9075,7 +9090,7 @@
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" ht="15.6">
+    <row r="84" spans="1:12" ht="15.75">
       <c r="A84" s="78"/>
       <c r="B84" s="18"/>
       <c r="C84" s="19" t="s">
@@ -9093,7 +9108,7 @@
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" ht="15.6">
+    <row r="85" spans="1:12" ht="15.75">
       <c r="A85" s="78"/>
       <c r="B85" s="18"/>
       <c r="C85" s="19" t="s">
@@ -9111,7 +9126,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" ht="15.6">
+    <row r="86" spans="1:12" ht="15.75">
       <c r="A86" s="78"/>
       <c r="B86" s="18"/>
       <c r="C86" s="19" t="s">
@@ -9129,7 +9144,7 @@
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="1:12" ht="15.6">
+    <row r="87" spans="1:12" ht="15.75">
       <c r="A87" s="78"/>
       <c r="B87" s="18">
         <v>4.13</v>
@@ -9149,7 +9164,7 @@
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="1:12" ht="15.6">
+    <row r="88" spans="1:12" ht="15.75">
       <c r="A88" s="78"/>
       <c r="B88" s="18"/>
       <c r="C88" s="19" t="s">
@@ -9167,7 +9182,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="1:12" ht="15.6">
+    <row r="89" spans="1:12" ht="15.75">
       <c r="A89" s="78"/>
       <c r="B89" s="18">
         <v>4.1399999999999997</v>
@@ -9187,7 +9202,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="1:12" ht="15.6">
+    <row r="90" spans="1:12" ht="15.75">
       <c r="A90" s="78"/>
       <c r="B90" s="18">
         <v>4.1500000000000004</v>
@@ -9207,7 +9222,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="1:12" ht="15.6">
+    <row r="91" spans="1:12" ht="15.75">
       <c r="A91" s="78"/>
       <c r="B91" s="18"/>
       <c r="C91" s="19" t="s">
@@ -9225,7 +9240,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:12" ht="15.6">
+    <row r="92" spans="1:12" ht="15.75">
       <c r="A92" s="78"/>
       <c r="B92" s="18"/>
       <c r="C92" s="19" t="s">
@@ -9243,7 +9258,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="1:12" ht="15.6">
+    <row r="93" spans="1:12" ht="15.75">
       <c r="A93" s="78"/>
       <c r="B93" s="18"/>
       <c r="C93" s="19"/>
@@ -9261,7 +9276,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
     </row>
-    <row r="94" spans="1:12" ht="15.6">
+    <row r="94" spans="1:12" ht="15.75">
       <c r="A94" s="78"/>
       <c r="B94" s="17"/>
       <c r="C94" s="17"/>
@@ -9275,7 +9290,7 @@
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
     </row>
-    <row r="95" spans="1:12" ht="15.6">
+    <row r="95" spans="1:12" ht="15.75">
       <c r="A95" s="82"/>
       <c r="B95" s="79"/>
       <c r="C95" s="81" t="s">
@@ -9295,7 +9310,7 @@
       <c r="K95" s="56"/>
       <c r="L95" s="56"/>
     </row>
-    <row r="96" spans="1:12" ht="15.6">
+    <row r="96" spans="1:12" ht="15.75">
       <c r="A96" s="82"/>
       <c r="B96" s="79"/>
       <c r="C96" s="81"/>
@@ -9323,7 +9338,7 @@
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
     </row>
-    <row r="98" spans="1:12" ht="15.6">
+    <row r="98" spans="1:12" ht="15.75">
       <c r="A98" s="76">
         <v>5</v>
       </c>
@@ -9343,7 +9358,7 @@
       <c r="K98" s="3"/>
       <c r="L98" s="3"/>
     </row>
-    <row r="99" spans="1:12" ht="15.6">
+    <row r="99" spans="1:12" ht="15.75">
       <c r="A99" s="78"/>
       <c r="B99" s="18">
         <v>5.0999999999999996</v>
@@ -9363,7 +9378,7 @@
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
     </row>
-    <row r="100" spans="1:12" ht="15.6">
+    <row r="100" spans="1:12" ht="15.75">
       <c r="A100" s="78"/>
       <c r="B100" s="18">
         <v>5.2</v>
@@ -9383,7 +9398,7 @@
       <c r="K100" s="3"/>
       <c r="L100" s="3"/>
     </row>
-    <row r="101" spans="1:12" ht="15.6">
+    <row r="101" spans="1:12" ht="15.75">
       <c r="A101" s="78"/>
       <c r="B101" s="18">
         <v>5.3</v>
@@ -9403,7 +9418,7 @@
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
     </row>
-    <row r="102" spans="1:12" ht="15.6">
+    <row r="102" spans="1:12" ht="15.75">
       <c r="A102" s="78"/>
       <c r="B102" s="18"/>
       <c r="C102" s="19"/>
@@ -9417,7 +9432,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
     </row>
-    <row r="103" spans="1:12" ht="15.6">
+    <row r="103" spans="1:12" ht="15.75">
       <c r="A103" s="76">
         <v>6</v>
       </c>
@@ -9439,7 +9454,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
     </row>
-    <row r="104" spans="1:12" ht="15.6">
+    <row r="104" spans="1:12" ht="15.75">
       <c r="A104" s="78"/>
       <c r="B104" s="18">
         <v>6.1</v>
@@ -9457,7 +9472,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
     </row>
-    <row r="105" spans="1:12" ht="15.6">
+    <row r="105" spans="1:12" ht="15.75">
       <c r="A105" s="78"/>
       <c r="B105" s="18">
         <v>6.2</v>
@@ -9475,7 +9490,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
     </row>
-    <row r="106" spans="1:12" ht="15.6">
+    <row r="106" spans="1:12" ht="15.75">
       <c r="A106" s="78"/>
       <c r="B106" s="18">
         <v>6.3</v>
@@ -9493,7 +9508,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
     </row>
-    <row r="107" spans="1:12" ht="15.6">
+    <row r="107" spans="1:12" ht="15.75">
       <c r="A107" s="78"/>
       <c r="B107" s="18">
         <v>6.4</v>
@@ -9511,7 +9526,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="1:12" ht="15.6">
+    <row r="108" spans="1:12" ht="15.75">
       <c r="A108" s="78"/>
       <c r="B108" s="18">
         <v>6.5</v>
@@ -9529,7 +9544,7 @@
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
     </row>
-    <row r="109" spans="1:12" ht="15.6">
+    <row r="109" spans="1:12" ht="15.75">
       <c r="A109" s="78"/>
       <c r="B109" s="18">
         <v>6.6</v>
@@ -9547,7 +9562,7 @@
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
     </row>
-    <row r="110" spans="1:12" ht="15.6">
+    <row r="110" spans="1:12" ht="15.75">
       <c r="A110" s="78"/>
       <c r="B110" s="18"/>
       <c r="C110" s="19"/>
@@ -9561,7 +9576,7 @@
       <c r="K110" s="3"/>
       <c r="L110" s="3"/>
     </row>
-    <row r="111" spans="1:12" ht="93.6">
+    <row r="111" spans="1:12" ht="94.5">
       <c r="A111" s="82"/>
       <c r="B111" s="79"/>
       <c r="C111" s="81" t="s">
@@ -9618,7 +9633,7 @@
       <c r="K113" s="32"/>
       <c r="L113" s="32"/>
     </row>
-    <row r="114" spans="1:12" ht="15.6">
+    <row r="114" spans="1:12" ht="15.75">
       <c r="D114" s="22" t="s">
         <v>378</v>
       </c>

</xml_diff>

<commit_message>
DevExtreme editiors final demo modifications
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\officeWork\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93473A6E-7BD8-4D31-8AF6-7BC0781F6D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FB52A4-EB0B-4C10-B913-03CA956A70E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="4" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
   <sheets>
     <sheet name=" Basic GUI" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="483">
   <si>
     <t>Topic</t>
   </si>
@@ -1487,12 +1496,6 @@
   </si>
   <si>
     <t>https://docs.servicestack.net/ormlite/apis/select</t>
-  </si>
-  <si>
-    <t>check</t>
-  </si>
-  <si>
-    <t>error</t>
   </si>
 </sst>
 </file>
@@ -2475,20 +2478,20 @@
       <selection activeCell="J95" sqref="J95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="72" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="72" customWidth="1"/>
     <col min="2" max="2" width="6" style="29" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" customWidth="1"/>
     <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="5" width="53.42578125" customWidth="1"/>
-    <col min="6" max="9" width="9.28515625" style="29" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="51.42578125" customWidth="1"/>
+    <col min="5" max="5" width="53.44140625" customWidth="1"/>
+    <col min="6" max="9" width="9.33203125" style="29" customWidth="1"/>
+    <col min="10" max="10" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="51.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="40" customFormat="1" ht="18.75">
+    <row r="1" spans="1:12" s="40" customFormat="1" ht="18">
       <c r="A1" s="106" t="s">
         <v>0</v>
       </c>
@@ -2514,7 +2517,7 @@
       <c r="K1" s="41"/>
       <c r="L1" s="41"/>
     </row>
-    <row r="2" spans="1:12" s="29" customFormat="1" ht="18.75">
+    <row r="2" spans="1:12" s="29" customFormat="1" ht="18">
       <c r="A2" s="66">
         <v>1</v>
       </c>
@@ -2538,7 +2541,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75">
+    <row r="3" spans="1:12" ht="15.6">
       <c r="A3" s="47"/>
       <c r="B3" s="46">
         <v>1.1000000000000001</v>
@@ -2566,7 +2569,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="31.5">
+    <row r="4" spans="1:12" ht="31.2">
       <c r="A4" s="67"/>
       <c r="B4" s="24"/>
       <c r="C4" s="31" t="s">
@@ -2586,7 +2589,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75">
+    <row r="5" spans="1:12" ht="15.6">
       <c r="A5" s="67"/>
       <c r="B5" s="24"/>
       <c r="C5" s="31" t="s">
@@ -2604,7 +2607,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75">
+    <row r="6" spans="1:12" ht="15.6">
       <c r="A6" s="67"/>
       <c r="B6" s="24"/>
       <c r="C6" s="31" t="s">
@@ -2622,7 +2625,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75">
+    <row r="7" spans="1:12" ht="15.6">
       <c r="A7" s="47"/>
       <c r="B7" s="49">
         <v>1.2</v>
@@ -2650,7 +2653,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75">
+    <row r="8" spans="1:12" ht="15.6">
       <c r="A8" s="67"/>
       <c r="B8" s="24"/>
       <c r="C8" s="31" t="s">
@@ -2668,7 +2671,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75">
+    <row r="9" spans="1:12" ht="15.6">
       <c r="A9" s="67"/>
       <c r="B9" s="24"/>
       <c r="C9" s="31" t="s">
@@ -2686,7 +2689,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75">
+    <row r="10" spans="1:12" ht="15.6">
       <c r="A10" s="67"/>
       <c r="B10" s="24"/>
       <c r="C10" s="31" t="s">
@@ -2704,7 +2707,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75">
+    <row r="11" spans="1:12" ht="15.6">
       <c r="A11" s="67"/>
       <c r="B11" s="24"/>
       <c r="C11" s="31" t="s">
@@ -2722,7 +2725,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75">
+    <row r="12" spans="1:12" ht="15.6">
       <c r="A12" s="67"/>
       <c r="B12" s="24"/>
       <c r="C12" s="31" t="s">
@@ -2740,7 +2743,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75">
+    <row r="13" spans="1:12" ht="15.6">
       <c r="A13" s="67"/>
       <c r="B13" s="24"/>
       <c r="C13" s="31" t="s">
@@ -2758,7 +2761,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75">
+    <row r="14" spans="1:12" ht="15.6">
       <c r="A14" s="67"/>
       <c r="B14" s="24"/>
       <c r="C14" s="31" t="s">
@@ -2776,7 +2779,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75">
+    <row r="15" spans="1:12" ht="15.6">
       <c r="A15" s="67"/>
       <c r="B15" s="24"/>
       <c r="C15" s="31" t="s">
@@ -2794,7 +2797,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75">
+    <row r="16" spans="1:12" ht="15.6">
       <c r="A16" s="67"/>
       <c r="B16" s="24"/>
       <c r="C16" s="31" t="s">
@@ -2812,7 +2815,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75">
+    <row r="17" spans="1:12" ht="15.6">
       <c r="A17" s="47"/>
       <c r="B17" s="49">
         <v>1.3</v>
@@ -2840,7 +2843,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75">
+    <row r="18" spans="1:12" ht="15.6">
       <c r="A18" s="67"/>
       <c r="B18" s="24"/>
       <c r="C18" s="31" t="s">
@@ -2858,7 +2861,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75">
+    <row r="19" spans="1:12" ht="15.6">
       <c r="A19" s="67"/>
       <c r="B19" s="24"/>
       <c r="C19" s="31" t="s">
@@ -2876,7 +2879,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" ht="15.75">
+    <row r="20" spans="1:12" ht="15.6">
       <c r="A20" s="67"/>
       <c r="B20" s="24"/>
       <c r="C20" s="31" t="s">
@@ -2894,7 +2897,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75">
+    <row r="21" spans="1:12" ht="15.6">
       <c r="A21" s="67"/>
       <c r="B21" s="24"/>
       <c r="C21" s="31" t="s">
@@ -2912,7 +2915,7 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75">
+    <row r="22" spans="1:12" ht="15.6">
       <c r="A22" s="47"/>
       <c r="B22" s="49">
         <v>1.4</v>
@@ -2942,7 +2945,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75">
+    <row r="23" spans="1:12" ht="15.6">
       <c r="A23" s="67"/>
       <c r="B23" s="24"/>
       <c r="C23" s="31" t="s">
@@ -2960,7 +2963,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75">
+    <row r="24" spans="1:12" ht="15.6">
       <c r="A24" s="67"/>
       <c r="B24" s="24"/>
       <c r="C24" s="31" t="s">
@@ -2978,7 +2981,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" ht="31.5">
+    <row r="25" spans="1:12" ht="31.2">
       <c r="A25" s="67"/>
       <c r="B25" s="24"/>
       <c r="C25" s="31" t="s">
@@ -2996,7 +2999,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:12" ht="15.75">
+    <row r="26" spans="1:12" ht="15.6">
       <c r="A26" s="67"/>
       <c r="B26" s="24"/>
       <c r="C26" s="31"/>
@@ -3010,7 +3013,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:12" ht="15.75">
+    <row r="27" spans="1:12" ht="15.6">
       <c r="A27" s="85"/>
       <c r="B27" s="86">
         <v>1.5</v>
@@ -3040,7 +3043,7 @@
       <c r="K27" s="56"/>
       <c r="L27" s="56"/>
     </row>
-    <row r="28" spans="1:12" ht="15.75">
+    <row r="28" spans="1:12" ht="15.6">
       <c r="A28" s="67"/>
       <c r="B28" s="24"/>
       <c r="C28" s="31"/>
@@ -3054,7 +3057,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" ht="18.75">
+    <row r="29" spans="1:12" ht="18">
       <c r="A29" s="66">
         <v>2</v>
       </c>
@@ -3072,7 +3075,7 @@
       <c r="K29" s="44"/>
       <c r="L29" s="44"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75">
+    <row r="30" spans="1:12" ht="15.6">
       <c r="A30" s="47"/>
       <c r="B30" s="50">
         <v>2.1</v>
@@ -3100,7 +3103,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12" ht="15.75">
+    <row r="31" spans="1:12" ht="15.6">
       <c r="A31" s="67"/>
       <c r="B31" s="24"/>
       <c r="C31" s="11" t="s">
@@ -3120,7 +3123,7 @@
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
     </row>
-    <row r="32" spans="1:12" ht="47.25">
+    <row r="32" spans="1:12" ht="46.8">
       <c r="A32" s="67"/>
       <c r="B32" s="24"/>
       <c r="C32" s="11" t="s">
@@ -3140,7 +3143,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="1:12" ht="15.75">
+    <row r="33" spans="1:12" ht="15.6">
       <c r="A33" s="67"/>
       <c r="B33" s="24"/>
       <c r="C33" s="11" t="s">
@@ -3160,7 +3163,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="1:12" ht="15.75">
+    <row r="34" spans="1:12" ht="15.6">
       <c r="A34" s="67"/>
       <c r="B34" s="24"/>
       <c r="C34" s="11" t="s">
@@ -3180,7 +3183,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="1:12" ht="15.75">
+    <row r="35" spans="1:12" ht="15.6">
       <c r="A35" s="67"/>
       <c r="B35" s="24"/>
       <c r="C35" s="11" t="s">
@@ -3198,7 +3201,7 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="1:12" ht="15.75">
+    <row r="36" spans="1:12" ht="15.6">
       <c r="A36" s="67"/>
       <c r="B36" s="24"/>
       <c r="C36" s="11" t="s">
@@ -3218,7 +3221,7 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="1:12" ht="15.75">
+    <row r="37" spans="1:12" ht="15.6">
       <c r="A37" s="67"/>
       <c r="B37" s="24"/>
       <c r="C37" s="11"/>
@@ -3232,7 +3235,7 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="1:12" ht="15.75">
+    <row r="38" spans="1:12" ht="15.6">
       <c r="A38" s="85"/>
       <c r="B38" s="89" t="s">
         <v>70</v>
@@ -3262,7 +3265,7 @@
       <c r="K38" s="56"/>
       <c r="L38" s="56"/>
     </row>
-    <row r="39" spans="1:12" ht="15.75">
+    <row r="39" spans="1:12" ht="15.6">
       <c r="A39" s="67"/>
       <c r="B39" s="24"/>
       <c r="C39" s="31"/>
@@ -3276,7 +3279,7 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="1:12" ht="18.75">
+    <row r="40" spans="1:12" ht="18">
       <c r="A40" s="66">
         <v>3</v>
       </c>
@@ -3294,7 +3297,7 @@
       <c r="K40" s="44"/>
       <c r="L40" s="44"/>
     </row>
-    <row r="41" spans="1:12" ht="15.75">
+    <row r="41" spans="1:12" ht="15.6">
       <c r="A41" s="6"/>
       <c r="B41" s="49">
         <v>3.1</v>
@@ -3322,7 +3325,7 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="1:12" ht="15.75">
+    <row r="42" spans="1:12" ht="15.6">
       <c r="A42" s="67"/>
       <c r="B42" s="51"/>
       <c r="C42" s="11" t="s">
@@ -3340,7 +3343,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="1:12" ht="15.75">
+    <row r="43" spans="1:12" ht="15.6">
       <c r="A43" s="67"/>
       <c r="B43" s="24"/>
       <c r="C43" s="11" t="s">
@@ -3358,7 +3361,7 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="1:12" ht="15.75">
+    <row r="44" spans="1:12" ht="15.6">
       <c r="A44" s="67"/>
       <c r="B44" s="24"/>
       <c r="C44" s="11" t="s">
@@ -3376,7 +3379,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="1:12" ht="15.75">
+    <row r="45" spans="1:12" ht="15.6">
       <c r="A45" s="67"/>
       <c r="B45" s="24"/>
       <c r="C45" s="11"/>
@@ -3390,7 +3393,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="1:12" ht="15.75">
+    <row r="46" spans="1:12" ht="15.6">
       <c r="A46" s="67"/>
       <c r="B46" s="24"/>
       <c r="C46" s="105"/>
@@ -3404,7 +3407,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="1:12" ht="18.75">
+    <row r="47" spans="1:12" ht="18">
       <c r="A47" s="66">
         <v>4</v>
       </c>
@@ -3422,7 +3425,7 @@
       <c r="K47" s="44"/>
       <c r="L47" s="44"/>
     </row>
-    <row r="48" spans="1:12" ht="15.75">
+    <row r="48" spans="1:12" ht="15.6">
       <c r="A48" s="6"/>
       <c r="B48" s="49">
         <v>4.0999999999999996</v>
@@ -3452,7 +3455,7 @@
       </c>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:12" ht="15.75">
+    <row r="49" spans="1:12" ht="15.6">
       <c r="A49" s="67"/>
       <c r="B49" s="51"/>
       <c r="C49" s="11" t="s">
@@ -3470,7 +3473,7 @@
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:12" ht="15.75">
+    <row r="50" spans="1:12" ht="15.6">
       <c r="A50" s="67"/>
       <c r="B50" s="24"/>
       <c r="C50" s="11" t="s">
@@ -3488,7 +3491,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="1:12" ht="15.75">
+    <row r="51" spans="1:12" ht="15.6">
       <c r="A51" s="67"/>
       <c r="B51" s="24"/>
       <c r="C51" s="11" t="s">
@@ -3506,7 +3509,7 @@
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="1:12" ht="15.75">
+    <row r="52" spans="1:12" ht="15.6">
       <c r="A52" s="67"/>
       <c r="B52" s="24"/>
       <c r="C52" s="11" t="s">
@@ -3524,7 +3527,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="1:12" ht="15.75">
+    <row r="53" spans="1:12" ht="15.6">
       <c r="A53" s="67"/>
       <c r="B53" s="24"/>
       <c r="C53" s="11" t="s">
@@ -3542,7 +3545,7 @@
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="1:12" ht="15.75">
+    <row r="54" spans="1:12" ht="15.6">
       <c r="A54" s="67"/>
       <c r="B54" s="24"/>
       <c r="C54" s="11" t="s">
@@ -3560,7 +3563,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="1:12" ht="15.75">
+    <row r="55" spans="1:12" ht="15.6">
       <c r="A55" s="67"/>
       <c r="B55" s="24"/>
       <c r="C55" s="11"/>
@@ -3574,7 +3577,7 @@
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="1:12" ht="15.75">
+    <row r="56" spans="1:12" ht="15.6">
       <c r="A56" s="85"/>
       <c r="B56" s="89" t="s">
         <v>93</v>
@@ -3618,7 +3621,7 @@
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="1:12" ht="18.75">
+    <row r="58" spans="1:12" ht="18">
       <c r="A58" s="66">
         <v>5</v>
       </c>
@@ -3650,7 +3653,7 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="1:12" ht="15.75">
+    <row r="60" spans="1:12" ht="15.6">
       <c r="A60" s="69">
         <v>1</v>
       </c>
@@ -3680,7 +3683,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="15.75">
+    <row r="61" spans="1:12" ht="15.6">
       <c r="A61" s="67"/>
       <c r="B61" s="52">
         <v>1.1000000000000001</v>
@@ -3698,7 +3701,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="1:12" ht="15.75">
+    <row r="62" spans="1:12" ht="15.6">
       <c r="A62" s="67"/>
       <c r="B62" s="52">
         <v>1.2</v>
@@ -3716,7 +3719,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="1:12" ht="15.75">
+    <row r="63" spans="1:12" ht="15.6">
       <c r="A63" s="67"/>
       <c r="B63" s="52">
         <v>1.3</v>
@@ -3746,7 +3749,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="15.75">
+    <row r="64" spans="1:12" ht="15.6">
       <c r="A64" s="67"/>
       <c r="B64" s="52"/>
       <c r="C64" s="8" t="s">
@@ -3766,7 +3769,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="31.5">
+    <row r="65" spans="1:12" ht="31.2">
       <c r="A65" s="47"/>
       <c r="B65" s="52"/>
       <c r="C65" s="8" t="s">
@@ -3784,7 +3787,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75">
+    <row r="66" spans="1:12" ht="15.6">
       <c r="A66" s="67"/>
       <c r="B66" s="52"/>
       <c r="C66" s="8" t="s">
@@ -3802,7 +3805,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75">
+    <row r="67" spans="1:12" ht="15.6">
       <c r="A67" s="69">
         <v>2</v>
       </c>
@@ -3830,7 +3833,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75">
+    <row r="68" spans="1:12" ht="15.6">
       <c r="A68" s="70"/>
       <c r="B68" s="52">
         <v>2.1</v>
@@ -3848,7 +3851,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75">
+    <row r="69" spans="1:12" ht="15.6">
       <c r="A69" s="70"/>
       <c r="B69" s="52">
         <v>2.2000000000000002</v>
@@ -3866,7 +3869,7 @@
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75">
+    <row r="70" spans="1:12" ht="15.6">
       <c r="A70" s="70"/>
       <c r="B70" s="52">
         <v>2.2999999999999998</v>
@@ -3884,7 +3887,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75">
+    <row r="71" spans="1:12" ht="15.6">
       <c r="A71" s="70"/>
       <c r="B71" s="52"/>
       <c r="C71" s="8"/>
@@ -3898,7 +3901,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75">
+    <row r="72" spans="1:12" ht="15.6">
       <c r="A72" s="69">
         <v>3</v>
       </c>
@@ -3928,7 +3931,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75">
+    <row r="73" spans="1:12" ht="15.6">
       <c r="A73" s="70"/>
       <c r="B73" s="52">
         <v>3.1</v>
@@ -3946,7 +3949,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75">
+    <row r="74" spans="1:12" ht="15.6">
       <c r="A74" s="70"/>
       <c r="B74" s="52">
         <v>3.2</v>
@@ -3964,7 +3967,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75">
+    <row r="75" spans="1:12" ht="15.6">
       <c r="A75" s="70"/>
       <c r="B75" s="52">
         <v>3.3</v>
@@ -3982,7 +3985,7 @@
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75">
+    <row r="76" spans="1:12" ht="15.6">
       <c r="A76" s="70"/>
       <c r="B76" s="52">
         <v>3.4</v>
@@ -4000,7 +4003,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75">
+    <row r="77" spans="1:12" ht="15.6">
       <c r="A77" s="69">
         <v>4</v>
       </c>
@@ -4028,7 +4031,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75">
+    <row r="78" spans="1:12" ht="15.6">
       <c r="A78" s="70"/>
       <c r="B78" s="52">
         <v>4.0999999999999996</v>
@@ -4060,7 +4063,7 @@
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="1:12" ht="18.75">
+    <row r="80" spans="1:12" ht="18">
       <c r="A80" s="66">
         <v>5</v>
       </c>
@@ -4078,7 +4081,7 @@
       <c r="K80" s="44"/>
       <c r="L80" s="44"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75">
+    <row r="81" spans="1:12" ht="15.6">
       <c r="A81" s="6"/>
       <c r="B81" s="49">
         <v>5.0999999999999996</v>
@@ -4106,7 +4109,7 @@
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75">
+    <row r="82" spans="1:12" ht="15.6">
       <c r="A82" s="67"/>
       <c r="B82" s="24"/>
       <c r="C82" s="11" t="s">
@@ -4124,7 +4127,7 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" ht="31.5">
+    <row r="83" spans="1:12" ht="31.2">
       <c r="A83" s="67"/>
       <c r="B83" s="24"/>
       <c r="C83" s="11" t="s">
@@ -4142,7 +4145,7 @@
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" ht="31.5">
+    <row r="84" spans="1:12" ht="31.2">
       <c r="A84" s="67"/>
       <c r="B84" s="24"/>
       <c r="C84" s="11" t="s">
@@ -4162,7 +4165,7 @@
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" ht="31.5">
+    <row r="85" spans="1:12" ht="31.2">
       <c r="A85" s="67"/>
       <c r="B85" s="24"/>
       <c r="C85" s="11" t="s">
@@ -4182,7 +4185,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" ht="31.5">
+    <row r="86" spans="1:12" ht="31.2">
       <c r="A86" s="47"/>
       <c r="B86" s="49">
         <v>5.2</v>
@@ -4212,7 +4215,7 @@
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75">
+    <row r="87" spans="1:12" ht="15.6">
       <c r="A87" s="67"/>
       <c r="B87" s="24"/>
       <c r="C87" s="11" t="s">
@@ -4230,7 +4233,7 @@
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75">
+    <row r="88" spans="1:12" ht="15.6">
       <c r="A88" s="67"/>
       <c r="B88" s="24"/>
       <c r="C88" s="11" t="s">
@@ -4248,7 +4251,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75">
+    <row r="89" spans="1:12" ht="15.6">
       <c r="A89" s="67"/>
       <c r="B89" s="24"/>
       <c r="C89" s="11" t="s">
@@ -4266,7 +4269,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75">
+    <row r="90" spans="1:12" ht="15.6">
       <c r="A90" s="67"/>
       <c r="B90" s="24"/>
       <c r="C90" s="11"/>
@@ -4280,7 +4283,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75">
+    <row r="91" spans="1:12" ht="15.6">
       <c r="A91" s="47"/>
       <c r="B91" s="49">
         <v>5.3</v>
@@ -4308,7 +4311,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75">
+    <row r="92" spans="1:12" ht="15.6">
       <c r="A92" s="67"/>
       <c r="B92" s="24"/>
       <c r="C92" s="11" t="s">
@@ -4326,7 +4329,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75">
+    <row r="93" spans="1:12" ht="15.6">
       <c r="A93" s="67"/>
       <c r="B93" s="24"/>
       <c r="C93" s="11" t="s">
@@ -4344,7 +4347,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75">
+    <row r="94" spans="1:12" ht="15.6">
       <c r="A94" s="67"/>
       <c r="B94" s="24"/>
       <c r="C94" s="11"/>
@@ -4358,7 +4361,7 @@
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
     </row>
-    <row r="95" spans="1:12" ht="47.25">
+    <row r="95" spans="1:12" ht="31.2">
       <c r="A95" s="67"/>
       <c r="B95" s="49">
         <v>5.4</v>
@@ -4388,7 +4391,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="30">
+    <row r="96" spans="1:12" ht="28.8">
       <c r="A96" s="47"/>
       <c r="B96" s="49">
         <v>5.5</v>
@@ -4408,7 +4411,7 @@
       <c r="K96" s="3"/>
       <c r="L96" s="3"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75">
+    <row r="97" spans="1:12" ht="15.6">
       <c r="A97" s="47"/>
       <c r="B97" s="49">
         <v>5.6</v>
@@ -4426,7 +4429,7 @@
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75">
+    <row r="98" spans="1:12" ht="15.6">
       <c r="A98" s="47"/>
       <c r="B98" s="49">
         <v>5.7</v>
@@ -4460,7 +4463,7 @@
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75">
+    <row r="100" spans="1:12" ht="15.6">
       <c r="A100" s="6"/>
       <c r="B100" s="1">
         <v>5.8</v>
@@ -4492,7 +4495,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="15.75">
+    <row r="101" spans="1:12" ht="15.6">
       <c r="A101" s="67"/>
       <c r="B101" s="24"/>
       <c r="C101" s="11" t="s">
@@ -4512,7 +4515,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="15.75">
+    <row r="102" spans="1:12" ht="15.6">
       <c r="A102" s="67"/>
       <c r="B102" s="24"/>
       <c r="C102" s="11" t="s">
@@ -4530,7 +4533,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75">
+    <row r="103" spans="1:12" ht="15.6">
       <c r="A103" s="67"/>
       <c r="B103" s="24"/>
       <c r="C103" s="11" t="s">
@@ -4548,7 +4551,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
     </row>
-    <row r="104" spans="1:12" ht="31.5">
+    <row r="104" spans="1:12" ht="31.2">
       <c r="A104" s="67"/>
       <c r="B104" s="24"/>
       <c r="C104" s="11" t="s">
@@ -4566,7 +4569,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75">
+    <row r="105" spans="1:12" ht="15.6">
       <c r="A105" s="67"/>
       <c r="B105" s="24"/>
       <c r="C105" s="11" t="s">
@@ -4586,7 +4589,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75">
+    <row r="106" spans="1:12" ht="15.6">
       <c r="A106" s="67"/>
       <c r="B106" s="24"/>
       <c r="C106" s="11" t="s">
@@ -4604,7 +4607,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75">
+    <row r="107" spans="1:12" ht="15.6">
       <c r="A107" s="67"/>
       <c r="B107" s="24"/>
       <c r="C107" s="11"/>
@@ -4618,7 +4621,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="1:12" s="20" customFormat="1" ht="37.5">
+    <row r="108" spans="1:12" s="20" customFormat="1" ht="36">
       <c r="A108" s="71">
         <v>6</v>
       </c>
@@ -4732,18 +4735,18 @@
       <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9" style="29" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" style="29" customWidth="1"/>
-    <col min="3" max="3" width="65.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" style="29" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="29" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="89.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" style="29" customWidth="1"/>
+    <col min="3" max="3" width="65.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" style="29" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="29" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="89.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="29" customFormat="1">
@@ -4778,7 +4781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="45">
+    <row r="2" spans="1:10" ht="43.2">
       <c r="A2" s="28" t="s">
         <v>160</v>
       </c>
@@ -6183,17 +6186,17 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="29"/>
-    <col min="2" max="2" width="25.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="29"/>
+    <col min="2" max="2" width="25.33203125" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="29"/>
-    <col min="5" max="5" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="29" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="29"/>
+    <col min="5" max="5" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" style="29" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="29" customFormat="1">
@@ -6750,19 +6753,19 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="29"/>
-    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="29"/>
+    <col min="2" max="2" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" style="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="29" customFormat="1">
@@ -7403,21 +7406,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3782443B-979F-4126-A9F9-516CD045F0D0}">
   <dimension ref="A1:L114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="P75" sqref="P75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="29"/>
-    <col min="4" max="4" width="66.85546875" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" style="29" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" style="29" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="29"/>
+    <col min="4" max="4" width="66.88671875" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" style="29" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" style="29" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" customHeight="1">
@@ -7436,7 +7439,7 @@
       <c r="K1" s="111"/>
       <c r="L1" s="111"/>
     </row>
-    <row r="2" spans="1:12" ht="18.75">
+    <row r="2" spans="1:12" ht="18">
       <c r="A2" s="112" t="s">
         <v>422</v>
       </c>
@@ -7466,7 +7469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75">
+    <row r="3" spans="1:12" ht="15.6">
       <c r="A3" s="23"/>
       <c r="B3" s="16"/>
       <c r="C3" s="15"/>
@@ -7482,7 +7485,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75">
+    <row r="4" spans="1:12" ht="15.6">
       <c r="A4" s="76">
         <v>1</v>
       </c>
@@ -7502,7 +7505,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75">
+    <row r="5" spans="1:12" ht="15.6">
       <c r="A5" s="78"/>
       <c r="B5" s="18">
         <v>1.1000000000000001</v>
@@ -7522,7 +7525,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75">
+    <row r="6" spans="1:12" ht="15.6">
       <c r="A6" s="78"/>
       <c r="B6" s="18">
         <v>1.2</v>
@@ -7542,7 +7545,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75">
+    <row r="7" spans="1:12" ht="15.6">
       <c r="A7" s="78"/>
       <c r="B7" s="18">
         <v>1.3</v>
@@ -7562,7 +7565,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75">
+    <row r="8" spans="1:12" ht="15.6">
       <c r="A8" s="78"/>
       <c r="B8" s="18"/>
       <c r="C8" s="19" t="s">
@@ -7580,7 +7583,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75">
+    <row r="9" spans="1:12" ht="15.6">
       <c r="A9" s="78"/>
       <c r="B9" s="18"/>
       <c r="C9" s="19" t="s">
@@ -7604,7 +7607,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75">
+    <row r="10" spans="1:12" ht="15.6">
       <c r="A10" s="78"/>
       <c r="B10" s="18"/>
       <c r="C10" s="19" t="s">
@@ -7622,7 +7625,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75">
+    <row r="11" spans="1:12" ht="15.6">
       <c r="A11" s="78"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19" t="s">
@@ -7640,7 +7643,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75">
+    <row r="12" spans="1:12" ht="15.6">
       <c r="A12" s="78"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19" t="s">
@@ -7658,7 +7661,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75">
+    <row r="13" spans="1:12" ht="15.6">
       <c r="A13" s="78"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19" t="s">
@@ -7676,7 +7679,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75">
+    <row r="14" spans="1:12" ht="15.6">
       <c r="A14" s="78"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
@@ -7690,7 +7693,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75">
+    <row r="15" spans="1:12" ht="15.6">
       <c r="A15" s="76">
         <v>2</v>
       </c>
@@ -7714,7 +7717,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75">
+    <row r="16" spans="1:12" ht="15.6">
       <c r="A16" s="78"/>
       <c r="B16" s="18">
         <v>2.1</v>
@@ -7738,7 +7741,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75">
+    <row r="17" spans="1:12" ht="15.6">
       <c r="A17" s="78"/>
       <c r="B17" s="18">
         <v>2.2000000000000002</v>
@@ -7762,14 +7765,12 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75">
+    <row r="18" spans="1:12" ht="15.6">
       <c r="A18" s="78"/>
       <c r="B18" s="18">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C18" s="99" t="s">
-        <v>483</v>
-      </c>
+      <c r="C18" s="99"/>
       <c r="D18" s="18" t="s">
         <v>294</v>
       </c>
@@ -7788,14 +7789,12 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75">
+    <row r="19" spans="1:12" ht="15.6">
       <c r="A19" s="78"/>
       <c r="B19" s="18">
         <v>2.4</v>
       </c>
-      <c r="C19" s="99" t="s">
-        <v>483</v>
-      </c>
+      <c r="C19" s="99"/>
       <c r="D19" s="18" t="s">
         <v>295</v>
       </c>
@@ -7814,7 +7813,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" ht="15.75">
+    <row r="20" spans="1:12" ht="15.6">
       <c r="A20" s="78"/>
       <c r="B20" s="18">
         <v>2.5</v>
@@ -7834,7 +7833,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75">
+    <row r="21" spans="1:12" ht="15.6">
       <c r="A21" s="78"/>
       <c r="B21" s="18"/>
       <c r="C21" s="19" t="s">
@@ -7856,7 +7855,7 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75">
+    <row r="22" spans="1:12" ht="15.6">
       <c r="A22" s="78"/>
       <c r="B22" s="18"/>
       <c r="C22" s="19" t="s">
@@ -7878,7 +7877,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75">
+    <row r="23" spans="1:12" ht="15.6">
       <c r="A23" s="78"/>
       <c r="B23" s="18"/>
       <c r="C23" s="19" t="s">
@@ -7900,7 +7899,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75">
+    <row r="24" spans="1:12" ht="15.6">
       <c r="A24" s="78"/>
       <c r="B24" s="18">
         <v>2.6</v>
@@ -7924,7 +7923,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" ht="15.75">
+    <row r="25" spans="1:12" ht="15.6">
       <c r="A25" s="78"/>
       <c r="B25" s="18">
         <v>2.7</v>
@@ -7948,14 +7947,12 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:12" ht="15.75">
+    <row r="26" spans="1:12" ht="15.6">
       <c r="A26" s="78"/>
       <c r="B26" s="18">
         <v>2.8</v>
       </c>
-      <c r="C26" s="99" t="s">
-        <v>484</v>
-      </c>
+      <c r="C26" s="99"/>
       <c r="D26" s="18" t="s">
         <v>305</v>
       </c>
@@ -7972,7 +7969,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:12" ht="15.75">
+    <row r="27" spans="1:12" ht="15.6">
       <c r="A27" s="78"/>
       <c r="B27" s="18">
         <v>2.9</v>
@@ -7994,7 +7991,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="1:12" ht="15.75">
+    <row r="28" spans="1:12" ht="15.6">
       <c r="A28" s="78"/>
       <c r="B28" s="18">
         <v>2.1</v>
@@ -8018,7 +8015,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" ht="15.75">
+    <row r="29" spans="1:12" ht="15.6">
       <c r="A29" s="78"/>
       <c r="B29" s="18"/>
       <c r="C29" s="19"/>
@@ -8038,7 +8035,7 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75">
+    <row r="30" spans="1:12" ht="15.6">
       <c r="A30" s="78"/>
       <c r="B30" s="18"/>
       <c r="C30" s="17"/>
@@ -8052,7 +8049,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12" ht="31.5">
+    <row r="31" spans="1:12" ht="31.2">
       <c r="A31" s="82"/>
       <c r="B31" s="79"/>
       <c r="C31" s="84" t="s">
@@ -8076,7 +8073,7 @@
       <c r="K31" s="56"/>
       <c r="L31" s="56"/>
     </row>
-    <row r="32" spans="1:12" ht="15.75">
+    <row r="32" spans="1:12" ht="15.6">
       <c r="A32" s="76"/>
       <c r="B32" s="16"/>
       <c r="C32" s="15"/>
@@ -8092,7 +8089,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="1:12" ht="15.75">
+    <row r="33" spans="1:12" ht="15.6">
       <c r="A33" s="78"/>
       <c r="B33" s="18"/>
       <c r="C33" s="19"/>
@@ -8106,7 +8103,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="1:12" ht="15.75">
+    <row r="34" spans="1:12" ht="15.6">
       <c r="A34" s="78"/>
       <c r="B34" s="18"/>
       <c r="C34" s="19"/>
@@ -8122,7 +8119,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="1:12" ht="15.75">
+    <row r="35" spans="1:12" ht="15.6">
       <c r="A35" s="76">
         <v>3</v>
       </c>
@@ -8142,7 +8139,7 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="1:12" ht="15.75">
+    <row r="36" spans="1:12" ht="15.6">
       <c r="A36" s="78"/>
       <c r="B36" s="18">
         <v>3.1</v>
@@ -8168,7 +8165,7 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="1:12" ht="15.75">
+    <row r="37" spans="1:12" ht="15.6">
       <c r="A37" s="78"/>
       <c r="B37" s="18">
         <v>3.2</v>
@@ -8188,7 +8185,7 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="1:12" ht="15.75">
+    <row r="38" spans="1:12" ht="15.6">
       <c r="A38" s="78"/>
       <c r="B38" s="18">
         <v>3.3</v>
@@ -8208,7 +8205,7 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="1:12" ht="15.75">
+    <row r="39" spans="1:12" ht="15.6">
       <c r="A39" s="78"/>
       <c r="B39" s="18">
         <v>3.4</v>
@@ -8228,7 +8225,7 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="1:12" ht="15.75">
+    <row r="40" spans="1:12" ht="15.6">
       <c r="A40" s="78"/>
       <c r="B40" s="18">
         <v>3.5</v>
@@ -8248,7 +8245,7 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="1:12" ht="15.75">
+    <row r="41" spans="1:12" ht="15.6">
       <c r="A41" s="78"/>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
@@ -8262,7 +8259,7 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="1:12" ht="15.75">
+    <row r="42" spans="1:12" ht="15.6">
       <c r="A42" s="78"/>
       <c r="B42" s="18"/>
       <c r="C42" s="19"/>
@@ -8276,7 +8273,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="1:12" ht="15.75">
+    <row r="43" spans="1:12" ht="15.6">
       <c r="A43" s="76">
         <v>4</v>
       </c>
@@ -8296,7 +8293,7 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="1:12" ht="15.75">
+    <row r="44" spans="1:12" ht="15.6">
       <c r="A44" s="78"/>
       <c r="B44" s="18">
         <v>4.0999999999999996</v>
@@ -8320,7 +8317,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="1:12" ht="15.75">
+    <row r="45" spans="1:12" ht="15.6">
       <c r="A45" s="78"/>
       <c r="B45" s="18"/>
       <c r="C45" s="19" t="s">
@@ -8338,7 +8335,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="1:12" ht="15.75">
+    <row r="46" spans="1:12" ht="15.6">
       <c r="A46" s="78"/>
       <c r="B46" s="18"/>
       <c r="C46" s="19" t="s">
@@ -8356,7 +8353,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="1:12" ht="15.75">
+    <row r="47" spans="1:12" ht="15.6">
       <c r="A47" s="78"/>
       <c r="B47" s="18">
         <v>4.2</v>
@@ -8380,7 +8377,7 @@
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="1:12" ht="15.75">
+    <row r="48" spans="1:12" ht="15.6">
       <c r="A48" s="78"/>
       <c r="B48" s="18"/>
       <c r="C48" s="19" t="s">
@@ -8398,7 +8395,7 @@
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:12" ht="15.75">
+    <row r="49" spans="1:12" ht="15.6">
       <c r="A49" s="78"/>
       <c r="B49" s="18"/>
       <c r="C49" s="19" t="s">
@@ -8416,7 +8413,7 @@
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:12" ht="15.75">
+    <row r="50" spans="1:12" ht="15.6">
       <c r="A50" s="78"/>
       <c r="B50" s="18"/>
       <c r="C50" s="19" t="s">
@@ -8434,7 +8431,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="1:12" ht="15.75">
+    <row r="51" spans="1:12" ht="15.6">
       <c r="A51" s="78"/>
       <c r="B51" s="18">
         <v>4.3</v>
@@ -8460,7 +8457,7 @@
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="1:12" ht="15.75">
+    <row r="52" spans="1:12" ht="15.6">
       <c r="A52" s="78"/>
       <c r="B52" s="18"/>
       <c r="C52" s="19" t="s">
@@ -8478,7 +8475,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="1:12" ht="15.75">
+    <row r="53" spans="1:12" ht="15.6">
       <c r="A53" s="78"/>
       <c r="B53" s="18"/>
       <c r="C53" s="19" t="s">
@@ -8496,7 +8493,7 @@
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="1:12" ht="15.75">
+    <row r="54" spans="1:12" ht="15.6">
       <c r="A54" s="78"/>
       <c r="B54" s="18"/>
       <c r="C54" s="19" t="s">
@@ -8514,7 +8511,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="1:12" ht="15.75">
+    <row r="55" spans="1:12" ht="15.6">
       <c r="A55" s="78"/>
       <c r="B55" s="18"/>
       <c r="C55" s="19" t="s">
@@ -8532,7 +8529,7 @@
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="1:12" ht="15.75">
+    <row r="56" spans="1:12" ht="15.6">
       <c r="A56" s="78"/>
       <c r="B56" s="18"/>
       <c r="C56" s="19" t="s">
@@ -8550,7 +8547,7 @@
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
     </row>
-    <row r="57" spans="1:12" ht="15.75">
+    <row r="57" spans="1:12" ht="15.6">
       <c r="A57" s="78"/>
       <c r="B57" s="18"/>
       <c r="C57" s="19" t="s">
@@ -8568,7 +8565,7 @@
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="1:12" ht="15.75">
+    <row r="58" spans="1:12" ht="15.6">
       <c r="A58" s="78"/>
       <c r="B58" s="18"/>
       <c r="C58" s="19" t="s">
@@ -8586,7 +8583,7 @@
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="1:12" ht="15.75">
+    <row r="59" spans="1:12" ht="15.6">
       <c r="A59" s="78"/>
       <c r="B59" s="18">
         <v>4.4000000000000004</v>
@@ -8612,7 +8609,7 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="1:12" ht="15.75">
+    <row r="60" spans="1:12" ht="15.6">
       <c r="A60" s="78"/>
       <c r="B60" s="18"/>
       <c r="C60" s="19" t="s">
@@ -8630,7 +8627,7 @@
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="1:12" ht="15.75">
+    <row r="61" spans="1:12" ht="15.6">
       <c r="A61" s="78"/>
       <c r="B61" s="18">
         <v>4.5</v>
@@ -8656,7 +8653,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="1:12" ht="15.75">
+    <row r="62" spans="1:12" ht="15.6">
       <c r="A62" s="78"/>
       <c r="B62" s="18"/>
       <c r="C62" s="19" t="s">
@@ -8674,7 +8671,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="1:12" ht="15.75">
+    <row r="63" spans="1:12" ht="15.6">
       <c r="A63" s="78"/>
       <c r="B63" s="18"/>
       <c r="C63" s="19" t="s">
@@ -8692,7 +8689,7 @@
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="1:12" ht="15.75">
+    <row r="64" spans="1:12" ht="15.6">
       <c r="A64" s="78"/>
       <c r="B64" s="18">
         <v>4.5999999999999996</v>
@@ -8718,7 +8715,7 @@
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75">
+    <row r="65" spans="1:12" ht="15.6">
       <c r="A65" s="78"/>
       <c r="B65" s="18"/>
       <c r="C65" s="19" t="s">
@@ -8736,7 +8733,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75">
+    <row r="66" spans="1:12" ht="15.6">
       <c r="A66" s="78"/>
       <c r="B66" s="18">
         <v>4.7</v>
@@ -8762,7 +8759,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75">
+    <row r="67" spans="1:12" ht="15.6">
       <c r="A67" s="78"/>
       <c r="B67" s="18"/>
       <c r="C67" s="19" t="s">
@@ -8780,7 +8777,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75">
+    <row r="68" spans="1:12" ht="15.6">
       <c r="A68" s="78"/>
       <c r="B68" s="18"/>
       <c r="C68" s="19" t="s">
@@ -8798,7 +8795,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75">
+    <row r="69" spans="1:12" ht="15.6">
       <c r="A69" s="78"/>
       <c r="B69" s="18">
         <v>4.8</v>
@@ -8824,7 +8821,7 @@
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75">
+    <row r="70" spans="1:12" ht="15.6">
       <c r="A70" s="78"/>
       <c r="B70" s="18"/>
       <c r="C70" s="19" t="s">
@@ -8842,7 +8839,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75">
+    <row r="71" spans="1:12" ht="15.6">
       <c r="A71" s="78"/>
       <c r="B71" s="18"/>
       <c r="C71" s="19" t="s">
@@ -8860,7 +8857,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75">
+    <row r="72" spans="1:12" ht="15.6">
       <c r="A72" s="78"/>
       <c r="B72" s="18"/>
       <c r="C72" s="19" t="s">
@@ -8878,7 +8875,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75">
+    <row r="73" spans="1:12" ht="15.6">
       <c r="A73" s="78"/>
       <c r="B73" s="18"/>
       <c r="C73" s="19" t="s">
@@ -8896,7 +8893,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75">
+    <row r="74" spans="1:12" ht="15.6">
       <c r="A74" s="78"/>
       <c r="B74" s="18"/>
       <c r="C74" s="19" t="s">
@@ -8914,7 +8911,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75">
+    <row r="75" spans="1:12" ht="15.6">
       <c r="A75" s="78"/>
       <c r="B75" s="18">
         <v>4.9000000000000004</v>
@@ -8940,7 +8937,7 @@
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75">
+    <row r="76" spans="1:12" ht="15.6">
       <c r="A76" s="78"/>
       <c r="B76" s="18">
         <v>4.0999999999999996</v>
@@ -8960,7 +8957,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75">
+    <row r="77" spans="1:12" ht="15.6">
       <c r="A77" s="78"/>
       <c r="B77" s="18"/>
       <c r="C77" s="19" t="s">
@@ -8978,7 +8975,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75">
+    <row r="78" spans="1:12" ht="15.6">
       <c r="A78" s="78"/>
       <c r="B78" s="18">
         <v>4.1100000000000003</v>
@@ -8998,7 +8995,7 @@
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75">
+    <row r="79" spans="1:12" ht="15.6">
       <c r="A79" s="78"/>
       <c r="B79" s="18"/>
       <c r="C79" s="19" t="s">
@@ -9016,7 +9013,7 @@
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="1:12" ht="15.75">
+    <row r="80" spans="1:12" ht="15.6">
       <c r="A80" s="78"/>
       <c r="B80" s="18"/>
       <c r="C80" s="19" t="s">
@@ -9034,7 +9031,7 @@
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75">
+    <row r="81" spans="1:12" ht="15.6">
       <c r="A81" s="78"/>
       <c r="B81" s="18"/>
       <c r="C81" s="19" t="s">
@@ -9052,7 +9049,7 @@
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75">
+    <row r="82" spans="1:12" ht="15.6">
       <c r="A82" s="78"/>
       <c r="B82" s="18"/>
       <c r="C82" s="19" t="s">
@@ -9070,7 +9067,7 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" ht="15.75">
+    <row r="83" spans="1:12" ht="15.6">
       <c r="A83" s="78"/>
       <c r="B83" s="18">
         <v>4.12</v>
@@ -9090,7 +9087,7 @@
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" ht="15.75">
+    <row r="84" spans="1:12" ht="15.6">
       <c r="A84" s="78"/>
       <c r="B84" s="18"/>
       <c r="C84" s="19" t="s">
@@ -9108,7 +9105,7 @@
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" ht="15.75">
+    <row r="85" spans="1:12" ht="15.6">
       <c r="A85" s="78"/>
       <c r="B85" s="18"/>
       <c r="C85" s="19" t="s">
@@ -9126,7 +9123,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" ht="15.75">
+    <row r="86" spans="1:12" ht="15.6">
       <c r="A86" s="78"/>
       <c r="B86" s="18"/>
       <c r="C86" s="19" t="s">
@@ -9144,7 +9141,7 @@
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75">
+    <row r="87" spans="1:12" ht="15.6">
       <c r="A87" s="78"/>
       <c r="B87" s="18">
         <v>4.13</v>
@@ -9164,7 +9161,7 @@
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75">
+    <row r="88" spans="1:12" ht="15.6">
       <c r="A88" s="78"/>
       <c r="B88" s="18"/>
       <c r="C88" s="19" t="s">
@@ -9182,7 +9179,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75">
+    <row r="89" spans="1:12" ht="15.6">
       <c r="A89" s="78"/>
       <c r="B89" s="18">
         <v>4.1399999999999997</v>
@@ -9202,7 +9199,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75">
+    <row r="90" spans="1:12" ht="15.6">
       <c r="A90" s="78"/>
       <c r="B90" s="18">
         <v>4.1500000000000004</v>
@@ -9222,7 +9219,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75">
+    <row r="91" spans="1:12" ht="15.6">
       <c r="A91" s="78"/>
       <c r="B91" s="18"/>
       <c r="C91" s="19" t="s">
@@ -9240,7 +9237,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75">
+    <row r="92" spans="1:12" ht="15.6">
       <c r="A92" s="78"/>
       <c r="B92" s="18"/>
       <c r="C92" s="19" t="s">
@@ -9258,7 +9255,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75">
+    <row r="93" spans="1:12" ht="15.6">
       <c r="A93" s="78"/>
       <c r="B93" s="18"/>
       <c r="C93" s="19"/>
@@ -9276,7 +9273,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75">
+    <row r="94" spans="1:12" ht="15.6">
       <c r="A94" s="78"/>
       <c r="B94" s="17"/>
       <c r="C94" s="17"/>
@@ -9290,7 +9287,7 @@
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75">
+    <row r="95" spans="1:12" ht="15.6">
       <c r="A95" s="82"/>
       <c r="B95" s="79"/>
       <c r="C95" s="81" t="s">
@@ -9310,7 +9307,7 @@
       <c r="K95" s="56"/>
       <c r="L95" s="56"/>
     </row>
-    <row r="96" spans="1:12" ht="15.75">
+    <row r="96" spans="1:12" ht="15.6">
       <c r="A96" s="82"/>
       <c r="B96" s="79"/>
       <c r="C96" s="81"/>
@@ -9338,7 +9335,7 @@
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75">
+    <row r="98" spans="1:12" ht="15.6">
       <c r="A98" s="76">
         <v>5</v>
       </c>
@@ -9358,7 +9355,7 @@
       <c r="K98" s="3"/>
       <c r="L98" s="3"/>
     </row>
-    <row r="99" spans="1:12" ht="15.75">
+    <row r="99" spans="1:12" ht="15.6">
       <c r="A99" s="78"/>
       <c r="B99" s="18">
         <v>5.0999999999999996</v>
@@ -9378,7 +9375,7 @@
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75">
+    <row r="100" spans="1:12" ht="15.6">
       <c r="A100" s="78"/>
       <c r="B100" s="18">
         <v>5.2</v>
@@ -9398,7 +9395,7 @@
       <c r="K100" s="3"/>
       <c r="L100" s="3"/>
     </row>
-    <row r="101" spans="1:12" ht="15.75">
+    <row r="101" spans="1:12" ht="15.6">
       <c r="A101" s="78"/>
       <c r="B101" s="18">
         <v>5.3</v>
@@ -9418,7 +9415,7 @@
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
     </row>
-    <row r="102" spans="1:12" ht="15.75">
+    <row r="102" spans="1:12" ht="15.6">
       <c r="A102" s="78"/>
       <c r="B102" s="18"/>
       <c r="C102" s="19"/>
@@ -9432,7 +9429,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75">
+    <row r="103" spans="1:12" ht="15.6">
       <c r="A103" s="76">
         <v>6</v>
       </c>
@@ -9454,7 +9451,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
     </row>
-    <row r="104" spans="1:12" ht="15.75">
+    <row r="104" spans="1:12" ht="15.6">
       <c r="A104" s="78"/>
       <c r="B104" s="18">
         <v>6.1</v>
@@ -9472,7 +9469,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75">
+    <row r="105" spans="1:12" ht="15.6">
       <c r="A105" s="78"/>
       <c r="B105" s="18">
         <v>6.2</v>
@@ -9490,7 +9487,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75">
+    <row r="106" spans="1:12" ht="15.6">
       <c r="A106" s="78"/>
       <c r="B106" s="18">
         <v>6.3</v>
@@ -9508,7 +9505,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75">
+    <row r="107" spans="1:12" ht="15.6">
       <c r="A107" s="78"/>
       <c r="B107" s="18">
         <v>6.4</v>
@@ -9526,7 +9523,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="1:12" ht="15.75">
+    <row r="108" spans="1:12" ht="15.6">
       <c r="A108" s="78"/>
       <c r="B108" s="18">
         <v>6.5</v>
@@ -9544,7 +9541,7 @@
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
     </row>
-    <row r="109" spans="1:12" ht="15.75">
+    <row r="109" spans="1:12" ht="15.6">
       <c r="A109" s="78"/>
       <c r="B109" s="18">
         <v>6.6</v>
@@ -9562,7 +9559,7 @@
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
     </row>
-    <row r="110" spans="1:12" ht="15.75">
+    <row r="110" spans="1:12" ht="15.6">
       <c r="A110" s="78"/>
       <c r="B110" s="18"/>
       <c r="C110" s="19"/>
@@ -9576,7 +9573,7 @@
       <c r="K110" s="3"/>
       <c r="L110" s="3"/>
     </row>
-    <row r="111" spans="1:12" ht="94.5">
+    <row r="111" spans="1:12" ht="93.6">
       <c r="A111" s="82"/>
       <c r="B111" s="79"/>
       <c r="C111" s="81" t="s">
@@ -9633,7 +9630,7 @@
       <c r="K113" s="32"/>
       <c r="L113" s="32"/>
     </row>
-    <row r="114" spans="1:12" ht="15.75">
+    <row r="114" spans="1:12" ht="15.6">
       <c r="D114" s="22" t="s">
         <v>378</v>
       </c>

</xml_diff>

<commit_message>
editors final demo complete
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93473A6E-7BD8-4D31-8AF6-7BC0781F6D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1B2953-A41C-42A5-835F-E858E46362C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
+    <workbookView xWindow="1365" yWindow="1470" windowWidth="21615" windowHeight="14130" firstSheet="1" activeTab="4" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
   <sheets>
     <sheet name=" Basic GUI" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="485">
   <si>
     <t>Topic</t>
   </si>
@@ -7403,8 +7403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3782443B-979F-4126-A9F9-516CD045F0D0}">
   <dimension ref="A1:L114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="P75" sqref="P75"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="I78" sqref="I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8991,9 +8991,15 @@
       <c r="F78" s="78">
         <v>6</v>
       </c>
-      <c r="G78" s="78"/>
-      <c r="H78" s="78"/>
-      <c r="I78" s="78"/>
+      <c r="G78" s="78">
+        <v>4</v>
+      </c>
+      <c r="H78" s="101">
+        <v>45716</v>
+      </c>
+      <c r="I78" s="78" t="s">
+        <v>433</v>
+      </c>
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>

</xml_diff>

<commit_message>
DataGrid Template, Data Summaries, Master Detail, Export, Adaptability Complete
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1B2953-A41C-42A5-835F-E858E46362C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0697130-5F56-409F-B6EE-2ECC8E80496E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="1470" windowWidth="21615" windowHeight="14130" firstSheet="1" activeTab="4" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
   <sheets>
     <sheet name=" Basic GUI" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="485">
   <si>
     <t>Topic</t>
   </si>
@@ -7403,8 +7403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3782443B-979F-4126-A9F9-516CD045F0D0}">
   <dimension ref="A1:L114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="I78" sqref="I78"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8953,9 +8953,15 @@
       <c r="F76" s="78">
         <v>1</v>
       </c>
-      <c r="G76" s="78"/>
-      <c r="H76" s="78"/>
-      <c r="I76" s="78"/>
+      <c r="G76" s="78">
+        <v>1</v>
+      </c>
+      <c r="H76" s="101">
+        <v>45715</v>
+      </c>
+      <c r="I76" s="78" t="s">
+        <v>433</v>
+      </c>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
@@ -9089,9 +9095,15 @@
       <c r="F83" s="78">
         <v>5</v>
       </c>
-      <c r="G83" s="78"/>
-      <c r="H83" s="78"/>
-      <c r="I83" s="78"/>
+      <c r="G83" s="78">
+        <v>4</v>
+      </c>
+      <c r="H83" s="101">
+        <v>45719</v>
+      </c>
+      <c r="I83" s="78" t="s">
+        <v>433</v>
+      </c>
       <c r="J83" s="3"/>
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
@@ -9163,9 +9175,15 @@
       <c r="F87" s="78">
         <v>2</v>
       </c>
-      <c r="G87" s="78"/>
-      <c r="H87" s="78"/>
-      <c r="I87" s="78"/>
+      <c r="G87" s="78">
+        <v>1</v>
+      </c>
+      <c r="H87" s="101">
+        <v>45719</v>
+      </c>
+      <c r="I87" s="78" t="s">
+        <v>433</v>
+      </c>
       <c r="J87" s="3"/>
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
@@ -9201,9 +9219,15 @@
       <c r="F89" s="78">
         <v>2</v>
       </c>
-      <c r="G89" s="78"/>
-      <c r="H89" s="78"/>
-      <c r="I89" s="78"/>
+      <c r="G89" s="78">
+        <v>1</v>
+      </c>
+      <c r="H89" s="101">
+        <v>45719</v>
+      </c>
+      <c r="I89" s="78" t="s">
+        <v>433</v>
+      </c>
       <c r="J89" s="3"/>
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
@@ -9221,9 +9245,15 @@
       <c r="F90" s="78">
         <v>4</v>
       </c>
-      <c r="G90" s="78"/>
-      <c r="H90" s="78"/>
-      <c r="I90" s="78"/>
+      <c r="G90" s="78">
+        <v>2</v>
+      </c>
+      <c r="H90" s="101">
+        <v>45719</v>
+      </c>
+      <c r="I90" s="78" t="s">
+        <v>433</v>
+      </c>
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>

</xml_diff>

<commit_message>
final demo modifications - datagrid
</commit_message>
<xml_diff>
--- a/DEV Training 2025 - freshers - Hina Jadav.xlsx
+++ b/DEV Training 2025 - freshers - Hina Jadav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE0D275-AFBD-4C38-A970-5F6FAF1FEE25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3066DAE-BAA6-479B-ABB3-3570BE3FCC38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{38EE270B-E879-46F8-A665-6AA84C0B30A6}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="485">
   <si>
     <t>Topic</t>
   </si>
@@ -1816,7 +1816,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2093,6 +2093,9 @@
     <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2132,8 +2135,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="7" fillId="6" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2492,13 +2495,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="40" customFormat="1" ht="18.75">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="108"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="109"/>
       <c r="F1" s="39" t="s">
         <v>425</v>
       </c>
@@ -3396,8 +3399,8 @@
     <row r="46" spans="1:12" ht="15.75">
       <c r="A46" s="67"/>
       <c r="B46" s="24"/>
-      <c r="C46" s="105"/>
-      <c r="D46" s="105"/>
+      <c r="C46" s="106"/>
+      <c r="D46" s="106"/>
       <c r="E46" s="8"/>
       <c r="F46" s="27"/>
       <c r="G46" s="27"/>
@@ -4652,13 +4655,13 @@
       </c>
     </row>
     <row r="109" spans="1:12">
-      <c r="A109" s="102" t="s">
+      <c r="A109" s="103" t="s">
         <v>155</v>
       </c>
-      <c r="B109" s="103"/>
-      <c r="C109" s="103"/>
-      <c r="D109" s="103"/>
-      <c r="E109" s="104"/>
+      <c r="B109" s="104"/>
+      <c r="C109" s="104"/>
+      <c r="D109" s="104"/>
+      <c r="E109" s="105"/>
       <c r="F109" s="33">
         <f>SUM(F3:F108)</f>
         <v>95</v>
@@ -4673,13 +4676,13 @@
       <c r="L109" s="32"/>
     </row>
     <row r="110" spans="1:12">
-      <c r="A110" s="102" t="s">
+      <c r="A110" s="103" t="s">
         <v>156</v>
       </c>
-      <c r="B110" s="103"/>
-      <c r="C110" s="103"/>
-      <c r="D110" s="103"/>
-      <c r="E110" s="104"/>
+      <c r="B110" s="104"/>
+      <c r="C110" s="104"/>
+      <c r="D110" s="104"/>
+      <c r="E110" s="105"/>
       <c r="F110" s="33">
         <v>100</v>
       </c>
@@ -5413,7 +5416,7 @@
       <c r="C28" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="D28" s="109">
+      <c r="D28" s="110">
         <v>8</v>
       </c>
       <c r="E28" s="27"/>
@@ -5435,7 +5438,7 @@
       <c r="C29" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D29" s="109"/>
+      <c r="D29" s="110"/>
       <c r="E29" s="27"/>
       <c r="F29" s="94">
         <v>45640</v>
@@ -5455,7 +5458,7 @@
       <c r="C30" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D30" s="109"/>
+      <c r="D30" s="110"/>
       <c r="E30" s="27">
         <v>7</v>
       </c>
@@ -5499,10 +5502,10 @@
       <c r="A33" s="55" t="s">
         <v>194</v>
       </c>
-      <c r="B33" s="110" t="s">
+      <c r="B33" s="111" t="s">
         <v>379</v>
       </c>
-      <c r="C33" s="110"/>
+      <c r="C33" s="111"/>
       <c r="D33" s="57">
         <v>8</v>
       </c>
@@ -5857,10 +5860,10 @@
       <c r="A56" s="55" t="s">
         <v>216</v>
       </c>
-      <c r="B56" s="110" t="s">
+      <c r="B56" s="111" t="s">
         <v>380</v>
       </c>
-      <c r="C56" s="110"/>
+      <c r="C56" s="111"/>
       <c r="D56" s="57">
         <v>14</v>
       </c>
@@ -6109,10 +6112,10 @@
       <c r="A70" s="55" t="s">
         <v>226</v>
       </c>
-      <c r="B70" s="110" t="s">
+      <c r="B70" s="111" t="s">
         <v>381</v>
       </c>
-      <c r="C70" s="110"/>
+      <c r="C70" s="111"/>
       <c r="D70" s="57">
         <v>8</v>
       </c>
@@ -6128,11 +6131,11 @@
       <c r="J70" s="56"/>
     </row>
     <row r="71" spans="1:10">
-      <c r="A71" s="102" t="s">
+      <c r="A71" s="103" t="s">
         <v>155</v>
       </c>
-      <c r="B71" s="103"/>
-      <c r="C71" s="104"/>
+      <c r="B71" s="104"/>
+      <c r="C71" s="105"/>
       <c r="D71" s="33">
         <f>SUM(D2:D70)</f>
         <v>110.5</v>
@@ -6145,11 +6148,11 @@
       <c r="J71" s="32"/>
     </row>
     <row r="72" spans="1:10">
-      <c r="A72" s="102" t="s">
+      <c r="A72" s="103" t="s">
         <v>156</v>
       </c>
-      <c r="B72" s="103"/>
-      <c r="C72" s="104"/>
+      <c r="B72" s="104"/>
+      <c r="C72" s="105"/>
       <c r="D72" s="33">
         <v>120.5</v>
       </c>
@@ -6651,10 +6654,10 @@
       <c r="A24" s="55" t="s">
         <v>226</v>
       </c>
-      <c r="B24" s="110" t="s">
+      <c r="B24" s="111" t="s">
         <v>382</v>
       </c>
-      <c r="C24" s="110"/>
+      <c r="C24" s="111"/>
       <c r="D24" s="57">
         <v>12</v>
       </c>
@@ -6690,11 +6693,11 @@
       <c r="J25" s="3"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="102" t="s">
+      <c r="A26" s="103" t="s">
         <v>155</v>
       </c>
-      <c r="B26" s="103"/>
-      <c r="C26" s="104"/>
+      <c r="B26" s="104"/>
+      <c r="C26" s="105"/>
       <c r="D26" s="33">
         <f>SUM(D2:D25)</f>
         <v>54</v>
@@ -7322,12 +7325,12 @@
       <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="102" t="s">
+      <c r="A28" s="103" t="s">
         <v>155</v>
       </c>
-      <c r="B28" s="103"/>
-      <c r="C28" s="103"/>
-      <c r="D28" s="104"/>
+      <c r="B28" s="104"/>
+      <c r="C28" s="104"/>
+      <c r="D28" s="105"/>
       <c r="E28" s="33">
         <f>SUM(E2:E27)</f>
         <v>34.5</v>
@@ -7369,12 +7372,12 @@
       <c r="K29" s="32"/>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="102" t="s">
+      <c r="A30" s="103" t="s">
         <v>156</v>
       </c>
-      <c r="B30" s="103"/>
-      <c r="C30" s="103"/>
-      <c r="D30" s="104"/>
+      <c r="B30" s="104"/>
+      <c r="C30" s="104"/>
+      <c r="D30" s="105"/>
       <c r="E30" s="90">
         <v>44.5</v>
       </c>
@@ -7406,8 +7409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3782443B-979F-4126-A9F9-516CD045F0D0}">
   <dimension ref="A1:L114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="I106" sqref="I106"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="G111" sqref="G111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7424,29 +7427,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="112" t="s">
         <v>275</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
     </row>
     <row r="2" spans="1:12" ht="18.75">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="113" t="s">
         <v>422</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
       <c r="F2" s="73" t="s">
         <v>1</v>
       </c>
@@ -7495,7 +7498,7 @@
         <v>276</v>
       </c>
       <c r="E4" s="16"/>
-      <c r="F4" s="113">
+      <c r="F4" s="114">
         <v>4</v>
       </c>
       <c r="G4" s="23"/>
@@ -7517,7 +7520,7 @@
       <c r="E5" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F5" s="113"/>
+      <c r="F5" s="114"/>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
@@ -7537,7 +7540,7 @@
       <c r="E6" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F6" s="113"/>
+      <c r="F6" s="114"/>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
@@ -7557,7 +7560,7 @@
       <c r="E7" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F7" s="113"/>
+      <c r="F7" s="114"/>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
@@ -7575,7 +7578,7 @@
         <v>280</v>
       </c>
       <c r="E8" s="18"/>
-      <c r="F8" s="113"/>
+      <c r="F8" s="114"/>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
@@ -7593,7 +7596,7 @@
         <v>281</v>
       </c>
       <c r="E9" s="18"/>
-      <c r="F9" s="113"/>
+      <c r="F9" s="114"/>
       <c r="G9" s="23">
         <v>4</v>
       </c>
@@ -7617,7 +7620,7 @@
         <v>282</v>
       </c>
       <c r="E10" s="18"/>
-      <c r="F10" s="113"/>
+      <c r="F10" s="114"/>
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
       <c r="I10" s="23"/>
@@ -7635,7 +7638,7 @@
         <v>284</v>
       </c>
       <c r="E11" s="18"/>
-      <c r="F11" s="113"/>
+      <c r="F11" s="114"/>
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
       <c r="I11" s="23"/>
@@ -7653,7 +7656,7 @@
         <v>286</v>
       </c>
       <c r="E12" s="18"/>
-      <c r="F12" s="113"/>
+      <c r="F12" s="114"/>
       <c r="G12" s="23"/>
       <c r="H12" s="23"/>
       <c r="I12" s="23"/>
@@ -7671,7 +7674,7 @@
         <v>288</v>
       </c>
       <c r="E13" s="18"/>
-      <c r="F13" s="113"/>
+      <c r="F13" s="114"/>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
       <c r="I13" s="23"/>
@@ -7705,7 +7708,7 @@
       <c r="E15" s="74" t="s">
         <v>290</v>
       </c>
-      <c r="F15" s="113">
+      <c r="F15" s="114">
         <v>35</v>
       </c>
       <c r="G15" s="23">
@@ -7729,7 +7732,7 @@
       <c r="E16" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F16" s="113"/>
+      <c r="F16" s="114"/>
       <c r="G16" s="23"/>
       <c r="H16" s="98">
         <v>45695</v>
@@ -7753,7 +7756,7 @@
       <c r="E17" s="74" t="s">
         <v>293</v>
       </c>
-      <c r="F17" s="113"/>
+      <c r="F17" s="114"/>
       <c r="G17" s="23"/>
       <c r="H17" s="98">
         <v>45698</v>
@@ -7779,7 +7782,7 @@
       <c r="E18" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F18" s="113"/>
+      <c r="F18" s="114"/>
       <c r="G18" s="23"/>
       <c r="H18" s="98">
         <v>45699</v>
@@ -7805,7 +7808,7 @@
       <c r="E19" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F19" s="113"/>
+      <c r="F19" s="114"/>
       <c r="G19" s="23"/>
       <c r="H19" s="98">
         <v>45699</v>
@@ -7829,7 +7832,7 @@
       <c r="E20" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F20" s="113"/>
+      <c r="F20" s="114"/>
       <c r="G20" s="23"/>
       <c r="H20" s="98"/>
       <c r="I20" s="23"/>
@@ -7847,7 +7850,7 @@
         <v>298</v>
       </c>
       <c r="E21" s="18"/>
-      <c r="F21" s="113"/>
+      <c r="F21" s="114"/>
       <c r="G21" s="23"/>
       <c r="H21" s="98">
         <v>45700</v>
@@ -7869,7 +7872,7 @@
         <v>300</v>
       </c>
       <c r="E22" s="18"/>
-      <c r="F22" s="113"/>
+      <c r="F22" s="114"/>
       <c r="G22" s="23"/>
       <c r="H22" s="98">
         <v>45701</v>
@@ -7891,7 +7894,7 @@
         <v>302</v>
       </c>
       <c r="E23" s="18"/>
-      <c r="F23" s="113"/>
+      <c r="F23" s="114"/>
       <c r="G23" s="23"/>
       <c r="H23" s="98">
         <v>45701</v>
@@ -7915,7 +7918,7 @@
       <c r="E24" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F24" s="113"/>
+      <c r="F24" s="114"/>
       <c r="G24" s="23"/>
       <c r="H24" s="98">
         <v>45701</v>
@@ -7939,7 +7942,7 @@
       <c r="E25" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="F25" s="113"/>
+      <c r="F25" s="114"/>
       <c r="G25" s="23"/>
       <c r="H25" s="98">
         <v>45702</v>
@@ -7963,7 +7966,7 @@
         <v>305</v>
       </c>
       <c r="E26" s="18"/>
-      <c r="F26" s="113"/>
+      <c r="F26" s="114"/>
       <c r="G26" s="23"/>
       <c r="H26" s="98">
         <v>45702</v>
@@ -7985,7 +7988,7 @@
         <v>306</v>
       </c>
       <c r="E27" s="18"/>
-      <c r="F27" s="113"/>
+      <c r="F27" s="114"/>
       <c r="G27" s="23"/>
       <c r="H27" s="98">
         <v>45705</v>
@@ -8009,7 +8012,7 @@
       <c r="E28" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="F28" s="113"/>
+      <c r="F28" s="114"/>
       <c r="G28" s="23"/>
       <c r="H28" s="98">
         <v>45705</v>
@@ -8087,7 +8090,7 @@
       <c r="E32" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="F32" s="113"/>
+      <c r="F32" s="114"/>
       <c r="G32" s="23"/>
       <c r="H32" s="23"/>
       <c r="I32" s="23"/>
@@ -8101,7 +8104,7 @@
       <c r="C33" s="19"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
-      <c r="F33" s="113"/>
+      <c r="F33" s="114"/>
       <c r="G33" s="23"/>
       <c r="H33" s="23"/>
       <c r="I33" s="23"/>
@@ -8117,7 +8120,7 @@
         <v>311</v>
       </c>
       <c r="E34" s="18"/>
-      <c r="F34" s="113"/>
+      <c r="F34" s="114"/>
       <c r="G34" s="23"/>
       <c r="H34" s="23"/>
       <c r="I34" s="23"/>
@@ -8135,7 +8138,7 @@
         <v>312</v>
       </c>
       <c r="E35" s="16"/>
-      <c r="F35" s="113">
+      <c r="F35" s="114">
         <v>10</v>
       </c>
       <c r="G35" s="23"/>
@@ -8157,7 +8160,7 @@
       <c r="E36" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F36" s="113"/>
+      <c r="F36" s="114"/>
       <c r="G36" s="23">
         <v>11.5</v>
       </c>
@@ -8183,7 +8186,7 @@
       <c r="E37" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F37" s="113"/>
+      <c r="F37" s="114"/>
       <c r="G37" s="23"/>
       <c r="H37" s="23"/>
       <c r="I37" s="23"/>
@@ -8203,7 +8206,7 @@
       <c r="E38" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F38" s="113"/>
+      <c r="F38" s="114"/>
       <c r="G38" s="23"/>
       <c r="H38" s="23"/>
       <c r="I38" s="23"/>
@@ -8223,7 +8226,7 @@
       <c r="E39" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F39" s="113"/>
+      <c r="F39" s="114"/>
       <c r="G39" s="23"/>
       <c r="H39" s="23"/>
       <c r="I39" s="23"/>
@@ -8243,7 +8246,7 @@
       <c r="E40" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="F40" s="113"/>
+      <c r="F40" s="114"/>
       <c r="G40" s="23"/>
       <c r="H40" s="23"/>
       <c r="I40" s="23"/>
@@ -9342,9 +9345,15 @@
       <c r="F95" s="82">
         <v>8</v>
       </c>
-      <c r="G95" s="82"/>
-      <c r="H95" s="82"/>
-      <c r="I95" s="82"/>
+      <c r="G95" s="82">
+        <v>7</v>
+      </c>
+      <c r="H95" s="116">
+        <v>45722</v>
+      </c>
+      <c r="I95" s="82" t="s">
+        <v>433</v>
+      </c>
       <c r="J95" s="56"/>
       <c r="K95" s="56"/>
       <c r="L95" s="56"/>
@@ -9387,13 +9396,13 @@
         <v>368</v>
       </c>
       <c r="E98" s="16"/>
-      <c r="F98" s="114">
+      <c r="F98" s="115">
         <v>5</v>
       </c>
       <c r="G98" s="83">
         <v>4</v>
       </c>
-      <c r="H98" s="115">
+      <c r="H98" s="102">
         <v>45720</v>
       </c>
       <c r="I98" s="83" t="s">
@@ -9415,7 +9424,7 @@
       <c r="E99" s="74" t="s">
         <v>290</v>
       </c>
-      <c r="F99" s="114"/>
+      <c r="F99" s="115"/>
       <c r="G99" s="83"/>
       <c r="H99" s="83"/>
       <c r="I99" s="83"/>
@@ -9435,7 +9444,7 @@
       <c r="E100" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F100" s="114"/>
+      <c r="F100" s="115"/>
       <c r="G100" s="83"/>
       <c r="H100" s="83"/>
       <c r="I100" s="83"/>
@@ -9455,7 +9464,7 @@
       <c r="E101" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F101" s="114"/>
+      <c r="F101" s="115"/>
       <c r="G101" s="83"/>
       <c r="H101" s="83"/>
       <c r="I101" s="83"/>
@@ -9489,7 +9498,7 @@
       <c r="E103" s="74" t="s">
         <v>290</v>
       </c>
-      <c r="F103" s="114">
+      <c r="F103" s="115">
         <v>6</v>
       </c>
       <c r="G103" s="83"/>
@@ -9509,7 +9518,7 @@
         <v>298</v>
       </c>
       <c r="E104" s="18"/>
-      <c r="F104" s="114"/>
+      <c r="F104" s="115"/>
       <c r="G104" s="83"/>
       <c r="H104" s="83"/>
       <c r="I104" s="83"/>
@@ -9527,7 +9536,7 @@
         <v>372</v>
       </c>
       <c r="E105" s="18"/>
-      <c r="F105" s="114"/>
+      <c r="F105" s="115"/>
       <c r="G105" s="83"/>
       <c r="H105" s="83"/>
       <c r="I105" s="83"/>
@@ -9545,11 +9554,11 @@
         <v>373</v>
       </c>
       <c r="E106" s="18"/>
-      <c r="F106" s="114"/>
+      <c r="F106" s="115"/>
       <c r="G106" s="83">
         <v>5</v>
       </c>
-      <c r="H106" s="115">
+      <c r="H106" s="102">
         <v>45721</v>
       </c>
       <c r="I106" s="83" t="s">
@@ -9569,7 +9578,7 @@
         <v>374</v>
       </c>
       <c r="E107" s="18"/>
-      <c r="F107" s="114"/>
+      <c r="F107" s="115"/>
       <c r="G107" s="83"/>
       <c r="H107" s="83"/>
       <c r="I107" s="83"/>
@@ -9587,7 +9596,7 @@
         <v>375</v>
       </c>
       <c r="E108" s="18"/>
-      <c r="F108" s="114"/>
+      <c r="F108" s="115"/>
       <c r="G108" s="83"/>
       <c r="H108" s="83"/>
       <c r="I108" s="83"/>
@@ -9605,7 +9614,7 @@
         <v>376</v>
       </c>
       <c r="E109" s="18"/>
-      <c r="F109" s="114"/>
+      <c r="F109" s="115"/>
       <c r="G109" s="83"/>
       <c r="H109" s="83"/>
       <c r="I109" s="83"/>
@@ -9640,20 +9649,26 @@
       <c r="F111" s="82">
         <v>8</v>
       </c>
-      <c r="G111" s="82"/>
-      <c r="H111" s="82"/>
-      <c r="I111" s="82"/>
+      <c r="G111" s="82">
+        <v>6</v>
+      </c>
+      <c r="H111" s="116">
+        <v>45723</v>
+      </c>
+      <c r="I111" s="82" t="s">
+        <v>433</v>
+      </c>
       <c r="J111" s="56"/>
       <c r="K111" s="56"/>
       <c r="L111" s="56"/>
     </row>
     <row r="112" spans="1:12">
-      <c r="A112" s="102" t="s">
+      <c r="A112" s="103" t="s">
         <v>155</v>
       </c>
-      <c r="B112" s="103"/>
-      <c r="C112" s="103"/>
-      <c r="D112" s="104"/>
+      <c r="B112" s="104"/>
+      <c r="C112" s="104"/>
+      <c r="D112" s="105"/>
       <c r="E112" s="53"/>
       <c r="F112" s="53">
         <f>SUM(F4:F111)</f>
@@ -9667,12 +9682,12 @@
       <c r="L112" s="32"/>
     </row>
     <row r="113" spans="1:12">
-      <c r="A113" s="102" t="s">
+      <c r="A113" s="103" t="s">
         <v>156</v>
       </c>
-      <c r="B113" s="103"/>
-      <c r="C113" s="103"/>
-      <c r="D113" s="104"/>
+      <c r="B113" s="104"/>
+      <c r="C113" s="104"/>
+      <c r="D113" s="105"/>
       <c r="E113" s="32"/>
       <c r="F113" s="53">
         <v>145</v>

</xml_diff>